<commit_message>
add attribute for proportional contribution to an FBA objective to Reaction
</commit_message>
<xml_diff>
--- a/tests/fixtures/example-model.xlsx
+++ b/tests/fixtures/example-model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3260" windowWidth="27540" windowHeight="15540" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="2460" windowWidth="27540" windowHeight="15540" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Model!$A$1:$B$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Parameters!$A$1:$H$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Rate laws'!$A$1:$I$168</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Reactions!$A$1:$G$177</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Reactions!$A$1:$H$177</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">References!$A$1:$R$20</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Species types'!$A$1:$J$145</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Submodels!$A$1:$G$5</definedName>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2593" uniqueCount="1325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2594" uniqueCount="1326">
   <si>
     <t>Id</t>
   </si>
@@ -4025,13 +4025,16 @@
   </si>
   <si>
     <t>Max flux</t>
+  </si>
+  <si>
+    <t>Objective proportion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4046,8 +4049,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4057,6 +4067,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCCCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -4069,10 +4085,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -4080,9 +4097,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -10746,13 +10767,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G177"/>
+  <dimension ref="A1:H177"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10760,7 +10781,7 @@
     <col min="4" max="4" width="33.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10776,14 +10797,17 @@
       <c r="E1" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
+        <v>1325</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>517</v>
       </c>
@@ -10799,10 +10823,10 @@
       <c r="E2" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>520</v>
       </c>
@@ -10818,10 +10842,10 @@
       <c r="E3" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>523</v>
       </c>
@@ -10837,10 +10861,10 @@
       <c r="E4" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H4" s="2"/>
+    </row>
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>526</v>
       </c>
@@ -10856,10 +10880,10 @@
       <c r="E5" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H5" s="2"/>
+    </row>
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>529</v>
       </c>
@@ -10875,10 +10899,10 @@
       <c r="E6" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>532</v>
       </c>
@@ -10894,10 +10918,10 @@
       <c r="E7" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>535</v>
       </c>
@@ -10913,10 +10937,10 @@
       <c r="E8" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>538</v>
       </c>
@@ -10932,10 +10956,10 @@
       <c r="E9" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>541</v>
       </c>
@@ -10951,10 +10975,10 @@
       <c r="E10" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>544</v>
       </c>
@@ -10970,10 +10994,10 @@
       <c r="E11" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>547</v>
       </c>
@@ -10989,10 +11013,10 @@
       <c r="E12" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>550</v>
       </c>
@@ -11008,10 +11032,10 @@
       <c r="E13" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>553</v>
       </c>
@@ -11027,10 +11051,10 @@
       <c r="E14" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>556</v>
       </c>
@@ -11046,10 +11070,10 @@
       <c r="E15" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>559</v>
       </c>
@@ -11065,10 +11089,10 @@
       <c r="E16" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>562</v>
       </c>
@@ -11084,10 +11108,10 @@
       <c r="E17" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>565</v>
       </c>
@@ -11103,10 +11127,10 @@
       <c r="E18" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>568</v>
       </c>
@@ -11122,10 +11146,10 @@
       <c r="E19" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F19" s="2"/>
       <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>571</v>
       </c>
@@ -11141,10 +11165,10 @@
       <c r="E20" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>574</v>
       </c>
@@ -11160,10 +11184,10 @@
       <c r="E21" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>577</v>
       </c>
@@ -11179,10 +11203,10 @@
       <c r="E22" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F22" s="2"/>
       <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H22" s="2"/>
+    </row>
+    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>580</v>
       </c>
@@ -11198,10 +11222,10 @@
       <c r="E23" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H23" s="2"/>
+    </row>
+    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>583</v>
       </c>
@@ -11217,10 +11241,10 @@
       <c r="E24" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F24" s="2"/>
       <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H24" s="2"/>
+    </row>
+    <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>586</v>
       </c>
@@ -11236,10 +11260,10 @@
       <c r="E25" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F25" s="2"/>
       <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>589</v>
       </c>
@@ -11255,10 +11279,10 @@
       <c r="E26" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F26" s="2"/>
       <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>592</v>
       </c>
@@ -11274,10 +11298,10 @@
       <c r="E27" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F27" s="2"/>
       <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>595</v>
       </c>
@@ -11293,10 +11317,10 @@
       <c r="E28" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F28" s="2"/>
       <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>598</v>
       </c>
@@ -11312,10 +11336,10 @@
       <c r="E29" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F29" s="2"/>
       <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H29" s="2"/>
+    </row>
+    <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>601</v>
       </c>
@@ -11331,10 +11355,10 @@
       <c r="E30" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F30" s="2"/>
       <c r="G30" s="2"/>
-    </row>
-    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H30" s="2"/>
+    </row>
+    <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>604</v>
       </c>
@@ -11350,10 +11374,10 @@
       <c r="E31" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F31" s="2"/>
       <c r="G31" s="2"/>
-    </row>
-    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H31" s="2"/>
+    </row>
+    <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>607</v>
       </c>
@@ -11369,10 +11393,10 @@
       <c r="E32" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F32" s="2"/>
       <c r="G32" s="2"/>
-    </row>
-    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>610</v>
       </c>
@@ -11388,10 +11412,10 @@
       <c r="E33" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F33" s="2"/>
       <c r="G33" s="2"/>
-    </row>
-    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>613</v>
       </c>
@@ -11407,10 +11431,10 @@
       <c r="E34" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F34" s="2"/>
       <c r="G34" s="2"/>
-    </row>
-    <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>616</v>
       </c>
@@ -11426,10 +11450,10 @@
       <c r="E35" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F35" s="2"/>
       <c r="G35" s="2"/>
-    </row>
-    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H35" s="2"/>
+    </row>
+    <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>619</v>
       </c>
@@ -11445,10 +11469,10 @@
       <c r="E36" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F36" s="2"/>
       <c r="G36" s="2"/>
-    </row>
-    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H36" s="2"/>
+    </row>
+    <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>622</v>
       </c>
@@ -11464,10 +11488,10 @@
       <c r="E37" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F37" s="2"/>
       <c r="G37" s="2"/>
-    </row>
-    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H37" s="2"/>
+    </row>
+    <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>625</v>
       </c>
@@ -11483,10 +11507,10 @@
       <c r="E38" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F38" s="2"/>
       <c r="G38" s="2"/>
-    </row>
-    <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H38" s="2"/>
+    </row>
+    <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>628</v>
       </c>
@@ -11502,10 +11526,10 @@
       <c r="E39" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F39" s="2"/>
       <c r="G39" s="2"/>
-    </row>
-    <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H39" s="2"/>
+    </row>
+    <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>631</v>
       </c>
@@ -11521,10 +11545,10 @@
       <c r="E40" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F40" s="2"/>
       <c r="G40" s="2"/>
-    </row>
-    <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H40" s="2"/>
+    </row>
+    <row r="41" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>634</v>
       </c>
@@ -11540,10 +11564,10 @@
       <c r="E41" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F41" s="2"/>
       <c r="G41" s="2"/>
-    </row>
-    <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H41" s="2"/>
+    </row>
+    <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>637</v>
       </c>
@@ -11559,10 +11583,10 @@
       <c r="E42" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F42" s="2"/>
       <c r="G42" s="2"/>
-    </row>
-    <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H42" s="2"/>
+    </row>
+    <row r="43" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>640</v>
       </c>
@@ -11578,10 +11602,10 @@
       <c r="E43" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F43" s="2"/>
       <c r="G43" s="2"/>
-    </row>
-    <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H43" s="2"/>
+    </row>
+    <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>643</v>
       </c>
@@ -11597,10 +11621,10 @@
       <c r="E44" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F44" s="2"/>
       <c r="G44" s="2"/>
-    </row>
-    <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H44" s="2"/>
+    </row>
+    <row r="45" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>646</v>
       </c>
@@ -11616,10 +11640,10 @@
       <c r="E45" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F45" s="2"/>
       <c r="G45" s="2"/>
-    </row>
-    <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H45" s="2"/>
+    </row>
+    <row r="46" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>649</v>
       </c>
@@ -11635,10 +11659,10 @@
       <c r="E46" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F46" s="2"/>
       <c r="G46" s="2"/>
-    </row>
-    <row r="47" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H46" s="2"/>
+    </row>
+    <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>652</v>
       </c>
@@ -11654,10 +11678,10 @@
       <c r="E47" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F47" s="2"/>
       <c r="G47" s="2"/>
-    </row>
-    <row r="48" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H47" s="2"/>
+    </row>
+    <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>655</v>
       </c>
@@ -11673,10 +11697,10 @@
       <c r="E48" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F48" s="2"/>
       <c r="G48" s="2"/>
-    </row>
-    <row r="49" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H48" s="2"/>
+    </row>
+    <row r="49" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>658</v>
       </c>
@@ -11692,10 +11716,10 @@
       <c r="E49" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F49" s="2"/>
       <c r="G49" s="2"/>
-    </row>
-    <row r="50" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H49" s="2"/>
+    </row>
+    <row r="50" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>661</v>
       </c>
@@ -11711,10 +11735,10 @@
       <c r="E50" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F50" s="2"/>
       <c r="G50" s="2"/>
-    </row>
-    <row r="51" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H50" s="2"/>
+    </row>
+    <row r="51" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>664</v>
       </c>
@@ -11730,10 +11754,10 @@
       <c r="E51" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F51" s="2"/>
       <c r="G51" s="2"/>
-    </row>
-    <row r="52" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H51" s="2"/>
+    </row>
+    <row r="52" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>667</v>
       </c>
@@ -11749,10 +11773,10 @@
       <c r="E52" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F52" s="2"/>
       <c r="G52" s="2"/>
-    </row>
-    <row r="53" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H52" s="2"/>
+    </row>
+    <row r="53" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>670</v>
       </c>
@@ -11768,10 +11792,10 @@
       <c r="E53" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F53" s="2"/>
       <c r="G53" s="2"/>
-    </row>
-    <row r="54" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H53" s="2"/>
+    </row>
+    <row r="54" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>673</v>
       </c>
@@ -11787,10 +11811,13 @@
       <c r="E54" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F54" s="2"/>
+      <c r="F54">
+        <v>1</v>
+      </c>
       <c r="G54" s="2"/>
-    </row>
-    <row r="55" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H54" s="2"/>
+    </row>
+    <row r="55" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>676</v>
       </c>
@@ -11806,10 +11833,10 @@
       <c r="E55" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F55" s="2"/>
       <c r="G55" s="2"/>
-    </row>
-    <row r="56" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H55" s="2"/>
+    </row>
+    <row r="56" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>679</v>
       </c>
@@ -11825,10 +11852,10 @@
       <c r="E56" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F56" s="2"/>
       <c r="G56" s="2"/>
-    </row>
-    <row r="57" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H56" s="2"/>
+    </row>
+    <row r="57" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>682</v>
       </c>
@@ -11844,10 +11871,10 @@
       <c r="E57" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F57" s="2"/>
       <c r="G57" s="2"/>
-    </row>
-    <row r="58" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H57" s="2"/>
+    </row>
+    <row r="58" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>685</v>
       </c>
@@ -11863,10 +11890,10 @@
       <c r="E58" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F58" s="2"/>
       <c r="G58" s="2"/>
-    </row>
-    <row r="59" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H58" s="2"/>
+    </row>
+    <row r="59" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>688</v>
       </c>
@@ -11882,10 +11909,10 @@
       <c r="E59" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F59" s="2"/>
       <c r="G59" s="2"/>
-    </row>
-    <row r="60" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H59" s="2"/>
+    </row>
+    <row r="60" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>691</v>
       </c>
@@ -11901,10 +11928,10 @@
       <c r="E60" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F60" s="2"/>
       <c r="G60" s="2"/>
-    </row>
-    <row r="61" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H60" s="2"/>
+    </row>
+    <row r="61" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>694</v>
       </c>
@@ -11920,10 +11947,10 @@
       <c r="E61" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F61" s="2"/>
       <c r="G61" s="2"/>
-    </row>
-    <row r="62" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H61" s="2"/>
+    </row>
+    <row r="62" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>697</v>
       </c>
@@ -11939,10 +11966,10 @@
       <c r="E62" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F62" s="2"/>
       <c r="G62" s="2"/>
-    </row>
-    <row r="63" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H62" s="2"/>
+    </row>
+    <row r="63" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>700</v>
       </c>
@@ -11958,10 +11985,10 @@
       <c r="E63" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F63" s="2"/>
       <c r="G63" s="2"/>
-    </row>
-    <row r="64" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H63" s="2"/>
+    </row>
+    <row r="64" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>703</v>
       </c>
@@ -11977,10 +12004,10 @@
       <c r="E64" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F64" s="2"/>
       <c r="G64" s="2"/>
-    </row>
-    <row r="65" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H64" s="2"/>
+    </row>
+    <row r="65" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>706</v>
       </c>
@@ -11996,10 +12023,10 @@
       <c r="E65" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F65" s="2"/>
       <c r="G65" s="2"/>
-    </row>
-    <row r="66" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H65" s="2"/>
+    </row>
+    <row r="66" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>709</v>
       </c>
@@ -12015,10 +12042,10 @@
       <c r="E66" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F66" s="2"/>
       <c r="G66" s="2"/>
-    </row>
-    <row r="67" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H66" s="2"/>
+    </row>
+    <row r="67" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>712</v>
       </c>
@@ -12034,10 +12061,10 @@
       <c r="E67" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F67" s="2"/>
       <c r="G67" s="2"/>
-    </row>
-    <row r="68" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H67" s="2"/>
+    </row>
+    <row r="68" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>715</v>
       </c>
@@ -12053,10 +12080,10 @@
       <c r="E68" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F68" s="2"/>
       <c r="G68" s="2"/>
-    </row>
-    <row r="69" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H68" s="2"/>
+    </row>
+    <row r="69" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>718</v>
       </c>
@@ -12072,10 +12099,10 @@
       <c r="E69" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F69" s="2"/>
       <c r="G69" s="2"/>
-    </row>
-    <row r="70" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H69" s="2"/>
+    </row>
+    <row r="70" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>721</v>
       </c>
@@ -12091,10 +12118,10 @@
       <c r="E70" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F70" s="2"/>
       <c r="G70" s="2"/>
-    </row>
-    <row r="71" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H70" s="2"/>
+    </row>
+    <row r="71" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>724</v>
       </c>
@@ -12110,10 +12137,10 @@
       <c r="E71" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F71" s="2"/>
       <c r="G71" s="2"/>
-    </row>
-    <row r="72" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H71" s="2"/>
+    </row>
+    <row r="72" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>727</v>
       </c>
@@ -12129,10 +12156,10 @@
       <c r="E72" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F72" s="2"/>
       <c r="G72" s="2"/>
-    </row>
-    <row r="73" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H72" s="2"/>
+    </row>
+    <row r="73" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>730</v>
       </c>
@@ -12148,10 +12175,10 @@
       <c r="E73" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F73" s="2"/>
       <c r="G73" s="2"/>
-    </row>
-    <row r="74" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H73" s="2"/>
+    </row>
+    <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>733</v>
       </c>
@@ -12167,10 +12194,10 @@
       <c r="E74" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F74" s="2"/>
       <c r="G74" s="2"/>
-    </row>
-    <row r="75" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H74" s="2"/>
+    </row>
+    <row r="75" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>736</v>
       </c>
@@ -12186,10 +12213,10 @@
       <c r="E75" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F75" s="2"/>
       <c r="G75" s="2"/>
-    </row>
-    <row r="76" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H75" s="2"/>
+    </row>
+    <row r="76" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>739</v>
       </c>
@@ -12205,10 +12232,10 @@
       <c r="E76" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F76" s="2"/>
       <c r="G76" s="2"/>
-    </row>
-    <row r="77" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H76" s="2"/>
+    </row>
+    <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>742</v>
       </c>
@@ -12224,10 +12251,10 @@
       <c r="E77" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F77" s="2"/>
       <c r="G77" s="2"/>
-    </row>
-    <row r="78" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H77" s="2"/>
+    </row>
+    <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>745</v>
       </c>
@@ -12243,10 +12270,10 @@
       <c r="E78" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F78" s="2"/>
       <c r="G78" s="2"/>
-    </row>
-    <row r="79" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H78" s="2"/>
+    </row>
+    <row r="79" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>748</v>
       </c>
@@ -12262,10 +12289,10 @@
       <c r="E79" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F79" s="2"/>
       <c r="G79" s="2"/>
-    </row>
-    <row r="80" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H79" s="2"/>
+    </row>
+    <row r="80" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>751</v>
       </c>
@@ -12281,10 +12308,10 @@
       <c r="E80" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F80" s="2"/>
       <c r="G80" s="2"/>
-    </row>
-    <row r="81" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H80" s="2"/>
+    </row>
+    <row r="81" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>754</v>
       </c>
@@ -12300,10 +12327,10 @@
       <c r="E81" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F81" s="2"/>
       <c r="G81" s="2"/>
-    </row>
-    <row r="82" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H81" s="2"/>
+    </row>
+    <row r="82" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>757</v>
       </c>
@@ -12319,10 +12346,10 @@
       <c r="E82" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F82" s="2"/>
       <c r="G82" s="2"/>
-    </row>
-    <row r="83" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H82" s="2"/>
+    </row>
+    <row r="83" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>760</v>
       </c>
@@ -12338,10 +12365,10 @@
       <c r="E83" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F83" s="2"/>
       <c r="G83" s="2"/>
-    </row>
-    <row r="84" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H83" s="2"/>
+    </row>
+    <row r="84" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>763</v>
       </c>
@@ -12357,10 +12384,10 @@
       <c r="E84" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F84" s="2"/>
       <c r="G84" s="2"/>
-    </row>
-    <row r="85" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H84" s="2"/>
+    </row>
+    <row r="85" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>766</v>
       </c>
@@ -12376,10 +12403,10 @@
       <c r="E85" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F85" s="2"/>
       <c r="G85" s="2"/>
-    </row>
-    <row r="86" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H85" s="2"/>
+    </row>
+    <row r="86" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>769</v>
       </c>
@@ -12395,10 +12422,10 @@
       <c r="E86" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F86" s="2"/>
       <c r="G86" s="2"/>
-    </row>
-    <row r="87" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H86" s="2"/>
+    </row>
+    <row r="87" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>772</v>
       </c>
@@ -12414,10 +12441,10 @@
       <c r="E87" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F87" s="2"/>
       <c r="G87" s="2"/>
-    </row>
-    <row r="88" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H87" s="2"/>
+    </row>
+    <row r="88" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>775</v>
       </c>
@@ -12433,10 +12460,10 @@
       <c r="E88" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F88" s="2"/>
       <c r="G88" s="2"/>
-    </row>
-    <row r="89" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H88" s="2"/>
+    </row>
+    <row r="89" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>778</v>
       </c>
@@ -12452,10 +12479,10 @@
       <c r="E89" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F89" s="2"/>
       <c r="G89" s="2"/>
-    </row>
-    <row r="90" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H89" s="2"/>
+    </row>
+    <row r="90" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>781</v>
       </c>
@@ -12471,10 +12498,10 @@
       <c r="E90" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F90" s="2"/>
       <c r="G90" s="2"/>
-    </row>
-    <row r="91" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H90" s="2"/>
+    </row>
+    <row r="91" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>784</v>
       </c>
@@ -12490,10 +12517,10 @@
       <c r="E91" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F91" s="2"/>
       <c r="G91" s="2"/>
-    </row>
-    <row r="92" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H91" s="2"/>
+    </row>
+    <row r="92" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>787</v>
       </c>
@@ -12509,10 +12536,10 @@
       <c r="E92" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F92" s="2"/>
       <c r="G92" s="2"/>
-    </row>
-    <row r="93" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H92" s="2"/>
+    </row>
+    <row r="93" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>790</v>
       </c>
@@ -12528,10 +12555,10 @@
       <c r="E93" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F93" s="2"/>
       <c r="G93" s="2"/>
-    </row>
-    <row r="94" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H93" s="2"/>
+    </row>
+    <row r="94" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>793</v>
       </c>
@@ -12547,10 +12574,10 @@
       <c r="E94" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F94" s="2"/>
       <c r="G94" s="2"/>
-    </row>
-    <row r="95" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H94" s="2"/>
+    </row>
+    <row r="95" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>796</v>
       </c>
@@ -12566,10 +12593,10 @@
       <c r="E95" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F95" s="2"/>
       <c r="G95" s="2"/>
-    </row>
-    <row r="96" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H95" s="2"/>
+    </row>
+    <row r="96" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>799</v>
       </c>
@@ -12585,10 +12612,10 @@
       <c r="E96" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F96" s="2"/>
       <c r="G96" s="2"/>
-    </row>
-    <row r="97" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H96" s="2"/>
+    </row>
+    <row r="97" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>802</v>
       </c>
@@ -12604,10 +12631,10 @@
       <c r="E97" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F97" s="2"/>
       <c r="G97" s="2"/>
-    </row>
-    <row r="98" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H97" s="2"/>
+    </row>
+    <row r="98" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>805</v>
       </c>
@@ -12623,10 +12650,10 @@
       <c r="E98" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F98" s="2"/>
       <c r="G98" s="2"/>
-    </row>
-    <row r="99" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H98" s="2"/>
+    </row>
+    <row r="99" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>808</v>
       </c>
@@ -12642,10 +12669,10 @@
       <c r="E99" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F99" s="2"/>
       <c r="G99" s="2"/>
-    </row>
-    <row r="100" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H99" s="2"/>
+    </row>
+    <row r="100" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>811</v>
       </c>
@@ -12661,10 +12688,10 @@
       <c r="E100" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F100" s="2"/>
       <c r="G100" s="2"/>
-    </row>
-    <row r="101" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H100" s="2"/>
+    </row>
+    <row r="101" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>814</v>
       </c>
@@ -12680,10 +12707,10 @@
       <c r="E101" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F101" s="2"/>
       <c r="G101" s="2"/>
-    </row>
-    <row r="102" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H101" s="2"/>
+    </row>
+    <row r="102" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>817</v>
       </c>
@@ -12699,10 +12726,10 @@
       <c r="E102" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F102" s="2"/>
       <c r="G102" s="2"/>
-    </row>
-    <row r="103" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H102" s="2"/>
+    </row>
+    <row r="103" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>820</v>
       </c>
@@ -12718,10 +12745,10 @@
       <c r="E103" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F103" s="2"/>
       <c r="G103" s="2"/>
-    </row>
-    <row r="104" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H103" s="2"/>
+    </row>
+    <row r="104" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>823</v>
       </c>
@@ -12737,10 +12764,10 @@
       <c r="E104" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F104" s="2"/>
       <c r="G104" s="2"/>
-    </row>
-    <row r="105" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H104" s="2"/>
+    </row>
+    <row r="105" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>826</v>
       </c>
@@ -12756,10 +12783,10 @@
       <c r="E105" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F105" s="2"/>
       <c r="G105" s="2"/>
-    </row>
-    <row r="106" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H105" s="2"/>
+    </row>
+    <row r="106" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>829</v>
       </c>
@@ -12775,10 +12802,10 @@
       <c r="E106" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F106" s="2"/>
       <c r="G106" s="2"/>
-    </row>
-    <row r="107" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H106" s="2"/>
+    </row>
+    <row r="107" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>832</v>
       </c>
@@ -12794,10 +12821,10 @@
       <c r="E107" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F107" s="2"/>
       <c r="G107" s="2"/>
-    </row>
-    <row r="108" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H107" s="2"/>
+    </row>
+    <row r="108" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>835</v>
       </c>
@@ -12813,10 +12840,10 @@
       <c r="E108" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F108" s="2"/>
       <c r="G108" s="2"/>
-    </row>
-    <row r="109" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H108" s="2"/>
+    </row>
+    <row r="109" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>838</v>
       </c>
@@ -12832,10 +12859,10 @@
       <c r="E109" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F109" s="2"/>
       <c r="G109" s="2"/>
-    </row>
-    <row r="110" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H109" s="2"/>
+    </row>
+    <row r="110" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>841</v>
       </c>
@@ -12851,10 +12878,10 @@
       <c r="E110" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F110" s="2"/>
       <c r="G110" s="2"/>
-    </row>
-    <row r="111" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H110" s="2"/>
+    </row>
+    <row r="111" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>844</v>
       </c>
@@ -12870,10 +12897,10 @@
       <c r="E111" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F111" s="2"/>
       <c r="G111" s="2"/>
-    </row>
-    <row r="112" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H111" s="2"/>
+    </row>
+    <row r="112" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>847</v>
       </c>
@@ -12889,10 +12916,10 @@
       <c r="E112" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F112" s="2"/>
       <c r="G112" s="2"/>
-    </row>
-    <row r="113" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H112" s="2"/>
+    </row>
+    <row r="113" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>850</v>
       </c>
@@ -12908,10 +12935,10 @@
       <c r="E113" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F113" s="2"/>
       <c r="G113" s="2"/>
-    </row>
-    <row r="114" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H113" s="2"/>
+    </row>
+    <row r="114" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>853</v>
       </c>
@@ -12927,10 +12954,10 @@
       <c r="E114" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F114" s="2"/>
       <c r="G114" s="2"/>
-    </row>
-    <row r="115" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H114" s="2"/>
+    </row>
+    <row r="115" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>856</v>
       </c>
@@ -12946,10 +12973,10 @@
       <c r="E115" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F115" s="2"/>
       <c r="G115" s="2"/>
-    </row>
-    <row r="116" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H115" s="2"/>
+    </row>
+    <row r="116" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>859</v>
       </c>
@@ -12965,10 +12992,10 @@
       <c r="E116" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F116" s="2"/>
       <c r="G116" s="2"/>
-    </row>
-    <row r="117" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H116" s="2"/>
+    </row>
+    <row r="117" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>862</v>
       </c>
@@ -12984,10 +13011,10 @@
       <c r="E117" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F117" s="2"/>
       <c r="G117" s="2"/>
-    </row>
-    <row r="118" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H117" s="2"/>
+    </row>
+    <row r="118" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>865</v>
       </c>
@@ -13003,10 +13030,10 @@
       <c r="E118" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F118" s="2"/>
       <c r="G118" s="2"/>
-    </row>
-    <row r="119" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H118" s="2"/>
+    </row>
+    <row r="119" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>868</v>
       </c>
@@ -13022,10 +13049,10 @@
       <c r="E119" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F119" s="2"/>
       <c r="G119" s="2"/>
-    </row>
-    <row r="120" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H119" s="2"/>
+    </row>
+    <row r="120" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>871</v>
       </c>
@@ -13041,10 +13068,10 @@
       <c r="E120" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F120" s="2"/>
       <c r="G120" s="2"/>
-    </row>
-    <row r="121" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H120" s="2"/>
+    </row>
+    <row r="121" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>874</v>
       </c>
@@ -13060,10 +13087,10 @@
       <c r="E121" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F121" s="2"/>
       <c r="G121" s="2"/>
-    </row>
-    <row r="122" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H121" s="2"/>
+    </row>
+    <row r="122" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>877</v>
       </c>
@@ -13079,10 +13106,10 @@
       <c r="E122" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F122" s="2"/>
       <c r="G122" s="2"/>
-    </row>
-    <row r="123" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H122" s="2"/>
+    </row>
+    <row r="123" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>880</v>
       </c>
@@ -13098,10 +13125,10 @@
       <c r="E123" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F123" s="2"/>
       <c r="G123" s="2"/>
-    </row>
-    <row r="124" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H123" s="2"/>
+    </row>
+    <row r="124" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>883</v>
       </c>
@@ -13117,10 +13144,10 @@
       <c r="E124" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F124" s="2"/>
       <c r="G124" s="2"/>
-    </row>
-    <row r="125" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H124" s="2"/>
+    </row>
+    <row r="125" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>886</v>
       </c>
@@ -13136,10 +13163,10 @@
       <c r="E125" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F125" s="2"/>
       <c r="G125" s="2"/>
-    </row>
-    <row r="126" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H125" s="2"/>
+    </row>
+    <row r="126" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>889</v>
       </c>
@@ -13155,10 +13182,10 @@
       <c r="E126" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F126" s="2"/>
       <c r="G126" s="2"/>
-    </row>
-    <row r="127" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H126" s="2"/>
+    </row>
+    <row r="127" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>892</v>
       </c>
@@ -13174,10 +13201,10 @@
       <c r="E127" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F127" s="2"/>
       <c r="G127" s="2"/>
-    </row>
-    <row r="128" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H127" s="2"/>
+    </row>
+    <row r="128" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>895</v>
       </c>
@@ -13193,10 +13220,10 @@
       <c r="E128" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F128" s="2"/>
       <c r="G128" s="2"/>
-    </row>
-    <row r="129" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H128" s="2"/>
+    </row>
+    <row r="129" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>898</v>
       </c>
@@ -13212,10 +13239,10 @@
       <c r="E129" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F129" s="2"/>
       <c r="G129" s="2"/>
-    </row>
-    <row r="130" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H129" s="2"/>
+    </row>
+    <row r="130" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>901</v>
       </c>
@@ -13231,10 +13258,10 @@
       <c r="E130" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F130" s="2"/>
       <c r="G130" s="2"/>
-    </row>
-    <row r="131" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H130" s="2"/>
+    </row>
+    <row r="131" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>904</v>
       </c>
@@ -13250,10 +13277,10 @@
       <c r="E131" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F131" s="2"/>
       <c r="G131" s="2"/>
-    </row>
-    <row r="132" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H131" s="2"/>
+    </row>
+    <row r="132" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>907</v>
       </c>
@@ -13269,10 +13296,10 @@
       <c r="E132" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F132" s="2"/>
       <c r="G132" s="2"/>
-    </row>
-    <row r="133" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H132" s="2"/>
+    </row>
+    <row r="133" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>910</v>
       </c>
@@ -13288,10 +13315,10 @@
       <c r="E133" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F133" s="2"/>
       <c r="G133" s="2"/>
-    </row>
-    <row r="134" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H133" s="2"/>
+    </row>
+    <row r="134" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>913</v>
       </c>
@@ -13307,10 +13334,10 @@
       <c r="E134" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F134" s="2"/>
       <c r="G134" s="2"/>
-    </row>
-    <row r="135" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H134" s="2"/>
+    </row>
+    <row r="135" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>916</v>
       </c>
@@ -13326,10 +13353,10 @@
       <c r="E135" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F135" s="2"/>
       <c r="G135" s="2"/>
-    </row>
-    <row r="136" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H135" s="2"/>
+    </row>
+    <row r="136" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>919</v>
       </c>
@@ -13345,10 +13372,10 @@
       <c r="E136" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F136" s="2"/>
       <c r="G136" s="2"/>
-    </row>
-    <row r="137" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H136" s="2"/>
+    </row>
+    <row r="137" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>922</v>
       </c>
@@ -13364,10 +13391,10 @@
       <c r="E137" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F137" s="2"/>
       <c r="G137" s="2"/>
-    </row>
-    <row r="138" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H137" s="2"/>
+    </row>
+    <row r="138" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>925</v>
       </c>
@@ -13383,10 +13410,10 @@
       <c r="E138" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F138" s="2"/>
       <c r="G138" s="2"/>
-    </row>
-    <row r="139" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H138" s="2"/>
+    </row>
+    <row r="139" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>928</v>
       </c>
@@ -13402,10 +13429,10 @@
       <c r="E139" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F139" s="2"/>
       <c r="G139" s="2"/>
-    </row>
-    <row r="140" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H139" s="2"/>
+    </row>
+    <row r="140" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>931</v>
       </c>
@@ -13421,10 +13448,10 @@
       <c r="E140" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F140" s="2"/>
       <c r="G140" s="2"/>
-    </row>
-    <row r="141" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H140" s="2"/>
+    </row>
+    <row r="141" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>934</v>
       </c>
@@ -13440,10 +13467,10 @@
       <c r="E141" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F141" s="2"/>
       <c r="G141" s="2"/>
-    </row>
-    <row r="142" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H141" s="2"/>
+    </row>
+    <row r="142" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>937</v>
       </c>
@@ -13459,10 +13486,10 @@
       <c r="E142" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F142" s="2"/>
       <c r="G142" s="2"/>
-    </row>
-    <row r="143" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H142" s="2"/>
+    </row>
+    <row r="143" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>940</v>
       </c>
@@ -13478,10 +13505,10 @@
       <c r="E143" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F143" s="2"/>
       <c r="G143" s="2"/>
-    </row>
-    <row r="144" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H143" s="2"/>
+    </row>
+    <row r="144" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>943</v>
       </c>
@@ -13497,10 +13524,10 @@
       <c r="E144" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F144" s="2"/>
       <c r="G144" s="2"/>
-    </row>
-    <row r="145" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H144" s="2"/>
+    </row>
+    <row r="145" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>946</v>
       </c>
@@ -13516,10 +13543,10 @@
       <c r="E145" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F145" s="2"/>
       <c r="G145" s="2"/>
-    </row>
-    <row r="146" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H145" s="2"/>
+    </row>
+    <row r="146" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>949</v>
       </c>
@@ -13535,10 +13562,10 @@
       <c r="E146" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F146" s="2"/>
       <c r="G146" s="2"/>
-    </row>
-    <row r="147" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H146" s="2"/>
+    </row>
+    <row r="147" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>952</v>
       </c>
@@ -13554,10 +13581,10 @@
       <c r="E147" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F147" s="2"/>
       <c r="G147" s="2"/>
-    </row>
-    <row r="148" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H147" s="2"/>
+    </row>
+    <row r="148" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>955</v>
       </c>
@@ -13573,10 +13600,10 @@
       <c r="E148" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F148" s="2"/>
       <c r="G148" s="2"/>
-    </row>
-    <row r="149" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H148" s="2"/>
+    </row>
+    <row r="149" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>958</v>
       </c>
@@ -13592,10 +13619,10 @@
       <c r="E149" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F149" s="2"/>
       <c r="G149" s="2"/>
-    </row>
-    <row r="150" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H149" s="2"/>
+    </row>
+    <row r="150" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>961</v>
       </c>
@@ -13611,10 +13638,10 @@
       <c r="E150" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F150" s="2"/>
       <c r="G150" s="2"/>
-    </row>
-    <row r="151" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H150" s="2"/>
+    </row>
+    <row r="151" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>964</v>
       </c>
@@ -13630,10 +13657,10 @@
       <c r="E151" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F151" s="2"/>
       <c r="G151" s="2"/>
-    </row>
-    <row r="152" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H151" s="2"/>
+    </row>
+    <row r="152" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>967</v>
       </c>
@@ -13649,10 +13676,10 @@
       <c r="E152" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F152" s="2"/>
       <c r="G152" s="2"/>
-    </row>
-    <row r="153" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H152" s="2"/>
+    </row>
+    <row r="153" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>970</v>
       </c>
@@ -13668,10 +13695,10 @@
       <c r="E153" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F153" s="2"/>
       <c r="G153" s="2"/>
-    </row>
-    <row r="154" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H153" s="2"/>
+    </row>
+    <row r="154" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>973</v>
       </c>
@@ -13687,10 +13714,10 @@
       <c r="E154" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F154" s="2"/>
       <c r="G154" s="2"/>
-    </row>
-    <row r="155" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H154" s="2"/>
+    </row>
+    <row r="155" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>976</v>
       </c>
@@ -13706,10 +13733,10 @@
       <c r="E155" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F155" s="2"/>
       <c r="G155" s="2"/>
-    </row>
-    <row r="156" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H155" s="2"/>
+    </row>
+    <row r="156" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>979</v>
       </c>
@@ -13725,10 +13752,10 @@
       <c r="E156" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F156" s="2"/>
       <c r="G156" s="2"/>
-    </row>
-    <row r="157" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H156" s="2"/>
+    </row>
+    <row r="157" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>982</v>
       </c>
@@ -13744,10 +13771,10 @@
       <c r="E157" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F157" s="2"/>
       <c r="G157" s="2"/>
-    </row>
-    <row r="158" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H157" s="2"/>
+    </row>
+    <row r="158" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>985</v>
       </c>
@@ -13763,10 +13790,10 @@
       <c r="E158" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F158" s="2"/>
       <c r="G158" s="2"/>
-    </row>
-    <row r="159" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H158" s="2"/>
+    </row>
+    <row r="159" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>988</v>
       </c>
@@ -13782,10 +13809,10 @@
       <c r="E159" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F159" s="2"/>
       <c r="G159" s="2"/>
-    </row>
-    <row r="160" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H159" s="2"/>
+    </row>
+    <row r="160" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>991</v>
       </c>
@@ -13801,10 +13828,10 @@
       <c r="E160" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F160" s="2"/>
       <c r="G160" s="2"/>
-    </row>
-    <row r="161" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H160" s="2"/>
+    </row>
+    <row r="161" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>994</v>
       </c>
@@ -13820,10 +13847,10 @@
       <c r="E161" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F161" s="2"/>
       <c r="G161" s="2"/>
-    </row>
-    <row r="162" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H161" s="2"/>
+    </row>
+    <row r="162" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>997</v>
       </c>
@@ -13839,10 +13866,10 @@
       <c r="E162" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F162" s="2"/>
       <c r="G162" s="2"/>
-    </row>
-    <row r="163" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H162" s="2"/>
+    </row>
+    <row r="163" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>1000</v>
       </c>
@@ -13858,10 +13885,10 @@
       <c r="E163" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F163" s="2"/>
       <c r="G163" s="2"/>
-    </row>
-    <row r="164" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H163" s="2"/>
+    </row>
+    <row r="164" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>1003</v>
       </c>
@@ -13877,10 +13904,10 @@
       <c r="E164" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F164" s="2"/>
       <c r="G164" s="2"/>
-    </row>
-    <row r="165" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H164" s="2"/>
+    </row>
+    <row r="165" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>1006</v>
       </c>
@@ -13896,10 +13923,10 @@
       <c r="E165" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F165" s="2"/>
       <c r="G165" s="2"/>
-    </row>
-    <row r="166" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H165" s="2"/>
+    </row>
+    <row r="166" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>1009</v>
       </c>
@@ -13915,10 +13942,10 @@
       <c r="E166" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F166" s="2"/>
       <c r="G166" s="2"/>
-    </row>
-    <row r="167" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H166" s="2"/>
+    </row>
+    <row r="167" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>1012</v>
       </c>
@@ -13934,10 +13961,10 @@
       <c r="E167" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F167" s="2"/>
       <c r="G167" s="2"/>
-    </row>
-    <row r="168" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H167" s="2"/>
+    </row>
+    <row r="168" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>1015</v>
       </c>
@@ -13953,10 +13980,10 @@
       <c r="E168" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F168" s="2"/>
       <c r="G168" s="2"/>
-    </row>
-    <row r="169" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H168" s="2"/>
+    </row>
+    <row r="169" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>1018</v>
       </c>
@@ -13972,10 +13999,10 @@
       <c r="E169" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F169" s="2"/>
       <c r="G169" s="2"/>
-    </row>
-    <row r="170" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H169" s="2"/>
+    </row>
+    <row r="170" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>1021</v>
       </c>
@@ -13991,10 +14018,10 @@
       <c r="E170" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F170" s="2"/>
       <c r="G170" s="2"/>
-    </row>
-    <row r="171" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H170" s="2"/>
+    </row>
+    <row r="171" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>1024</v>
       </c>
@@ -14010,10 +14037,10 @@
       <c r="E171" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F171" s="2"/>
       <c r="G171" s="2"/>
-    </row>
-    <row r="172" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H171" s="2"/>
+    </row>
+    <row r="172" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>1027</v>
       </c>
@@ -14029,10 +14056,10 @@
       <c r="E172" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F172" s="2"/>
       <c r="G172" s="2"/>
-    </row>
-    <row r="173" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H172" s="2"/>
+    </row>
+    <row r="173" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>1030</v>
       </c>
@@ -14048,10 +14075,10 @@
       <c r="E173" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F173" s="2"/>
       <c r="G173" s="2"/>
-    </row>
-    <row r="174" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H173" s="2"/>
+    </row>
+    <row r="174" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>1033</v>
       </c>
@@ -14067,10 +14094,10 @@
       <c r="E174" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F174" s="2"/>
       <c r="G174" s="2"/>
-    </row>
-    <row r="175" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H174" s="2"/>
+    </row>
+    <row r="175" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
         <v>1036</v>
       </c>
@@ -14086,10 +14113,10 @@
       <c r="E175" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F175" s="2"/>
       <c r="G175" s="2"/>
-    </row>
-    <row r="176" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H175" s="2"/>
+    </row>
+    <row r="176" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>1039</v>
       </c>
@@ -14105,10 +14132,10 @@
       <c r="E176" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="F176" s="2"/>
       <c r="G176" s="2"/>
-    </row>
-    <row r="177" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H176" s="2"/>
+    </row>
+    <row r="177" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
         <v>1042</v>
       </c>
@@ -14124,11 +14151,11 @@
       <c r="E177" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F177" s="2"/>
       <c r="G177" s="2"/>
+      <c r="H177" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G177"/>
+  <autoFilter ref="A1:H177"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -14137,7 +14164,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I168"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="166" zoomScaleNormal="166" zoomScalePageLayoutView="166" workbookViewId="0">
+    <sheetView zoomScale="166" zoomScaleNormal="166" zoomScalePageLayoutView="166" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>

</xml_diff>

<commit_message>
add Model BiomassComponent for describing the biomass reaction remove Parameter.validate_unique(cls, objects): unique_together attributes are generically checked by Model.validate_unique(cls, objects)
</commit_message>
<xml_diff>
--- a/tests/fixtures/example-model.xlsx
+++ b/tests/fixtures/example-model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2460" windowWidth="27540" windowHeight="15540" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="32700" windowHeight="20560" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -20,19 +20,20 @@
     <sheet name="Concentrations" sheetId="6" r:id="rId6"/>
     <sheet name="Reactions" sheetId="7" r:id="rId7"/>
     <sheet name="Rate laws" sheetId="8" r:id="rId8"/>
-    <sheet name="Parameters" sheetId="9" r:id="rId9"/>
-    <sheet name="References" sheetId="10" r:id="rId10"/>
-    <sheet name="Cross references" sheetId="11" r:id="rId11"/>
+    <sheet name="Biomass components" sheetId="12" r:id="rId9"/>
+    <sheet name="Parameters" sheetId="9" r:id="rId10"/>
+    <sheet name="References" sheetId="10" r:id="rId11"/>
+    <sheet name="Cross references" sheetId="11" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Compartments!$A$1:$F$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Concentrations!$A$1:$D$126</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'Cross references'!$A$1:$J$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'Cross references'!$A$1:$J$20</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Model!$A$1:$B$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Parameters!$A$1:$H$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Parameters!$A$1:$H$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Rate laws'!$A$1:$I$168</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Reactions!$A$1:$H$177</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">References!$A$1:$R$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">References!$A$1:$R$20</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Species types'!$A$1:$J$145</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Submodels!$A$1:$G$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Taxon!$A$1:$B$6</definedName>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2594" uniqueCount="1326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2735" uniqueCount="1394">
   <si>
     <t>Id</t>
   </si>
@@ -4028,13 +4029,217 @@
   </si>
   <si>
     <t>Objective proportion</t>
+  </si>
+  <si>
+    <t>Coefficient</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>ALA_biomass_comp</t>
+  </si>
+  <si>
+    <t>ARG_biomass_comp</t>
+  </si>
+  <si>
+    <t>ASN_biomass_comp</t>
+  </si>
+  <si>
+    <t>ASP_biomass_comp</t>
+  </si>
+  <si>
+    <t>ATP_biomass_comp</t>
+  </si>
+  <si>
+    <t>CTP_biomass_comp</t>
+  </si>
+  <si>
+    <t>CYS_biomass_comp</t>
+  </si>
+  <si>
+    <t>GLN_biomass_comp</t>
+  </si>
+  <si>
+    <t>GLU_biomass_comp</t>
+  </si>
+  <si>
+    <t>GLY_biomass_comp</t>
+  </si>
+  <si>
+    <t>GTP_biomass_comp</t>
+  </si>
+  <si>
+    <t>H2O_biomass_comp</t>
+  </si>
+  <si>
+    <t>HIS_biomass_comp</t>
+  </si>
+  <si>
+    <t>ILE_biomass_comp</t>
+  </si>
+  <si>
+    <t>LEU_biomass_comp</t>
+  </si>
+  <si>
+    <t>LYS_biomass_comp</t>
+  </si>
+  <si>
+    <t>MET_biomass_comp</t>
+  </si>
+  <si>
+    <t>PHE_biomass_comp</t>
+  </si>
+  <si>
+    <t>PRO_biomass_comp</t>
+  </si>
+  <si>
+    <t>SER_biomass_comp</t>
+  </si>
+  <si>
+    <t>THR_biomass_comp</t>
+  </si>
+  <si>
+    <t>TRP_biomass_comp</t>
+  </si>
+  <si>
+    <t>TYR_biomass_comp</t>
+  </si>
+  <si>
+    <t>UTP_biomass_comp</t>
+  </si>
+  <si>
+    <t>VAL_biomass_comp</t>
+  </si>
+  <si>
+    <t>AMP_biomass_comp</t>
+  </si>
+  <si>
+    <t>CMP_biomass_comp</t>
+  </si>
+  <si>
+    <t>GDP_biomass_comp</t>
+  </si>
+  <si>
+    <t>GMP_biomass_comp</t>
+  </si>
+  <si>
+    <t>H_biomass_comp</t>
+  </si>
+  <si>
+    <t>Pi_biomass_comp</t>
+  </si>
+  <si>
+    <t>PPi_biomass_comp</t>
+  </si>
+  <si>
+    <t>UMP_biomass_comp</t>
+  </si>
+  <si>
+    <t>biomass_id_001</t>
+  </si>
+  <si>
+    <t>biomass_id_002</t>
+  </si>
+  <si>
+    <t>biomass_id_003</t>
+  </si>
+  <si>
+    <t>biomass_id_004</t>
+  </si>
+  <si>
+    <t>biomass_id_005</t>
+  </si>
+  <si>
+    <t>biomass_id_006</t>
+  </si>
+  <si>
+    <t>biomass_id_007</t>
+  </si>
+  <si>
+    <t>biomass_id_008</t>
+  </si>
+  <si>
+    <t>biomass_id_009</t>
+  </si>
+  <si>
+    <t>biomass_id_010</t>
+  </si>
+  <si>
+    <t>biomass_id_011</t>
+  </si>
+  <si>
+    <t>biomass_id_012</t>
+  </si>
+  <si>
+    <t>biomass_id_013</t>
+  </si>
+  <si>
+    <t>biomass_id_014</t>
+  </si>
+  <si>
+    <t>biomass_id_015</t>
+  </si>
+  <si>
+    <t>biomass_id_016</t>
+  </si>
+  <si>
+    <t>biomass_id_017</t>
+  </si>
+  <si>
+    <t>biomass_id_018</t>
+  </si>
+  <si>
+    <t>biomass_id_019</t>
+  </si>
+  <si>
+    <t>biomass_id_020</t>
+  </si>
+  <si>
+    <t>biomass_id_021</t>
+  </si>
+  <si>
+    <t>biomass_id_022</t>
+  </si>
+  <si>
+    <t>biomass_id_023</t>
+  </si>
+  <si>
+    <t>biomass_id_024</t>
+  </si>
+  <si>
+    <t>biomass_id_025</t>
+  </si>
+  <si>
+    <t>biomass_id_026</t>
+  </si>
+  <si>
+    <t>biomass_id_027</t>
+  </si>
+  <si>
+    <t>biomass_id_028</t>
+  </si>
+  <si>
+    <t>biomass_id_029</t>
+  </si>
+  <si>
+    <t>biomass_id_030</t>
+  </si>
+  <si>
+    <t>biomass_id_031</t>
+  </si>
+  <si>
+    <t>biomass_id_032</t>
+  </si>
+  <si>
+    <t>biomass_id_033</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4056,8 +4261,40 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4075,6 +4312,12 @@
         <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -4085,11 +4328,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -4100,8 +4349,21 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="8">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -4457,6 +4719,161 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="M25" sqref="M25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1162</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1163</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2">
+        <v>12</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>1166</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>1167</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>1169</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2">
+        <v>28800</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>1171</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+    </row>
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>1172</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>1173</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>1174</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2" t="s">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>1177</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="2">
+        <v>20</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>1166</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>1178</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>1179</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>1180</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2">
+        <v>300</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>1171</v>
+      </c>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:H6"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5242,7 +5659,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J20"/>
   <sheetViews>
@@ -5716,7 +6133,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5910,10 +6327,10 @@
   <dimension ref="A1:J145"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10769,11 +11186,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H177"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomRight" activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -17756,155 +18173,617 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+    <sheetView tabSelected="1" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="143" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" customWidth="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1162</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>1163</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="C1" s="4" t="s">
+        <v>514</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>1326</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>1299</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>1164</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1165</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1361</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1328</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="2">
-        <v>12</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>1166</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>1167</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="D2" s="6">
+        <v>-34190.379999999997</v>
+      </c>
+      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>1327</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>1168</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>1169</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>1170</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2">
-        <v>28800</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>1171</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>1172</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>1173</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>1174</v>
-      </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2" t="s">
-        <v>1175</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>1176</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>1177</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1362</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1329</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="2">
-        <v>20</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>1166</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>1178</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>1168</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>1179</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>1180</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2">
-        <v>300</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>1171</v>
-      </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="D3" s="6">
+        <v>-40890.379999999997</v>
+      </c>
+      <c r="E3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1363</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1330</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="6">
+        <v>-23190.38</v>
+      </c>
+      <c r="E4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1364</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1331</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="6">
+        <v>-24290.38</v>
+      </c>
+      <c r="E5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>1365</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1332</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="6">
+        <v>-1101856</v>
+      </c>
+      <c r="E6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>1366</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1333</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="6">
+        <v>-1164906</v>
+      </c>
+      <c r="E7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>1367</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1334</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="6">
+        <v>-22290.38</v>
+      </c>
+      <c r="E8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>1368</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1335</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="6">
+        <v>-24690.38</v>
+      </c>
+      <c r="E9" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>1369</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1336</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="6">
+        <v>-22690.38</v>
+      </c>
+      <c r="E10" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>1370</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1337</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="6">
+        <v>-31190.38</v>
+      </c>
+      <c r="E11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>1371</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1338</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="6">
+        <v>-1728316</v>
+      </c>
+      <c r="E12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>1372</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1339</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="6">
+        <v>-1521617000</v>
+      </c>
+      <c r="E13" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>1373</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1340</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="6">
+        <v>-21590.38</v>
+      </c>
+      <c r="E14" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>1374</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1341</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="6">
+        <v>-29290.38</v>
+      </c>
+      <c r="E15" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>1375</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1342</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="6">
+        <v>-41190.379999999997</v>
+      </c>
+      <c r="E16" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>1376</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1343</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="6">
+        <v>-21990.38</v>
+      </c>
+      <c r="E17" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>1377</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1344</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="6">
+        <v>-21390.38</v>
+      </c>
+      <c r="E18" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>1378</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1345</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="6">
+        <v>-23890.38</v>
+      </c>
+      <c r="E19" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>1379</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1346</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="6">
+        <v>-34390.379999999997</v>
+      </c>
+      <c r="E20" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>1380</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1347</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="6">
+        <v>-44490.38</v>
+      </c>
+      <c r="E21" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>1381</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1348</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="6">
+        <v>-36190.379999999997</v>
+      </c>
+      <c r="E22" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>1382</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1349</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="6">
+        <v>-22190.38</v>
+      </c>
+      <c r="E23" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>1383</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1350</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="6">
+        <v>-21990.38</v>
+      </c>
+      <c r="E24" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>1384</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1351</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="6">
+        <v>-1132896</v>
+      </c>
+      <c r="E25" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>1385</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1352</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="6">
+        <v>-33790.379999999997</v>
+      </c>
+      <c r="E26" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>1386</v>
+      </c>
+      <c r="B27" t="s">
+        <v>1353</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="6">
+        <v>1035619</v>
+      </c>
+      <c r="E27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>1387</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1354</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="6">
+        <v>1098019</v>
+      </c>
+      <c r="E28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>1388</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1355</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="6">
+        <v>581419.19999999995</v>
+      </c>
+      <c r="E29" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>1389</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1356</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="6">
+        <v>1052899</v>
+      </c>
+      <c r="E30" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>1390</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1357</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" s="6">
+        <v>4972350</v>
+      </c>
+      <c r="E31" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>1391</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1358</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="6">
+        <v>471096.2</v>
+      </c>
+      <c r="E32" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>1392</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1359</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="6">
+        <v>4381069</v>
+      </c>
+      <c r="E33" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>1393</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1360</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" s="6">
+        <v>1066339</v>
+      </c>
+      <c r="E34" t="s">
+        <v>368</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H6"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <sortState ref="A27:E34">
+    <sortCondition ref="A27:A34"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add BiomassReaction; remove Reaction.objective_proportion
</commit_message>
<xml_diff>
--- a/tests/fixtures/example-model.xlsx
+++ b/tests/fixtures/example-model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="32700" windowHeight="20560" activeTab="8"/>
+    <workbookView xWindow="-28800" yWindow="460" windowWidth="24460" windowHeight="15540" firstSheet="1" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -20,20 +20,21 @@
     <sheet name="Concentrations" sheetId="6" r:id="rId6"/>
     <sheet name="Reactions" sheetId="7" r:id="rId7"/>
     <sheet name="Rate laws" sheetId="8" r:id="rId8"/>
-    <sheet name="Biomass components" sheetId="12" r:id="rId9"/>
-    <sheet name="Parameters" sheetId="9" r:id="rId10"/>
-    <sheet name="References" sheetId="10" r:id="rId11"/>
-    <sheet name="Cross references" sheetId="11" r:id="rId12"/>
+    <sheet name="Biomass components" sheetId="14" r:id="rId9"/>
+    <sheet name="Biomass reactions" sheetId="13" r:id="rId10"/>
+    <sheet name="Parameters" sheetId="9" r:id="rId11"/>
+    <sheet name="References" sheetId="10" r:id="rId12"/>
+    <sheet name="Cross references" sheetId="11" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Compartments!$A$1:$F$3</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Concentrations!$A$1:$D$126</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'Cross references'!$A$1:$J$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'Cross references'!$A$1:$J$20</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Model!$A$1:$B$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">Parameters!$A$1:$H$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">Parameters!$A$1:$H$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Rate laws'!$A$1:$I$168</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Reactions!$A$1:$H$177</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">References!$A$1:$R$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Reactions!$A$1:$G$177</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">References!$A$1:$R$20</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Species types'!$A$1:$J$145</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Submodels!$A$1:$G$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Taxon!$A$1:$B$6</definedName>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2735" uniqueCount="1394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2743" uniqueCount="1397">
   <si>
     <t>Id</t>
   </si>
@@ -4028,9 +4029,6 @@
     <t>Max flux</t>
   </si>
   <si>
-    <t>Objective proportion</t>
-  </si>
-  <si>
     <t>Coefficient</t>
   </si>
   <si>
@@ -4233,13 +4231,25 @@
   </si>
   <si>
     <t>biomass_id_033</t>
+  </si>
+  <si>
+    <t>Biomass reaction</t>
+  </si>
+  <si>
+    <t>Metabolism_biomass</t>
+  </si>
+  <si>
+    <t>Metabolism biomass reaction</t>
+  </si>
+  <si>
+    <t>No comment</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4293,8 +4303,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4304,12 +4321,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCCCCCC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCCCCC"/>
-        <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -4328,7 +4339,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4337,8 +4348,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -4346,18 +4358,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="8"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="7" fillId="0" borderId="0" xfId="8" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -4366,6 +4385,7 @@
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -4719,13 +4739,63 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14:G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>514</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>1394</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1395</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1396</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="M25" sqref="M25"/>
+      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4872,7 +4942,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R20"/>
   <sheetViews>
@@ -4880,7 +4950,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5659,7 +5729,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J20"/>
   <sheetViews>
@@ -5667,7 +5737,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6129,11 +6199,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="154" zoomScaleNormal="154" zoomScalePageLayoutView="154" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6247,7 +6317,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="135" zoomScaleNormal="135" zoomScalePageLayoutView="135" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -6257,7 +6327,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -11184,13 +11254,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H177"/>
+  <dimension ref="A1:G177"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="157" zoomScaleNormal="157" zoomScalePageLayoutView="157" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D54" sqref="D54"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11198,7 +11268,7 @@
     <col min="4" max="4" width="33.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11214,17 +11284,14 @@
       <c r="E1" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>1325</v>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>517</v>
       </c>
@@ -11240,10 +11307,10 @@
       <c r="E2" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>520</v>
       </c>
@@ -11259,10 +11326,10 @@
       <c r="E3" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>523</v>
       </c>
@@ -11278,10 +11345,10 @@
       <c r="E4" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-    </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>526</v>
       </c>
@@ -11297,10 +11364,10 @@
       <c r="E5" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>529</v>
       </c>
@@ -11316,10 +11383,10 @@
       <c r="E6" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>532</v>
       </c>
@@ -11335,10 +11402,10 @@
       <c r="E7" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-    </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>535</v>
       </c>
@@ -11354,10 +11421,10 @@
       <c r="E8" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-    </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>538</v>
       </c>
@@ -11373,10 +11440,10 @@
       <c r="E9" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-    </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>541</v>
       </c>
@@ -11392,10 +11459,10 @@
       <c r="E10" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>544</v>
       </c>
@@ -11411,10 +11478,10 @@
       <c r="E11" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F11" s="2"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>547</v>
       </c>
@@ -11430,10 +11497,10 @@
       <c r="E12" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>550</v>
       </c>
@@ -11449,10 +11516,10 @@
       <c r="E13" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>553</v>
       </c>
@@ -11468,10 +11535,10 @@
       <c r="E14" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F14" s="2"/>
       <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>556</v>
       </c>
@@ -11487,10 +11554,10 @@
       <c r="E15" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-    </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>559</v>
       </c>
@@ -11506,10 +11573,10 @@
       <c r="E16" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F16" s="2"/>
       <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>562</v>
       </c>
@@ -11525,10 +11592,10 @@
       <c r="E17" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F17" s="2"/>
       <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-    </row>
-    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>565</v>
       </c>
@@ -11544,10 +11611,10 @@
       <c r="E18" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F18" s="2"/>
       <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-    </row>
-    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>568</v>
       </c>
@@ -11563,10 +11630,10 @@
       <c r="E19" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F19" s="2"/>
       <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-    </row>
-    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>571</v>
       </c>
@@ -11582,10 +11649,10 @@
       <c r="E20" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F20" s="2"/>
       <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-    </row>
-    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>574</v>
       </c>
@@ -11601,10 +11668,10 @@
       <c r="E21" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F21" s="2"/>
       <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-    </row>
-    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>577</v>
       </c>
@@ -11620,10 +11687,10 @@
       <c r="E22" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F22" s="2"/>
       <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-    </row>
-    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>580</v>
       </c>
@@ -11639,10 +11706,10 @@
       <c r="E23" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F23" s="2"/>
       <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-    </row>
-    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>583</v>
       </c>
@@ -11658,10 +11725,10 @@
       <c r="E24" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F24" s="2"/>
       <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-    </row>
-    <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>586</v>
       </c>
@@ -11677,10 +11744,10 @@
       <c r="E25" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F25" s="2"/>
       <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-    </row>
-    <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>589</v>
       </c>
@@ -11696,10 +11763,10 @@
       <c r="E26" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F26" s="2"/>
       <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-    </row>
-    <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>592</v>
       </c>
@@ -11715,10 +11782,10 @@
       <c r="E27" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F27" s="2"/>
       <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-    </row>
-    <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>595</v>
       </c>
@@ -11734,10 +11801,10 @@
       <c r="E28" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F28" s="2"/>
       <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-    </row>
-    <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>598</v>
       </c>
@@ -11753,10 +11820,10 @@
       <c r="E29" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F29" s="2"/>
       <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-    </row>
-    <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>601</v>
       </c>
@@ -11772,10 +11839,10 @@
       <c r="E30" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F30" s="2"/>
       <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-    </row>
-    <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>604</v>
       </c>
@@ -11791,10 +11858,10 @@
       <c r="E31" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F31" s="2"/>
       <c r="G31" s="2"/>
-      <c r="H31" s="2"/>
-    </row>
-    <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>607</v>
       </c>
@@ -11810,10 +11877,10 @@
       <c r="E32" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F32" s="2"/>
       <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-    </row>
-    <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>610</v>
       </c>
@@ -11829,10 +11896,10 @@
       <c r="E33" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F33" s="2"/>
       <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-    </row>
-    <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>613</v>
       </c>
@@ -11848,10 +11915,10 @@
       <c r="E34" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F34" s="2"/>
       <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-    </row>
-    <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>616</v>
       </c>
@@ -11867,10 +11934,10 @@
       <c r="E35" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F35" s="2"/>
       <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-    </row>
-    <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>619</v>
       </c>
@@ -11886,10 +11953,10 @@
       <c r="E36" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F36" s="2"/>
       <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-    </row>
-    <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>622</v>
       </c>
@@ -11905,10 +11972,10 @@
       <c r="E37" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F37" s="2"/>
       <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-    </row>
-    <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>625</v>
       </c>
@@ -11924,10 +11991,10 @@
       <c r="E38" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F38" s="2"/>
       <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-    </row>
-    <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>628</v>
       </c>
@@ -11943,10 +12010,10 @@
       <c r="E39" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F39" s="2"/>
       <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-    </row>
-    <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>631</v>
       </c>
@@ -11962,10 +12029,10 @@
       <c r="E40" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F40" s="2"/>
       <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-    </row>
-    <row r="41" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>634</v>
       </c>
@@ -11981,10 +12048,10 @@
       <c r="E41" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F41" s="2"/>
       <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-    </row>
-    <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>637</v>
       </c>
@@ -12000,10 +12067,10 @@
       <c r="E42" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F42" s="2"/>
       <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-    </row>
-    <row r="43" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>640</v>
       </c>
@@ -12019,10 +12086,10 @@
       <c r="E43" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F43" s="2"/>
       <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-    </row>
-    <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>643</v>
       </c>
@@ -12038,10 +12105,10 @@
       <c r="E44" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F44" s="2"/>
       <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-    </row>
-    <row r="45" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>646</v>
       </c>
@@ -12057,10 +12124,10 @@
       <c r="E45" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F45" s="2"/>
       <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-    </row>
-    <row r="46" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="46" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>649</v>
       </c>
@@ -12076,10 +12143,10 @@
       <c r="E46" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F46" s="2"/>
       <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-    </row>
-    <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>652</v>
       </c>
@@ -12095,10 +12162,10 @@
       <c r="E47" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F47" s="2"/>
       <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
-    </row>
-    <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>655</v>
       </c>
@@ -12114,10 +12181,10 @@
       <c r="E48" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F48" s="2"/>
       <c r="G48" s="2"/>
-      <c r="H48" s="2"/>
-    </row>
-    <row r="49" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="49" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>658</v>
       </c>
@@ -12133,10 +12200,10 @@
       <c r="E49" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F49" s="2"/>
       <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-    </row>
-    <row r="50" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>661</v>
       </c>
@@ -12152,10 +12219,10 @@
       <c r="E50" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F50" s="2"/>
       <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
-    </row>
-    <row r="51" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>664</v>
       </c>
@@ -12171,10 +12238,10 @@
       <c r="E51" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F51" s="2"/>
       <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
-    </row>
-    <row r="52" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="52" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>667</v>
       </c>
@@ -12190,10 +12257,10 @@
       <c r="E52" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F52" s="2"/>
       <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
-    </row>
-    <row r="53" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>670</v>
       </c>
@@ -12209,10 +12276,10 @@
       <c r="E53" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F53" s="2"/>
       <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
-    </row>
-    <row r="54" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>673</v>
       </c>
@@ -12228,13 +12295,10 @@
       <c r="E54" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="F54">
-        <v>1</v>
-      </c>
+      <c r="F54" s="2"/>
       <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
-    </row>
-    <row r="55" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>676</v>
       </c>
@@ -12250,10 +12314,10 @@
       <c r="E55" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F55" s="2"/>
       <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
-    </row>
-    <row r="56" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>679</v>
       </c>
@@ -12269,10 +12333,10 @@
       <c r="E56" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F56" s="2"/>
       <c r="G56" s="2"/>
-      <c r="H56" s="2"/>
-    </row>
-    <row r="57" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>682</v>
       </c>
@@ -12288,10 +12352,10 @@
       <c r="E57" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F57" s="2"/>
       <c r="G57" s="2"/>
-      <c r="H57" s="2"/>
-    </row>
-    <row r="58" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="58" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>685</v>
       </c>
@@ -12307,10 +12371,10 @@
       <c r="E58" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F58" s="2"/>
       <c r="G58" s="2"/>
-      <c r="H58" s="2"/>
-    </row>
-    <row r="59" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="59" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>688</v>
       </c>
@@ -12326,10 +12390,10 @@
       <c r="E59" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F59" s="2"/>
       <c r="G59" s="2"/>
-      <c r="H59" s="2"/>
-    </row>
-    <row r="60" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>691</v>
       </c>
@@ -12345,10 +12409,10 @@
       <c r="E60" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F60" s="2"/>
       <c r="G60" s="2"/>
-      <c r="H60" s="2"/>
-    </row>
-    <row r="61" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>694</v>
       </c>
@@ -12364,10 +12428,10 @@
       <c r="E61" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F61" s="2"/>
       <c r="G61" s="2"/>
-      <c r="H61" s="2"/>
-    </row>
-    <row r="62" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="62" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>697</v>
       </c>
@@ -12383,10 +12447,10 @@
       <c r="E62" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F62" s="2"/>
       <c r="G62" s="2"/>
-      <c r="H62" s="2"/>
-    </row>
-    <row r="63" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>700</v>
       </c>
@@ -12402,10 +12466,10 @@
       <c r="E63" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F63" s="2"/>
       <c r="G63" s="2"/>
-      <c r="H63" s="2"/>
-    </row>
-    <row r="64" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="64" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>703</v>
       </c>
@@ -12421,10 +12485,10 @@
       <c r="E64" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F64" s="2"/>
       <c r="G64" s="2"/>
-      <c r="H64" s="2"/>
-    </row>
-    <row r="65" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>706</v>
       </c>
@@ -12440,10 +12504,10 @@
       <c r="E65" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F65" s="2"/>
       <c r="G65" s="2"/>
-      <c r="H65" s="2"/>
-    </row>
-    <row r="66" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>709</v>
       </c>
@@ -12459,10 +12523,10 @@
       <c r="E66" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F66" s="2"/>
       <c r="G66" s="2"/>
-      <c r="H66" s="2"/>
-    </row>
-    <row r="67" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>712</v>
       </c>
@@ -12478,10 +12542,10 @@
       <c r="E67" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F67" s="2"/>
       <c r="G67" s="2"/>
-      <c r="H67" s="2"/>
-    </row>
-    <row r="68" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>715</v>
       </c>
@@ -12497,10 +12561,10 @@
       <c r="E68" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F68" s="2"/>
       <c r="G68" s="2"/>
-      <c r="H68" s="2"/>
-    </row>
-    <row r="69" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="69" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>718</v>
       </c>
@@ -12516,10 +12580,10 @@
       <c r="E69" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F69" s="2"/>
       <c r="G69" s="2"/>
-      <c r="H69" s="2"/>
-    </row>
-    <row r="70" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="70" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>721</v>
       </c>
@@ -12535,10 +12599,10 @@
       <c r="E70" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F70" s="2"/>
       <c r="G70" s="2"/>
-      <c r="H70" s="2"/>
-    </row>
-    <row r="71" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="71" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>724</v>
       </c>
@@ -12554,10 +12618,10 @@
       <c r="E71" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F71" s="2"/>
       <c r="G71" s="2"/>
-      <c r="H71" s="2"/>
-    </row>
-    <row r="72" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="72" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>727</v>
       </c>
@@ -12573,10 +12637,10 @@
       <c r="E72" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F72" s="2"/>
       <c r="G72" s="2"/>
-      <c r="H72" s="2"/>
-    </row>
-    <row r="73" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="73" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>730</v>
       </c>
@@ -12592,10 +12656,10 @@
       <c r="E73" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F73" s="2"/>
       <c r="G73" s="2"/>
-      <c r="H73" s="2"/>
-    </row>
-    <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="74" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>733</v>
       </c>
@@ -12611,10 +12675,10 @@
       <c r="E74" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F74" s="2"/>
       <c r="G74" s="2"/>
-      <c r="H74" s="2"/>
-    </row>
-    <row r="75" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="75" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>736</v>
       </c>
@@ -12630,10 +12694,10 @@
       <c r="E75" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F75" s="2"/>
       <c r="G75" s="2"/>
-      <c r="H75" s="2"/>
-    </row>
-    <row r="76" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="76" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>739</v>
       </c>
@@ -12649,10 +12713,10 @@
       <c r="E76" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F76" s="2"/>
       <c r="G76" s="2"/>
-      <c r="H76" s="2"/>
-    </row>
-    <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="77" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>742</v>
       </c>
@@ -12668,10 +12732,10 @@
       <c r="E77" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F77" s="2"/>
       <c r="G77" s="2"/>
-      <c r="H77" s="2"/>
-    </row>
-    <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="78" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>745</v>
       </c>
@@ -12687,10 +12751,10 @@
       <c r="E78" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F78" s="2"/>
       <c r="G78" s="2"/>
-      <c r="H78" s="2"/>
-    </row>
-    <row r="79" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="79" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>748</v>
       </c>
@@ -12706,10 +12770,10 @@
       <c r="E79" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F79" s="2"/>
       <c r="G79" s="2"/>
-      <c r="H79" s="2"/>
-    </row>
-    <row r="80" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>751</v>
       </c>
@@ -12725,10 +12789,10 @@
       <c r="E80" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F80" s="2"/>
       <c r="G80" s="2"/>
-      <c r="H80" s="2"/>
-    </row>
-    <row r="81" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="81" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>754</v>
       </c>
@@ -12744,10 +12808,10 @@
       <c r="E81" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F81" s="2"/>
       <c r="G81" s="2"/>
-      <c r="H81" s="2"/>
-    </row>
-    <row r="82" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="82" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>757</v>
       </c>
@@ -12763,10 +12827,10 @@
       <c r="E82" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F82" s="2"/>
       <c r="G82" s="2"/>
-      <c r="H82" s="2"/>
-    </row>
-    <row r="83" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="83" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>760</v>
       </c>
@@ -12782,10 +12846,10 @@
       <c r="E83" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F83" s="2"/>
       <c r="G83" s="2"/>
-      <c r="H83" s="2"/>
-    </row>
-    <row r="84" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="84" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>763</v>
       </c>
@@ -12801,10 +12865,10 @@
       <c r="E84" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F84" s="2"/>
       <c r="G84" s="2"/>
-      <c r="H84" s="2"/>
-    </row>
-    <row r="85" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="85" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>766</v>
       </c>
@@ -12820,10 +12884,10 @@
       <c r="E85" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F85" s="2"/>
       <c r="G85" s="2"/>
-      <c r="H85" s="2"/>
-    </row>
-    <row r="86" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="86" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>769</v>
       </c>
@@ -12839,10 +12903,10 @@
       <c r="E86" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F86" s="2"/>
       <c r="G86" s="2"/>
-      <c r="H86" s="2"/>
-    </row>
-    <row r="87" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="87" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>772</v>
       </c>
@@ -12858,10 +12922,10 @@
       <c r="E87" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F87" s="2"/>
       <c r="G87" s="2"/>
-      <c r="H87" s="2"/>
-    </row>
-    <row r="88" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="88" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>775</v>
       </c>
@@ -12877,10 +12941,10 @@
       <c r="E88" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F88" s="2"/>
       <c r="G88" s="2"/>
-      <c r="H88" s="2"/>
-    </row>
-    <row r="89" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="89" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>778</v>
       </c>
@@ -12896,10 +12960,10 @@
       <c r="E89" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F89" s="2"/>
       <c r="G89" s="2"/>
-      <c r="H89" s="2"/>
-    </row>
-    <row r="90" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="90" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>781</v>
       </c>
@@ -12915,10 +12979,10 @@
       <c r="E90" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F90" s="2"/>
       <c r="G90" s="2"/>
-      <c r="H90" s="2"/>
-    </row>
-    <row r="91" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="91" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>784</v>
       </c>
@@ -12934,10 +12998,10 @@
       <c r="E91" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F91" s="2"/>
       <c r="G91" s="2"/>
-      <c r="H91" s="2"/>
-    </row>
-    <row r="92" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="92" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>787</v>
       </c>
@@ -12953,10 +13017,10 @@
       <c r="E92" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F92" s="2"/>
       <c r="G92" s="2"/>
-      <c r="H92" s="2"/>
-    </row>
-    <row r="93" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="93" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>790</v>
       </c>
@@ -12972,10 +13036,10 @@
       <c r="E93" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F93" s="2"/>
       <c r="G93" s="2"/>
-      <c r="H93" s="2"/>
-    </row>
-    <row r="94" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="94" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>793</v>
       </c>
@@ -12991,10 +13055,10 @@
       <c r="E94" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F94" s="2"/>
       <c r="G94" s="2"/>
-      <c r="H94" s="2"/>
-    </row>
-    <row r="95" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="95" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>796</v>
       </c>
@@ -13010,10 +13074,10 @@
       <c r="E95" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F95" s="2"/>
       <c r="G95" s="2"/>
-      <c r="H95" s="2"/>
-    </row>
-    <row r="96" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="96" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>799</v>
       </c>
@@ -13029,10 +13093,10 @@
       <c r="E96" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F96" s="2"/>
       <c r="G96" s="2"/>
-      <c r="H96" s="2"/>
-    </row>
-    <row r="97" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="97" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>802</v>
       </c>
@@ -13048,10 +13112,10 @@
       <c r="E97" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F97" s="2"/>
       <c r="G97" s="2"/>
-      <c r="H97" s="2"/>
-    </row>
-    <row r="98" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="98" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>805</v>
       </c>
@@ -13067,10 +13131,10 @@
       <c r="E98" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F98" s="2"/>
       <c r="G98" s="2"/>
-      <c r="H98" s="2"/>
-    </row>
-    <row r="99" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="99" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>808</v>
       </c>
@@ -13086,10 +13150,10 @@
       <c r="E99" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F99" s="2"/>
       <c r="G99" s="2"/>
-      <c r="H99" s="2"/>
-    </row>
-    <row r="100" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="100" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>811</v>
       </c>
@@ -13105,10 +13169,10 @@
       <c r="E100" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F100" s="2"/>
       <c r="G100" s="2"/>
-      <c r="H100" s="2"/>
-    </row>
-    <row r="101" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="101" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>814</v>
       </c>
@@ -13124,10 +13188,10 @@
       <c r="E101" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F101" s="2"/>
       <c r="G101" s="2"/>
-      <c r="H101" s="2"/>
-    </row>
-    <row r="102" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="102" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>817</v>
       </c>
@@ -13143,10 +13207,10 @@
       <c r="E102" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F102" s="2"/>
       <c r="G102" s="2"/>
-      <c r="H102" s="2"/>
-    </row>
-    <row r="103" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="103" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>820</v>
       </c>
@@ -13162,10 +13226,10 @@
       <c r="E103" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F103" s="2"/>
       <c r="G103" s="2"/>
-      <c r="H103" s="2"/>
-    </row>
-    <row r="104" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="104" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>823</v>
       </c>
@@ -13181,10 +13245,10 @@
       <c r="E104" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F104" s="2"/>
       <c r="G104" s="2"/>
-      <c r="H104" s="2"/>
-    </row>
-    <row r="105" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="105" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>826</v>
       </c>
@@ -13200,10 +13264,10 @@
       <c r="E105" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F105" s="2"/>
       <c r="G105" s="2"/>
-      <c r="H105" s="2"/>
-    </row>
-    <row r="106" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="106" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>829</v>
       </c>
@@ -13219,10 +13283,10 @@
       <c r="E106" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F106" s="2"/>
       <c r="G106" s="2"/>
-      <c r="H106" s="2"/>
-    </row>
-    <row r="107" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="107" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>832</v>
       </c>
@@ -13238,10 +13302,10 @@
       <c r="E107" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F107" s="2"/>
       <c r="G107" s="2"/>
-      <c r="H107" s="2"/>
-    </row>
-    <row r="108" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="108" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>835</v>
       </c>
@@ -13257,10 +13321,10 @@
       <c r="E108" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F108" s="2"/>
       <c r="G108" s="2"/>
-      <c r="H108" s="2"/>
-    </row>
-    <row r="109" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="109" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>838</v>
       </c>
@@ -13276,10 +13340,10 @@
       <c r="E109" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F109" s="2"/>
       <c r="G109" s="2"/>
-      <c r="H109" s="2"/>
-    </row>
-    <row r="110" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="110" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>841</v>
       </c>
@@ -13295,10 +13359,10 @@
       <c r="E110" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F110" s="2"/>
       <c r="G110" s="2"/>
-      <c r="H110" s="2"/>
-    </row>
-    <row r="111" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="111" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>844</v>
       </c>
@@ -13314,10 +13378,10 @@
       <c r="E111" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F111" s="2"/>
       <c r="G111" s="2"/>
-      <c r="H111" s="2"/>
-    </row>
-    <row r="112" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="112" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>847</v>
       </c>
@@ -13333,10 +13397,10 @@
       <c r="E112" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F112" s="2"/>
       <c r="G112" s="2"/>
-      <c r="H112" s="2"/>
-    </row>
-    <row r="113" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="113" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>850</v>
       </c>
@@ -13352,10 +13416,10 @@
       <c r="E113" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F113" s="2"/>
       <c r="G113" s="2"/>
-      <c r="H113" s="2"/>
-    </row>
-    <row r="114" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="114" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>853</v>
       </c>
@@ -13371,10 +13435,10 @@
       <c r="E114" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F114" s="2"/>
       <c r="G114" s="2"/>
-      <c r="H114" s="2"/>
-    </row>
-    <row r="115" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="115" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>856</v>
       </c>
@@ -13390,10 +13454,10 @@
       <c r="E115" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F115" s="2"/>
       <c r="G115" s="2"/>
-      <c r="H115" s="2"/>
-    </row>
-    <row r="116" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="116" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>859</v>
       </c>
@@ -13409,10 +13473,10 @@
       <c r="E116" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F116" s="2"/>
       <c r="G116" s="2"/>
-      <c r="H116" s="2"/>
-    </row>
-    <row r="117" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="117" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>862</v>
       </c>
@@ -13428,10 +13492,10 @@
       <c r="E117" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F117" s="2"/>
       <c r="G117" s="2"/>
-      <c r="H117" s="2"/>
-    </row>
-    <row r="118" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="118" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>865</v>
       </c>
@@ -13447,10 +13511,10 @@
       <c r="E118" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F118" s="2"/>
       <c r="G118" s="2"/>
-      <c r="H118" s="2"/>
-    </row>
-    <row r="119" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="119" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>868</v>
       </c>
@@ -13466,10 +13530,10 @@
       <c r="E119" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F119" s="2"/>
       <c r="G119" s="2"/>
-      <c r="H119" s="2"/>
-    </row>
-    <row r="120" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="120" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>871</v>
       </c>
@@ -13485,10 +13549,10 @@
       <c r="E120" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F120" s="2"/>
       <c r="G120" s="2"/>
-      <c r="H120" s="2"/>
-    </row>
-    <row r="121" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="121" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>874</v>
       </c>
@@ -13504,10 +13568,10 @@
       <c r="E121" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F121" s="2"/>
       <c r="G121" s="2"/>
-      <c r="H121" s="2"/>
-    </row>
-    <row r="122" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="122" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>877</v>
       </c>
@@ -13523,10 +13587,10 @@
       <c r="E122" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F122" s="2"/>
       <c r="G122" s="2"/>
-      <c r="H122" s="2"/>
-    </row>
-    <row r="123" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="123" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>880</v>
       </c>
@@ -13542,10 +13606,10 @@
       <c r="E123" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F123" s="2"/>
       <c r="G123" s="2"/>
-      <c r="H123" s="2"/>
-    </row>
-    <row r="124" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="124" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>883</v>
       </c>
@@ -13561,10 +13625,10 @@
       <c r="E124" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F124" s="2"/>
       <c r="G124" s="2"/>
-      <c r="H124" s="2"/>
-    </row>
-    <row r="125" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="125" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>886</v>
       </c>
@@ -13580,10 +13644,10 @@
       <c r="E125" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F125" s="2"/>
       <c r="G125" s="2"/>
-      <c r="H125" s="2"/>
-    </row>
-    <row r="126" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="126" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>889</v>
       </c>
@@ -13599,10 +13663,10 @@
       <c r="E126" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F126" s="2"/>
       <c r="G126" s="2"/>
-      <c r="H126" s="2"/>
-    </row>
-    <row r="127" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="127" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>892</v>
       </c>
@@ -13618,10 +13682,10 @@
       <c r="E127" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F127" s="2"/>
       <c r="G127" s="2"/>
-      <c r="H127" s="2"/>
-    </row>
-    <row r="128" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="128" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>895</v>
       </c>
@@ -13637,10 +13701,10 @@
       <c r="E128" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F128" s="2"/>
       <c r="G128" s="2"/>
-      <c r="H128" s="2"/>
-    </row>
-    <row r="129" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="129" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>898</v>
       </c>
@@ -13656,10 +13720,10 @@
       <c r="E129" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F129" s="2"/>
       <c r="G129" s="2"/>
-      <c r="H129" s="2"/>
-    </row>
-    <row r="130" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="130" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>901</v>
       </c>
@@ -13675,10 +13739,10 @@
       <c r="E130" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F130" s="2"/>
       <c r="G130" s="2"/>
-      <c r="H130" s="2"/>
-    </row>
-    <row r="131" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="131" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>904</v>
       </c>
@@ -13694,10 +13758,10 @@
       <c r="E131" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F131" s="2"/>
       <c r="G131" s="2"/>
-      <c r="H131" s="2"/>
-    </row>
-    <row r="132" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="132" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>907</v>
       </c>
@@ -13713,10 +13777,10 @@
       <c r="E132" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F132" s="2"/>
       <c r="G132" s="2"/>
-      <c r="H132" s="2"/>
-    </row>
-    <row r="133" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="133" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>910</v>
       </c>
@@ -13732,10 +13796,10 @@
       <c r="E133" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F133" s="2"/>
       <c r="G133" s="2"/>
-      <c r="H133" s="2"/>
-    </row>
-    <row r="134" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="134" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>913</v>
       </c>
@@ -13751,10 +13815,10 @@
       <c r="E134" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F134" s="2"/>
       <c r="G134" s="2"/>
-      <c r="H134" s="2"/>
-    </row>
-    <row r="135" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="135" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>916</v>
       </c>
@@ -13770,10 +13834,10 @@
       <c r="E135" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F135" s="2"/>
       <c r="G135" s="2"/>
-      <c r="H135" s="2"/>
-    </row>
-    <row r="136" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="136" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>919</v>
       </c>
@@ -13789,10 +13853,10 @@
       <c r="E136" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F136" s="2"/>
       <c r="G136" s="2"/>
-      <c r="H136" s="2"/>
-    </row>
-    <row r="137" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="137" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>922</v>
       </c>
@@ -13808,10 +13872,10 @@
       <c r="E137" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F137" s="2"/>
       <c r="G137" s="2"/>
-      <c r="H137" s="2"/>
-    </row>
-    <row r="138" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="138" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>925</v>
       </c>
@@ -13827,10 +13891,10 @@
       <c r="E138" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F138" s="2"/>
       <c r="G138" s="2"/>
-      <c r="H138" s="2"/>
-    </row>
-    <row r="139" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="139" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>928</v>
       </c>
@@ -13846,10 +13910,10 @@
       <c r="E139" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F139" s="2"/>
       <c r="G139" s="2"/>
-      <c r="H139" s="2"/>
-    </row>
-    <row r="140" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="140" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>931</v>
       </c>
@@ -13865,10 +13929,10 @@
       <c r="E140" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F140" s="2"/>
       <c r="G140" s="2"/>
-      <c r="H140" s="2"/>
-    </row>
-    <row r="141" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="141" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>934</v>
       </c>
@@ -13884,10 +13948,10 @@
       <c r="E141" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F141" s="2"/>
       <c r="G141" s="2"/>
-      <c r="H141" s="2"/>
-    </row>
-    <row r="142" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="142" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>937</v>
       </c>
@@ -13903,10 +13967,10 @@
       <c r="E142" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F142" s="2"/>
       <c r="G142" s="2"/>
-      <c r="H142" s="2"/>
-    </row>
-    <row r="143" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="143" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>940</v>
       </c>
@@ -13922,10 +13986,10 @@
       <c r="E143" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F143" s="2"/>
       <c r="G143" s="2"/>
-      <c r="H143" s="2"/>
-    </row>
-    <row r="144" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="144" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>943</v>
       </c>
@@ -13941,10 +14005,10 @@
       <c r="E144" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F144" s="2"/>
       <c r="G144" s="2"/>
-      <c r="H144" s="2"/>
-    </row>
-    <row r="145" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="145" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>946</v>
       </c>
@@ -13960,10 +14024,10 @@
       <c r="E145" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F145" s="2"/>
       <c r="G145" s="2"/>
-      <c r="H145" s="2"/>
-    </row>
-    <row r="146" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="146" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>949</v>
       </c>
@@ -13979,10 +14043,10 @@
       <c r="E146" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F146" s="2"/>
       <c r="G146" s="2"/>
-      <c r="H146" s="2"/>
-    </row>
-    <row r="147" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="147" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>952</v>
       </c>
@@ -13998,10 +14062,10 @@
       <c r="E147" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F147" s="2"/>
       <c r="G147" s="2"/>
-      <c r="H147" s="2"/>
-    </row>
-    <row r="148" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="148" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>955</v>
       </c>
@@ -14017,10 +14081,10 @@
       <c r="E148" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F148" s="2"/>
       <c r="G148" s="2"/>
-      <c r="H148" s="2"/>
-    </row>
-    <row r="149" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="149" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>958</v>
       </c>
@@ -14036,10 +14100,10 @@
       <c r="E149" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F149" s="2"/>
       <c r="G149" s="2"/>
-      <c r="H149" s="2"/>
-    </row>
-    <row r="150" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="150" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>961</v>
       </c>
@@ -14055,10 +14119,10 @@
       <c r="E150" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F150" s="2"/>
       <c r="G150" s="2"/>
-      <c r="H150" s="2"/>
-    </row>
-    <row r="151" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="151" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>964</v>
       </c>
@@ -14074,10 +14138,10 @@
       <c r="E151" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F151" s="2"/>
       <c r="G151" s="2"/>
-      <c r="H151" s="2"/>
-    </row>
-    <row r="152" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="152" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>967</v>
       </c>
@@ -14093,10 +14157,10 @@
       <c r="E152" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F152" s="2"/>
       <c r="G152" s="2"/>
-      <c r="H152" s="2"/>
-    </row>
-    <row r="153" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="153" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>970</v>
       </c>
@@ -14112,10 +14176,10 @@
       <c r="E153" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F153" s="2"/>
       <c r="G153" s="2"/>
-      <c r="H153" s="2"/>
-    </row>
-    <row r="154" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="154" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>973</v>
       </c>
@@ -14131,10 +14195,10 @@
       <c r="E154" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F154" s="2"/>
       <c r="G154" s="2"/>
-      <c r="H154" s="2"/>
-    </row>
-    <row r="155" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="155" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>976</v>
       </c>
@@ -14150,10 +14214,10 @@
       <c r="E155" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F155" s="2"/>
       <c r="G155" s="2"/>
-      <c r="H155" s="2"/>
-    </row>
-    <row r="156" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="156" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>979</v>
       </c>
@@ -14169,10 +14233,10 @@
       <c r="E156" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F156" s="2"/>
       <c r="G156" s="2"/>
-      <c r="H156" s="2"/>
-    </row>
-    <row r="157" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="157" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>982</v>
       </c>
@@ -14188,10 +14252,10 @@
       <c r="E157" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F157" s="2"/>
       <c r="G157" s="2"/>
-      <c r="H157" s="2"/>
-    </row>
-    <row r="158" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="158" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>985</v>
       </c>
@@ -14207,10 +14271,10 @@
       <c r="E158" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F158" s="2"/>
       <c r="G158" s="2"/>
-      <c r="H158" s="2"/>
-    </row>
-    <row r="159" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="159" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>988</v>
       </c>
@@ -14226,10 +14290,10 @@
       <c r="E159" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F159" s="2"/>
       <c r="G159" s="2"/>
-      <c r="H159" s="2"/>
-    </row>
-    <row r="160" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="160" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>991</v>
       </c>
@@ -14245,10 +14309,10 @@
       <c r="E160" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F160" s="2"/>
       <c r="G160" s="2"/>
-      <c r="H160" s="2"/>
-    </row>
-    <row r="161" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="161" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>994</v>
       </c>
@@ -14264,10 +14328,10 @@
       <c r="E161" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F161" s="2"/>
       <c r="G161" s="2"/>
-      <c r="H161" s="2"/>
-    </row>
-    <row r="162" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="162" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>997</v>
       </c>
@@ -14283,10 +14347,10 @@
       <c r="E162" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F162" s="2"/>
       <c r="G162" s="2"/>
-      <c r="H162" s="2"/>
-    </row>
-    <row r="163" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="163" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>1000</v>
       </c>
@@ -14302,10 +14366,10 @@
       <c r="E163" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F163" s="2"/>
       <c r="G163" s="2"/>
-      <c r="H163" s="2"/>
-    </row>
-    <row r="164" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="164" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>1003</v>
       </c>
@@ -14321,10 +14385,10 @@
       <c r="E164" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F164" s="2"/>
       <c r="G164" s="2"/>
-      <c r="H164" s="2"/>
-    </row>
-    <row r="165" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="165" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>1006</v>
       </c>
@@ -14340,10 +14404,10 @@
       <c r="E165" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F165" s="2"/>
       <c r="G165" s="2"/>
-      <c r="H165" s="2"/>
-    </row>
-    <row r="166" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="166" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>1009</v>
       </c>
@@ -14359,10 +14423,10 @@
       <c r="E166" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F166" s="2"/>
       <c r="G166" s="2"/>
-      <c r="H166" s="2"/>
-    </row>
-    <row r="167" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="167" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>1012</v>
       </c>
@@ -14378,10 +14442,10 @@
       <c r="E167" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F167" s="2"/>
       <c r="G167" s="2"/>
-      <c r="H167" s="2"/>
-    </row>
-    <row r="168" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="168" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>1015</v>
       </c>
@@ -14397,10 +14461,10 @@
       <c r="E168" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F168" s="2"/>
       <c r="G168" s="2"/>
-      <c r="H168" s="2"/>
-    </row>
-    <row r="169" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="169" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>1018</v>
       </c>
@@ -14416,10 +14480,10 @@
       <c r="E169" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F169" s="2"/>
       <c r="G169" s="2"/>
-      <c r="H169" s="2"/>
-    </row>
-    <row r="170" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="170" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>1021</v>
       </c>
@@ -14435,10 +14499,10 @@
       <c r="E170" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F170" s="2"/>
       <c r="G170" s="2"/>
-      <c r="H170" s="2"/>
-    </row>
-    <row r="171" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="171" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>1024</v>
       </c>
@@ -14454,10 +14518,10 @@
       <c r="E171" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F171" s="2"/>
       <c r="G171" s="2"/>
-      <c r="H171" s="2"/>
-    </row>
-    <row r="172" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="172" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>1027</v>
       </c>
@@ -14473,10 +14537,10 @@
       <c r="E172" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F172" s="2"/>
       <c r="G172" s="2"/>
-      <c r="H172" s="2"/>
-    </row>
-    <row r="173" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="173" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>1030</v>
       </c>
@@ -14492,10 +14556,10 @@
       <c r="E173" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F173" s="2"/>
       <c r="G173" s="2"/>
-      <c r="H173" s="2"/>
-    </row>
-    <row r="174" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="174" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>1033</v>
       </c>
@@ -14511,10 +14575,10 @@
       <c r="E174" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F174" s="2"/>
       <c r="G174" s="2"/>
-      <c r="H174" s="2"/>
-    </row>
-    <row r="175" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="175" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
         <v>1036</v>
       </c>
@@ -14530,10 +14594,10 @@
       <c r="E175" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F175" s="2"/>
       <c r="G175" s="2"/>
-      <c r="H175" s="2"/>
-    </row>
-    <row r="176" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="176" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>1039</v>
       </c>
@@ -14549,10 +14613,10 @@
       <c r="E176" s="2" t="b">
         <v>1</v>
       </c>
+      <c r="F176" s="2"/>
       <c r="G176" s="2"/>
-      <c r="H176" s="2"/>
-    </row>
-    <row r="177" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="177" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
         <v>1042</v>
       </c>
@@ -14568,11 +14632,11 @@
       <c r="E177" s="2" t="b">
         <v>0</v>
       </c>
+      <c r="F177" s="2"/>
       <c r="G177" s="2"/>
-      <c r="H177" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H177"/>
+  <autoFilter ref="A1:G177"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -14585,7 +14649,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18175,615 +18239,613 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="143" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="143" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" customWidth="1"/>
-    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>514</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="6" t="s">
+        <v>1393</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>1325</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>1299</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>1360</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>1327</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D2" s="9">
+        <v>-34190.379999999997</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>1326</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>1299</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="G2" s="8" t="s">
+        <v>1168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
         <v>1361</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" s="7" t="s">
         <v>1328</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="6">
-        <v>-34190.379999999997</v>
-      </c>
-      <c r="E2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>1327</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>1168</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="C3" s="8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D3" s="9">
+        <v>-40890.379999999997</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
         <v>1362</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" s="7" t="s">
         <v>1329</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="6">
-        <v>-40890.379999999997</v>
-      </c>
-      <c r="E3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="C4" s="8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D4" s="9">
+        <v>-23190.38</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
         <v>1363</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" s="7" t="s">
         <v>1330</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="6">
-        <v>-23190.38</v>
-      </c>
-      <c r="E4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="C5" s="8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D5" s="9">
+        <v>-24290.38</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
         <v>1364</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" s="7" t="s">
         <v>1331</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="6">
-        <v>-24290.38</v>
-      </c>
-      <c r="E5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="C6" s="8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D6" s="9">
+        <v>-1101856</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
         <v>1365</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" s="7" t="s">
         <v>1332</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="6">
-        <v>-1101856</v>
-      </c>
-      <c r="E6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="C7" s="8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D7" s="9">
+        <v>-1164906</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
         <v>1366</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" s="7" t="s">
         <v>1333</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="6">
-        <v>-1164906</v>
-      </c>
-      <c r="E7" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="C8" s="8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D8" s="9">
+        <v>-22290.38</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
         <v>1367</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" s="7" t="s">
         <v>1334</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="6">
-        <v>-22290.38</v>
-      </c>
-      <c r="E8" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="C9" s="8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D9" s="9">
+        <v>-24690.38</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
         <v>1368</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" s="7" t="s">
         <v>1335</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="6">
-        <v>-24690.38</v>
-      </c>
-      <c r="E9" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="C10" s="8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D10" s="9">
+        <v>-22690.38</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
         <v>1369</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" s="7" t="s">
         <v>1336</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="6">
-        <v>-22690.38</v>
-      </c>
-      <c r="E10" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="C11" s="8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D11" s="9">
+        <v>-31190.38</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
         <v>1370</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" s="7" t="s">
         <v>1337</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="6">
-        <v>-31190.38</v>
-      </c>
-      <c r="E11" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="C12" s="8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D12" s="9">
+        <v>-1728316</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
         <v>1371</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" s="7" t="s">
         <v>1338</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="6">
-        <v>-1728316</v>
-      </c>
-      <c r="E12" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="C13" s="8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D13" s="9">
+        <v>-1521617000</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
         <v>1372</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" s="7" t="s">
         <v>1339</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="6">
-        <v>-1521617000</v>
-      </c>
-      <c r="E13" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="C14" s="8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D14" s="9">
+        <v>-21590.38</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
         <v>1373</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" s="7" t="s">
         <v>1340</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="6">
-        <v>-21590.38</v>
-      </c>
-      <c r="E14" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="C15" s="8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D15" s="9">
+        <v>-29290.38</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
         <v>1374</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" s="7" t="s">
         <v>1341</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="6">
-        <v>-29290.38</v>
-      </c>
-      <c r="E15" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="C16" s="8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D16" s="9">
+        <v>-41190.379999999997</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
         <v>1375</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" s="7" t="s">
         <v>1342</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="6">
-        <v>-41190.379999999997</v>
-      </c>
-      <c r="E16" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="C17" s="8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D17" s="9">
+        <v>-21990.38</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
         <v>1376</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" s="7" t="s">
         <v>1343</v>
       </c>
-      <c r="C17" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="6">
+      <c r="C18" s="8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D18" s="9">
+        <v>-21390.38</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>1377</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>1344</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D19" s="9">
+        <v>-23890.38</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
+        <v>1378</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>1345</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D20" s="9">
+        <v>-34390.379999999997</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
+        <v>1379</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>1346</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D21" s="9">
+        <v>-44490.38</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
+        <v>1380</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>1347</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D22" s="9">
+        <v>-36190.379999999997</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
+        <v>1381</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>1348</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D23" s="9">
+        <v>-22190.38</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
+        <v>1382</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>1349</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D24" s="9">
         <v>-21990.38</v>
       </c>
-      <c r="E17" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>1377</v>
-      </c>
-      <c r="B18" t="s">
-        <v>1344</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="6">
-        <v>-21390.38</v>
-      </c>
-      <c r="E18" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>1378</v>
-      </c>
-      <c r="B19" t="s">
-        <v>1345</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="6">
-        <v>-23890.38</v>
-      </c>
-      <c r="E19" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>1379</v>
-      </c>
-      <c r="B20" t="s">
-        <v>1346</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="6">
-        <v>-34390.379999999997</v>
-      </c>
-      <c r="E20" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>1380</v>
-      </c>
-      <c r="B21" t="s">
-        <v>1347</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" s="6">
-        <v>-44490.38</v>
-      </c>
-      <c r="E21" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>1381</v>
-      </c>
-      <c r="B22" t="s">
-        <v>1348</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="6">
-        <v>-36190.379999999997</v>
-      </c>
-      <c r="E22" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>1382</v>
-      </c>
-      <c r="B23" t="s">
-        <v>1349</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="6">
-        <v>-22190.38</v>
-      </c>
-      <c r="E23" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="E24" s="7" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="7" t="s">
         <v>1383</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" s="7" t="s">
         <v>1350</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D24" s="6">
-        <v>-21990.38</v>
-      </c>
-      <c r="E24" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="C25" s="8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D25" s="9">
+        <v>-1132896</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="7" t="s">
         <v>1384</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" s="7" t="s">
         <v>1351</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="6">
-        <v>-1132896</v>
-      </c>
-      <c r="E25" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="C26" s="8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D26" s="9">
+        <v>-33790.379999999997</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="7" t="s">
         <v>1385</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" s="7" t="s">
         <v>1352</v>
       </c>
-      <c r="C26" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="6">
-        <v>-33790.379999999997</v>
-      </c>
-      <c r="E26" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="C27" s="8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D27" s="9">
+        <v>1035619</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="7" t="s">
         <v>1386</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" s="7" t="s">
         <v>1353</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27" s="6">
-        <v>1035619</v>
-      </c>
-      <c r="E27" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="C28" s="8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D28" s="9">
+        <v>1098019</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="7" t="s">
         <v>1387</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" s="7" t="s">
         <v>1354</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" s="6">
-        <v>1098019</v>
-      </c>
-      <c r="E28" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="C29" s="8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D29" s="9">
+        <v>581419.19999999995</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="7" t="s">
         <v>1388</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" s="7" t="s">
         <v>1355</v>
       </c>
-      <c r="C29" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29" s="6">
-        <v>581419.19999999995</v>
-      </c>
-      <c r="E29" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="C30" s="8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D30" s="9">
+        <v>1052899</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="7" t="s">
         <v>1389</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" s="7" t="s">
         <v>1356</v>
       </c>
-      <c r="C30" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D30" s="6">
-        <v>1052899</v>
-      </c>
-      <c r="E30" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="C31" s="8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D31" s="9">
+        <v>4972350</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="7" t="s">
         <v>1390</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B32" s="7" t="s">
         <v>1357</v>
       </c>
-      <c r="C31" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="6">
-        <v>4972350</v>
-      </c>
-      <c r="E31" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="C32" s="8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D32" s="9">
+        <v>471096.2</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="7" t="s">
         <v>1391</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B33" s="7" t="s">
         <v>1358</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32" s="6">
-        <v>471096.2</v>
-      </c>
-      <c r="E32" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="C33" s="8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D33" s="9">
+        <v>4381069</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="7" t="s">
         <v>1392</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" s="7" t="s">
         <v>1359</v>
       </c>
-      <c r="C33" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D33" s="6">
-        <v>4381069</v>
-      </c>
-      <c r="E33" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>1393</v>
-      </c>
-      <c r="B34" t="s">
-        <v>1360</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D34" s="6">
+      <c r="C34" s="8" t="s">
+        <v>1394</v>
+      </c>
+      <c r="D34" s="9">
         <v>1066339</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="7" t="s">
         <v>368</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A27:E34">
-    <sortCondition ref="A27:A34"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
create ObjectiveFunction, and add as attribute to Submodel; move some docstrings from wc_lang to obj_model
</commit_message>
<xml_diff>
--- a/tests/fixtures/example-model.xlsx
+++ b/tests/fixtures/example-model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38700" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="940" windowWidth="28060" windowHeight="17060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Reactions!$A$1:$I$176</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">References!$A$1:$R$20</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Species types'!$A$1:$J$144</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Submodels!$A$1:$G$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Submodels!$A$1:$I$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Taxon!$A$1:$B$6</definedName>
   </definedNames>
   <calcPr calcId="0" concurrentCalc="0"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2735" uniqueCount="1392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2737" uniqueCount="1394">
   <si>
     <t>Id</t>
   </si>
@@ -4228,6 +4228,12 @@
   </si>
   <si>
     <t>No comment</t>
+  </si>
+  <si>
+    <t>Objective function</t>
+  </si>
+  <si>
+    <t>2 * AdnTransport + Metabolism_biomass</t>
   </si>
 </sst>
 </file>
@@ -4669,12 +4675,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -4724,10 +4725,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView zoomScale="232" zoomScaleNormal="232" zoomScalePageLayoutView="232" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="180" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4736,7 +4737,7 @@
     <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4744,16 +4745,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>512</v>
+        <v>7</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>1389</v>
       </c>
@@ -4761,9 +4759,6 @@
         <v>1390</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
         <v>1391</v>
       </c>
     </row>
@@ -4776,12 +4771,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -4931,12 +4921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -5718,12 +5703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J1" sqref="J1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -6121,12 +6101,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -6182,18 +6157,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView zoomScale="154" zoomScaleNormal="154" zoomScalePageLayoutView="154" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="190" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6210,13 +6187,19 @@
         <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>1388</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1392</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
@@ -6232,10 +6215,16 @@
       <c r="E2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F2" s="5" t="s">
+        <v>1389</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>1393</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -6253,8 +6242,10 @@
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-    </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+    </row>
+    <row r="4" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -6272,8 +6263,10 @@
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -6291,9 +6284,11 @@
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G5"/>
+  <autoFilter ref="A1:I5"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -6302,12 +6297,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView zoomScale="135" zoomScaleNormal="135" zoomScalePageLayoutView="135" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -6381,12 +6371,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J144"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A18" sqref="A18:XFD18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -9818,12 +9803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D126"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -11221,15 +11201,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I176"/>
   <sheetViews>
-    <sheetView zoomScale="157" zoomScaleNormal="157" zoomScalePageLayoutView="157" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F1" sqref="F1:G1048576"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane ySplit="980" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="23" customWidth="1"/>
     <col min="2" max="2" width="23.83203125" customWidth="1"/>
     <col min="4" max="4" width="33.1640625" customWidth="1"/>
   </cols>
@@ -14932,11 +14911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G168"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="166" zoomScaleNormal="166" zoomScalePageLayoutView="166" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L21" sqref="L21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18186,8 +18162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView zoomScale="143" zoomScaleNormal="143" zoomScalePageLayoutView="143" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
parse objective functions into a linear representation and save them in ObjectiveFunction expand BiomassReaction: add a compartment attribute, ensure that all their species are defined, and write them to SBML
</commit_message>
<xml_diff>
--- a/tests/fixtures/example-model.xlsx
+++ b/tests/fixtures/example-model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="940" windowWidth="28060" windowHeight="17060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="3260" windowWidth="28680" windowHeight="17880" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2737" uniqueCount="1394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2744" uniqueCount="1398">
   <si>
     <t>Id</t>
   </si>
@@ -4233,7 +4233,19 @@
     <t>Objective function</t>
   </si>
   <si>
-    <t>2 * AdnTransport + Metabolism_biomass</t>
+    <t>Other_biomass</t>
+  </si>
+  <si>
+    <t>Other biomass</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>E.g., obj. fn.</t>
+  </si>
+  <si>
+    <t>Metabolism_biomass + AdnTransport</t>
   </si>
 </sst>
 </file>
@@ -4675,7 +4687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -4725,41 +4737,62 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="180" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>1389</v>
       </c>
       <c r="B2" t="s">
         <v>1390</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
         <v>1391</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>1393</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1394</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1395</v>
       </c>
     </row>
   </sheetData>
@@ -6159,15 +6192,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" zoomScalePageLayoutView="190" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3:G5"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="180" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="34.33203125" customWidth="1"/>
+    <col min="7" max="7" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -6218,10 +6251,12 @@
       <c r="F2" s="5" t="s">
         <v>1389</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>1393</v>
-      </c>
-      <c r="H2" s="2"/>
+      <c r="G2" s="5" t="s">
+        <v>1397</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>1396</v>
+      </c>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -14911,7 +14946,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G168"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -18163,7 +18198,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add biomass_reaction to the 'types' searched by Model.get_component() update get_model_summary() with new Models update a docstring
</commit_message>
<xml_diff>
--- a/tests/fixtures/example-model.xlsx
+++ b/tests/fixtures/example-model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3260" windowWidth="28680" windowHeight="17880" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="180" yWindow="660" windowWidth="24940" windowHeight="15540" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -4740,7 +4740,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="180" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5736,7 +5736,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="114" zoomScaleNormal="114" zoomScalePageLayoutView="114" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -6192,8 +6194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="180" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="180" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6332,7 +6334,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="142" zoomScaleNormal="142" zoomScalePageLayoutView="142" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -6406,7 +6408,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J144"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A98" workbookViewId="0">
+      <selection activeCell="A117" sqref="A117"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -9838,7 +9842,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D126"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A90" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="A104" sqref="A104"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -11236,9 +11242,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I176"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <pane ySplit="980" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <pane ySplit="980" topLeftCell="A163" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="I176" sqref="A1:I176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14937,7 +14943,11 @@
       <c r="I176" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I176"/>
+  <autoFilter ref="A1:I176">
+    <sortState ref="A2:I176">
+      <sortCondition ref="A2:A176"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -14946,8 +14956,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G168"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18198,7 +18208,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
adding stop condition and adding tests for config
</commit_message>
<xml_diff>
--- a/tests/fixtures/example-model.xlsx
+++ b/tests/fixtures/example-model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,43 +20,55 @@
     <sheet name="Biomass components" sheetId="10" state="visible" r:id="rId11"/>
     <sheet name="Biomass reactions" sheetId="11" state="visible" r:id="rId12"/>
     <sheet name="Parameters" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="References" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="Database references" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="Stop conditions" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="References" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="Database references" sheetId="15" state="visible" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
     <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">Concentrations!$A$1:$D$126</definedName>
-    <definedName function="false" hidden="true" localSheetId="13" name="_xlnm._FilterDatabase" vbProcedure="false">'Database references'!$A$1:$J$20</definedName>
+    <definedName function="false" hidden="true" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">'Database references'!$A$1:$J$20</definedName>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Model!$A$1:$B$5</definedName>
     <definedName function="false" hidden="true" localSheetId="11" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$H$6</definedName>
     <definedName function="false" hidden="true" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">'Rate laws'!$A$1:$G$168</definedName>
     <definedName function="false" hidden="true" localSheetId="7" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$I$176</definedName>
-    <definedName function="false" hidden="true" localSheetId="12" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$R$20</definedName>
+    <definedName function="false" hidden="true" localSheetId="13" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$R$20</definedName>
     <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$J$144</definedName>
     <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Submodels!$A$1:$I$5</definedName>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Taxon!$A$1:$B$6</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Model!$A$1:$B$5</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Model!$A$1:$B$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Model!$A$1:$B$5</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Taxon!$A$1:$B$6</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">Taxon!$A$1:$B$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Taxon!$A$1:$B$6</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Submodels!$A$1:$I$5</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">Submodels!$A$1:$I$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Submodels!$A$1:$I$5</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$J$144</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$J$144</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$J$144</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">Concentrations!$A$1:$D$126</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">Concentrations!$A$1:$D$126</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Concentrations!$A$1:$D$126</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$I$176</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$I$176</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$I$176</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">'Rate laws'!$A$1:$G$168</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Rate laws'!$A$1:$G$168</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Rate laws'!$A$1:$G$168</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$H$6</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$H$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$R$20</definedName>
-    <definedName function="false" hidden="false" localSheetId="12" name="_xlnm._FilterDatabase_0" vbProcedure="false">References!$A$1:$R$20</definedName>
-    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase" vbProcedure="false">'Database references'!$A$1:$J$20</definedName>
-    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Database references'!$A$1:$J$20</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$H$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$R$20</definedName>
+    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0" vbProcedure="false">References!$A$1:$R$20</definedName>
+    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">References!$A$1:$R$20</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">'Database references'!$A$1:$J$20</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Database references'!$A$1:$J$20</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Database references'!$A$1:$J$20</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -68,7 +80,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2761" uniqueCount="1407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2778" uniqueCount="1416">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -3863,6 +3875,33 @@
   </si>
   <si>
     <t xml:space="preserve">RNA half life</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stop_cond_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATP[c] &gt; 1.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stop_cond_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATP[c] + ADP[c] + AMP[c] &lt; 2.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stop_cond_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AXP_c &gt;= 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stop_cond_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H2O[c] + AXP_c &lt;= -1</t>
   </si>
   <si>
     <t xml:space="preserve">Title</t>
@@ -4636,13 +4675,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="13.2834008097166"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="17.246963562753"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="6" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="20.6720647773279"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="6" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="6" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="6" width="9.31983805668016"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="6" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="6" width="10.8178137651822"/>
   </cols>
   <sheetData>
@@ -5260,8 +5299,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.246963562753"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="23.4574898785425"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -5329,19 +5368,19 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="177" zoomScaleNormal="177" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="23.6720647773279"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2834008097166"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4251012145749"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.1417004048583"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.5344129554656"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="11" width="31.5991902834008"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="11" width="31.8137651821862"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -5499,6 +5538,102 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D8" activeCellId="0" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.1"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1265</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>1266</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>1267</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>1268</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>1270</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>1271</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>1272</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>1273</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:R20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -5521,46 +5656,46 @@
         <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1265</v>
+        <v>1274</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1266</v>
+        <v>1275</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1267</v>
+        <v>1276</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1268</v>
+        <v>1277</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>41</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>1269</v>
+        <v>1278</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1270</v>
+        <v>1279</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>1271</v>
+        <v>1280</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>1272</v>
+        <v>1281</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>1273</v>
+        <v>1282</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>1274</v>
+        <v>1283</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>1275</v>
+        <v>1284</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>1276</v>
+        <v>1285</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>1277</v>
+        <v>1286</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>7</v>
@@ -5571,40 +5706,40 @@
         <v>32</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1278</v>
+        <v>1287</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>1279</v>
+        <v>1288</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>1280</v>
+        <v>1289</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="n">
         <v>2008</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>1281</v>
+        <v>1290</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>1282</v>
+        <v>1291</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2" t="s">
-        <v>1283</v>
+        <v>1292</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>1283</v>
+        <v>1292</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2" t="s">
-        <v>1284</v>
+        <v>1293</v>
       </c>
       <c r="R2" s="2"/>
     </row>
@@ -5613,26 +5748,26 @@
         <v>36</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1285</v>
+        <v>1294</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>1286</v>
+        <v>1295</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>1287</v>
+        <v>1296</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2" t="n">
         <v>2014</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>1281</v>
+        <v>1290</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>1288</v>
+        <v>1297</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -5642,127 +5777,127 @@
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2" t="s">
-        <v>1289</v>
+        <v>1298</v>
       </c>
       <c r="R3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>1290</v>
+        <v>1299</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>1291</v>
+        <v>1300</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>1292</v>
+        <v>1301</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>1293</v>
+        <v>1302</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="n">
         <v>2004</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>1281</v>
+        <v>1290</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>1288</v>
+        <v>1297</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2" t="s">
-        <v>1294</v>
+        <v>1303</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>1295</v>
+        <v>1304</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2" t="s">
-        <v>1296</v>
+        <v>1305</v>
       </c>
       <c r="R4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>1297</v>
+        <v>1306</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>1298</v>
+        <v>1307</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>1299</v>
+        <v>1308</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>1300</v>
+        <v>1309</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2" t="n">
         <v>2009</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>1281</v>
+        <v>1290</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>1301</v>
+        <v>1310</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2" t="s">
-        <v>1302</v>
+        <v>1311</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>1303</v>
+        <v>1312</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2" t="s">
-        <v>1304</v>
+        <v>1313</v>
       </c>
       <c r="R5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>1305</v>
+        <v>1314</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>1306</v>
+        <v>1315</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>1307</v>
+        <v>1316</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>1308</v>
+        <v>1317</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="n">
         <v>2007</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>1281</v>
+        <v>1290</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>1309</v>
+        <v>1318</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2" t="s">
-        <v>1310</v>
+        <v>1319</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>1283</v>
+        <v>1292</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -5775,27 +5910,27 @@
         <v>1259</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>1311</v>
+        <v>1320</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>1312</v>
+        <v>1321</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>1313</v>
+        <v>1322</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="n">
         <v>2001</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>1314</v>
+        <v>1323</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2" t="s">
-        <v>1315</v>
+        <v>1324</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
@@ -5811,29 +5946,29 @@
         <v>1064</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>1316</v>
+        <v>1325</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>1317</v>
+        <v>1326</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>1318</v>
+        <v>1327</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2" t="n">
         <v>2006</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>1319</v>
+        <v>1328</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>1320</v>
+        <v>1329</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>1321</v>
+        <v>1330</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
@@ -5846,211 +5981,211 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>1322</v>
+        <v>1331</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>1323</v>
+        <v>1332</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>1324</v>
+        <v>1333</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>1325</v>
+        <v>1334</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2" t="n">
         <v>1993</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>1281</v>
+        <v>1290</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>1326</v>
+        <v>1335</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2" t="s">
-        <v>1327</v>
+        <v>1336</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>1283</v>
+        <v>1292</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2" t="s">
-        <v>1328</v>
+        <v>1337</v>
       </c>
       <c r="R9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>1329</v>
+        <v>1338</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>1330</v>
+        <v>1339</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>1331</v>
+        <v>1340</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>1332</v>
+        <v>1341</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2" t="n">
         <v>2010</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>1281</v>
+        <v>1290</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>1333</v>
+        <v>1342</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2" t="s">
-        <v>1334</v>
+        <v>1343</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>1310</v>
+        <v>1319</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2" t="s">
-        <v>1335</v>
+        <v>1344</v>
       </c>
       <c r="R10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>1336</v>
+        <v>1345</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>1337</v>
+        <v>1346</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>1338</v>
+        <v>1347</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>1339</v>
+        <v>1348</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2" t="n">
         <v>2000</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>1281</v>
+        <v>1290</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>1340</v>
+        <v>1349</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2" t="s">
-        <v>1341</v>
+        <v>1350</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>1342</v>
+        <v>1351</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2" t="s">
-        <v>1343</v>
+        <v>1352</v>
       </c>
       <c r="R11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>1344</v>
+        <v>1353</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>1345</v>
+        <v>1354</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>1346</v>
+        <v>1355</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>1347</v>
+        <v>1356</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="n">
         <v>1999</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>1281</v>
+        <v>1290</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>1348</v>
+        <v>1357</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2" t="s">
-        <v>1283</v>
+        <v>1292</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>1310</v>
+        <v>1319</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2" t="s">
-        <v>1349</v>
+        <v>1358</v>
       </c>
       <c r="R12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>1350</v>
+        <v>1359</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>1351</v>
+        <v>1360</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>1352</v>
+        <v>1361</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>1353</v>
+        <v>1362</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2" t="n">
         <v>1979</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>1281</v>
+        <v>1290</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>1340</v>
+        <v>1349</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2" t="s">
-        <v>1354</v>
+        <v>1363</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>1355</v>
+        <v>1364</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2" t="s">
-        <v>1356</v>
+        <v>1365</v>
       </c>
       <c r="R13" s="2"/>
     </row>
@@ -6059,40 +6194,40 @@
         <v>46</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>1357</v>
+        <v>1366</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>1358</v>
+        <v>1367</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>1359</v>
+        <v>1368</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2" t="n">
         <v>2012</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>1281</v>
+        <v>1290</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>1360</v>
+        <v>1369</v>
       </c>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2" t="s">
-        <v>1361</v>
+        <v>1370</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>1303</v>
+        <v>1312</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2" t="s">
-        <v>1362</v>
+        <v>1371</v>
       </c>
       <c r="R14" s="2"/>
     </row>
@@ -6101,59 +6236,59 @@
         <v>159</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>1363</v>
+        <v>1372</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>1364</v>
+        <v>1373</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>1365</v>
+        <v>1374</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2" t="n">
         <v>2009</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>1281</v>
+        <v>1290</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>1366</v>
+        <v>1375</v>
       </c>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2" t="s">
-        <v>1367</v>
+        <v>1376</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>1368</v>
+        <v>1377</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2" t="s">
-        <v>1369</v>
+        <v>1378</v>
       </c>
       <c r="R15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>1370</v>
+        <v>1379</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>1371</v>
+        <v>1380</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2" t="s">
-        <v>1372</v>
+        <v>1381</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -6168,20 +6303,20 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>1373</v>
+        <v>1382</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>1374</v>
+        <v>1383</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2" t="s">
-        <v>1372</v>
+        <v>1381</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -6196,20 +6331,20 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>1375</v>
+        <v>1384</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>1376</v>
+        <v>1385</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2" t="s">
-        <v>1372</v>
+        <v>1381</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -6224,20 +6359,20 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>1377</v>
+        <v>1386</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>1378</v>
+        <v>1387</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2" t="s">
-        <v>1372</v>
+        <v>1381</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -6259,13 +6394,13 @@
         <v>1</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>1379</v>
+        <v>1388</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2" t="s">
-        <v>1372</v>
+        <v>1381</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -6291,7 +6426,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -6309,19 +6444,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>1380</v>
+        <v>1389</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1381</v>
+        <v>1390</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1382</v>
+        <v>1391</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1383</v>
+        <v>1392</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>526</v>
@@ -6336,15 +6471,15 @@
         <v>1055</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1384</v>
+        <v>1393</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>1385</v>
+        <v>1394</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1386</v>
+        <v>1395</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -6354,15 +6489,15 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
-        <v>1329</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>1385</v>
+        <v>1394</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1387</v>
+        <v>1396</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -6372,15 +6507,15 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2" t="s">
-        <v>1344</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>1385</v>
+        <v>1394</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1388</v>
+        <v>1397</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -6395,10 +6530,10 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>1385</v>
+        <v>1394</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1389</v>
+        <v>1398</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -6408,15 +6543,15 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2" t="s">
-        <v>1322</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>1385</v>
+        <v>1394</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1390</v>
+        <v>1399</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -6431,10 +6566,10 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>1385</v>
+        <v>1394</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1391</v>
+        <v>1400</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -6444,15 +6579,15 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2" t="s">
-        <v>1305</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>1385</v>
+        <v>1394</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>1392</v>
+        <v>1401</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -6462,15 +6597,15 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2" t="s">
-        <v>1336</v>
+        <v>1345</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>1385</v>
+        <v>1394</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1393</v>
+        <v>1402</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -6480,15 +6615,15 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2" t="s">
-        <v>1290</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>1385</v>
+        <v>1394</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1394</v>
+        <v>1403</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -6503,10 +6638,10 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>1385</v>
+        <v>1394</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>1395</v>
+        <v>1404</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -6521,10 +6656,10 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>1385</v>
+        <v>1394</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>1396</v>
+        <v>1405</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -6539,10 +6674,10 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>1385</v>
+        <v>1394</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>1397</v>
+        <v>1406</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -6552,15 +6687,15 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2" t="s">
-        <v>1297</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>1398</v>
+        <v>1407</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>1399</v>
+        <v>1408</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -6575,10 +6710,10 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>1400</v>
+        <v>1409</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>1401</v>
+        <v>1410</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -6588,18 +6723,18 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2" t="s">
-        <v>1350</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>1382</v>
+        <v>1391</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1402</v>
+        <v>1411</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>1402</v>
+        <v>1411</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -6608,18 +6743,18 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2" t="s">
-        <v>1375</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>1382</v>
+        <v>1391</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>1403</v>
+        <v>1412</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>1403</v>
+        <v>1412</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -6633,13 +6768,13 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>1382</v>
+        <v>1391</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>1404</v>
+        <v>1413</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>1404</v>
+        <v>1413</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -6648,18 +6783,18 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2" t="s">
-        <v>1370</v>
+        <v>1379</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>1382</v>
+        <v>1391</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>1405</v>
+        <v>1414</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>1405</v>
+        <v>1414</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -6668,18 +6803,18 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2" t="s">
-        <v>1373</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>1382</v>
+        <v>1391</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>1406</v>
+        <v>1415</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>1406</v>
+        <v>1415</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -6688,7 +6823,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2" t="s">
-        <v>1377</v>
+        <v>1386</v>
       </c>
     </row>
   </sheetData>
@@ -6793,10 +6928,10 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.0323886639676"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.0647773279352"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.2793522267206"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -6946,7 +7081,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -11892,12 +12027,12 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="bottomRight" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -11995,15 +12130,15 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="bottomRight" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.4251012145749"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.7408906882591"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.0647773279352"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -15722,7 +15857,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.6032388663968"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
making stop conditions only functions of observables and checking they evaluate to a bool
</commit_message>
<xml_diff>
--- a/tests/fixtures/example-model.xlsx
+++ b/tests/fixtures/example-model.xlsx
@@ -39,36 +39,47 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Model!$A$1:$B$5</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Model!$A$1:$B$5</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Model!$A$1:$B$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Model!$A$1:$B$5</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Taxon!$A$1:$B$6</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">Taxon!$A$1:$B$6</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Taxon!$A$1:$B$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Taxon!$A$1:$B$6</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Submodels!$A$1:$I$5</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">Submodels!$A$1:$I$5</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Submodels!$A$1:$I$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Submodels!$A$1:$I$5</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$J$144</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$J$144</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$J$144</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$144</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">Concentrations!$A$1:$D$126</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">Concentrations!$A$1:$D$126</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Concentrations!$A$1:$D$126</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Concentrations!$A$1:$D$126</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$I$176</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$I$176</definedName>
     <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$I$176</definedName>
+    <definedName function="false" hidden="false" localSheetId="7" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Reactions!$A$1:$I$176</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase" vbProcedure="false">'Rate laws'!$A$1:$G$168</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Rate laws'!$A$1:$G$168</definedName>
     <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Rate laws'!$A$1:$G$168</definedName>
+    <definedName function="false" hidden="false" localSheetId="8" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Rate laws'!$A$1:$G$168</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$H$6</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$H$6</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$H$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$H$6</definedName>
     <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$R$20</definedName>
     <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0" vbProcedure="false">References!$A$1:$R$20</definedName>
     <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">References!$A$1:$R$20</definedName>
+    <definedName function="false" hidden="false" localSheetId="13" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">References!$A$1:$R$20</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">'Database references'!$A$1:$J$20</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Database references'!$A$1:$J$20</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Database references'!$A$1:$J$20</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Database references'!$A$1:$J$20</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -80,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2778" uniqueCount="1416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2772" uniqueCount="1412">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -3883,25 +3894,13 @@
     <t xml:space="preserve">stop_cond_1</t>
   </si>
   <si>
-    <t xml:space="preserve">ATP[c] &gt; 1.5</t>
+    <t xml:space="preserve">AXP_c &gt;= 1</t>
   </si>
   <si>
     <t xml:space="preserve">stop_cond_2</t>
   </si>
   <si>
-    <t xml:space="preserve">ATP[c] + ADP[c] + AMP[c] &lt; 2.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stop_cond_3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AXP_c &gt;= 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stop_cond_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H2O[c] + AXP_c &lt;= -1</t>
+    <t xml:space="preserve">AXP_c + NTP_c &lt;= -1</t>
   </si>
   <si>
     <t xml:space="preserve">Title</t>
@@ -4676,8 +4675,8 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="6" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="17.3522267206478"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="20.6720647773279"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="6" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="20.7813765182186"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="6" width="9.31983805668016"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="6" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="6" width="9.31983805668016"/>
@@ -5299,8 +5298,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.3522267206478"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="23.5668016194332"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -5373,13 +5372,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.4615384615385"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="23.8866396761134"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="24.1012145748988"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5344129554656"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.1417004048583"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="11" width="31.8137651821862"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="11" width="32.0283400809717"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="10.6032388663968"/>
   </cols>
@@ -5538,19 +5537,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="bottomRight" activeCell="D4" activeCellId="0" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.1"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5592,30 +5591,6 @@
       </c>
       <c r="D3" s="2" t="s">
         <v>1269</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>1270</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>1271</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>1272</v>
-      </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>1273</v>
       </c>
     </row>
   </sheetData>
@@ -5656,46 +5631,46 @@
         <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>1274</v>
+        <v>1270</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1275</v>
+        <v>1271</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>1276</v>
+        <v>1272</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>1277</v>
+        <v>1273</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>41</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>1274</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>1275</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>1276</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>1277</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>1278</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>1279</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>1280</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>1281</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>1282</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>1283</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>1284</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>1285</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>1286</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>7</v>
@@ -5706,40 +5681,40 @@
         <v>32</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1287</v>
+        <v>1283</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>1288</v>
+        <v>1284</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>1289</v>
+        <v>1285</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="n">
         <v>2008</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>1290</v>
+        <v>1286</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>1291</v>
+        <v>1287</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2" t="s">
-        <v>1292</v>
+        <v>1288</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>1292</v>
+        <v>1288</v>
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2" t="s">
-        <v>1293</v>
+        <v>1289</v>
       </c>
       <c r="R2" s="2"/>
     </row>
@@ -5748,26 +5723,26 @@
         <v>36</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1294</v>
+        <v>1290</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>1295</v>
+        <v>1291</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>1296</v>
+        <v>1292</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2" t="n">
         <v>2014</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>1290</v>
+        <v>1286</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>1297</v>
+        <v>1293</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -5777,127 +5752,127 @@
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2" t="s">
-        <v>1298</v>
+        <v>1294</v>
       </c>
       <c r="R3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>1299</v>
+        <v>1295</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>1300</v>
+        <v>1296</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>1301</v>
+        <v>1297</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>1302</v>
+        <v>1298</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2" t="n">
         <v>2004</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>1290</v>
+        <v>1286</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>1297</v>
+        <v>1293</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2" t="s">
-        <v>1303</v>
+        <v>1299</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>1304</v>
+        <v>1300</v>
       </c>
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2" t="s">
-        <v>1305</v>
+        <v>1301</v>
       </c>
       <c r="R4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>1306</v>
+        <v>1302</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>1307</v>
+        <v>1303</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>1308</v>
+        <v>1304</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>1309</v>
+        <v>1305</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2" t="n">
         <v>2009</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>1290</v>
+        <v>1286</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>1310</v>
+        <v>1306</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2" t="s">
-        <v>1311</v>
+        <v>1307</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>1312</v>
+        <v>1308</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2" t="s">
-        <v>1313</v>
+        <v>1309</v>
       </c>
       <c r="R5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>1314</v>
+        <v>1310</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>1315</v>
+        <v>1311</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>1316</v>
+        <v>1312</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>1317</v>
+        <v>1313</v>
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="n">
         <v>2007</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>1290</v>
+        <v>1286</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>1318</v>
+        <v>1314</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2" t="s">
-        <v>1319</v>
+        <v>1315</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>1292</v>
+        <v>1288</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
@@ -5910,27 +5885,27 @@
         <v>1259</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>1320</v>
+        <v>1316</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>1321</v>
+        <v>1317</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>1322</v>
+        <v>1318</v>
       </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="n">
         <v>2001</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>1323</v>
+        <v>1319</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2" t="s">
-        <v>1324</v>
+        <v>1320</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
@@ -5946,29 +5921,29 @@
         <v>1064</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>1325</v>
+        <v>1321</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>1326</v>
+        <v>1322</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>1327</v>
+        <v>1323</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2" t="n">
         <v>2006</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>1328</v>
+        <v>1324</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>1329</v>
+        <v>1325</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>1330</v>
+        <v>1326</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
@@ -5981,211 +5956,211 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>1331</v>
+        <v>1327</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>1332</v>
+        <v>1328</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>1333</v>
+        <v>1329</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>1334</v>
+        <v>1330</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2" t="n">
         <v>1993</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>1290</v>
+        <v>1286</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>1335</v>
+        <v>1331</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2" t="s">
-        <v>1336</v>
+        <v>1332</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>1292</v>
+        <v>1288</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2" t="s">
-        <v>1337</v>
+        <v>1333</v>
       </c>
       <c r="R9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>1338</v>
+        <v>1334</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>1339</v>
+        <v>1335</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>1340</v>
+        <v>1336</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>1341</v>
+        <v>1337</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2" t="n">
         <v>2010</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>1290</v>
+        <v>1286</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>1342</v>
+        <v>1338</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2" t="s">
-        <v>1343</v>
+        <v>1339</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>1319</v>
+        <v>1315</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2" t="s">
-        <v>1344</v>
+        <v>1340</v>
       </c>
       <c r="R10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>1345</v>
+        <v>1341</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>1346</v>
+        <v>1342</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>1347</v>
+        <v>1343</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>1348</v>
+        <v>1344</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="2" t="n">
         <v>2000</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>1290</v>
+        <v>1286</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>1349</v>
+        <v>1345</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2" t="s">
-        <v>1350</v>
+        <v>1346</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>1351</v>
+        <v>1347</v>
       </c>
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2" t="s">
-        <v>1352</v>
+        <v>1348</v>
       </c>
       <c r="R11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>1353</v>
+        <v>1349</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>1354</v>
+        <v>1350</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>1355</v>
+        <v>1351</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>1356</v>
+        <v>1352</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="n">
         <v>1999</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>1290</v>
+        <v>1286</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>1357</v>
+        <v>1353</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2" t="s">
-        <v>1292</v>
+        <v>1288</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>1319</v>
+        <v>1315</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2" t="s">
-        <v>1358</v>
+        <v>1354</v>
       </c>
       <c r="R12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>1359</v>
+        <v>1355</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>1360</v>
+        <v>1356</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>1361</v>
+        <v>1357</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>1362</v>
+        <v>1358</v>
       </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2" t="n">
         <v>1979</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>1290</v>
+        <v>1286</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>1349</v>
+        <v>1345</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2" t="s">
-        <v>1363</v>
+        <v>1359</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>1364</v>
+        <v>1360</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2" t="s">
-        <v>1365</v>
+        <v>1361</v>
       </c>
       <c r="R13" s="2"/>
     </row>
@@ -6194,40 +6169,40 @@
         <v>46</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>1366</v>
+        <v>1362</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>1367</v>
+        <v>1363</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>1368</v>
+        <v>1364</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2" t="n">
         <v>2012</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>1290</v>
+        <v>1286</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>1369</v>
+        <v>1365</v>
       </c>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2" t="s">
-        <v>1370</v>
+        <v>1366</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>1312</v>
+        <v>1308</v>
       </c>
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2" t="s">
-        <v>1371</v>
+        <v>1367</v>
       </c>
       <c r="R14" s="2"/>
     </row>
@@ -6236,59 +6211,59 @@
         <v>159</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>1372</v>
+        <v>1368</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>1373</v>
+        <v>1369</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>1374</v>
+        <v>1370</v>
       </c>
       <c r="F15" s="2"/>
       <c r="G15" s="2" t="n">
         <v>2009</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>1290</v>
+        <v>1286</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>1375</v>
+        <v>1371</v>
       </c>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2" t="s">
-        <v>1376</v>
+        <v>1372</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>1377</v>
+        <v>1373</v>
       </c>
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2" t="s">
-        <v>1378</v>
+        <v>1374</v>
       </c>
       <c r="R15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>1379</v>
+        <v>1375</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>1380</v>
+        <v>1376</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2" t="s">
-        <v>1381</v>
+        <v>1377</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -6303,20 +6278,20 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>1382</v>
+        <v>1378</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>1383</v>
+        <v>1379</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2" t="s">
-        <v>1381</v>
+        <v>1377</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -6331,20 +6306,20 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>1384</v>
+        <v>1380</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>1385</v>
+        <v>1381</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2" t="s">
-        <v>1381</v>
+        <v>1377</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -6359,20 +6334,20 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>1386</v>
+        <v>1382</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>1387</v>
+        <v>1383</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2" t="s">
-        <v>1381</v>
+        <v>1377</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -6394,13 +6369,13 @@
         <v>1</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>1388</v>
+        <v>1384</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2" t="s">
-        <v>1381</v>
+        <v>1377</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -6444,19 +6419,19 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>1389</v>
+        <v>1385</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1390</v>
+        <v>1386</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1391</v>
+        <v>1387</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>1392</v>
+        <v>1388</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>526</v>
@@ -6471,15 +6446,15 @@
         <v>1055</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>1393</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>1394</v>
+        <v>1390</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1395</v>
+        <v>1391</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -6489,15 +6464,15 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
-        <v>1338</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>1394</v>
+        <v>1390</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1396</v>
+        <v>1392</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -6507,15 +6482,15 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2" t="s">
-        <v>1353</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>1394</v>
+        <v>1390</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1397</v>
+        <v>1393</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -6530,10 +6505,10 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>1390</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>1394</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>1398</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -6543,15 +6518,15 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2" t="s">
-        <v>1331</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>1394</v>
+        <v>1390</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1399</v>
+        <v>1395</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -6566,10 +6541,10 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>1394</v>
+        <v>1390</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1400</v>
+        <v>1396</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -6579,15 +6554,15 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2" t="s">
-        <v>1314</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>1394</v>
+        <v>1390</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>1401</v>
+        <v>1397</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -6597,15 +6572,15 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="2" t="s">
-        <v>1345</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>1394</v>
+        <v>1390</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1402</v>
+        <v>1398</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -6615,15 +6590,15 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2" t="s">
-        <v>1299</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>1394</v>
+        <v>1390</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1403</v>
+        <v>1399</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -6638,10 +6613,10 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>1394</v>
+        <v>1390</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>1404</v>
+        <v>1400</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -6656,10 +6631,10 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>1394</v>
+        <v>1390</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>1405</v>
+        <v>1401</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -6674,10 +6649,10 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>1394</v>
+        <v>1390</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>1406</v>
+        <v>1402</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -6687,15 +6662,15 @@
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2" t="s">
-        <v>1306</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>1407</v>
+        <v>1403</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>1408</v>
+        <v>1404</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -6710,10 +6685,10 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>1409</v>
+        <v>1405</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>1410</v>
+        <v>1406</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -6723,18 +6698,18 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2" t="s">
-        <v>1359</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>1391</v>
+        <v>1387</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1411</v>
+        <v>1407</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>1411</v>
+        <v>1407</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -6743,18 +6718,18 @@
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16" s="2" t="s">
-        <v>1384</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>1391</v>
+        <v>1387</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>1412</v>
+        <v>1408</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>1412</v>
+        <v>1408</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -6768,13 +6743,13 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>1391</v>
+        <v>1387</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>1413</v>
+        <v>1409</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>1413</v>
+        <v>1409</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -6783,18 +6758,18 @@
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
       <c r="J18" s="2" t="s">
-        <v>1379</v>
+        <v>1375</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>1391</v>
+        <v>1387</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>1414</v>
+        <v>1410</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>1414</v>
+        <v>1410</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -6803,18 +6778,18 @@
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2" t="s">
-        <v>1382</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>1391</v>
+        <v>1387</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>1415</v>
+        <v>1411</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>1415</v>
+        <v>1411</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -6823,7 +6798,7 @@
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20" s="2" t="s">
-        <v>1386</v>
+        <v>1382</v>
       </c>
     </row>
   </sheetData>
@@ -6930,8 +6905,8 @@
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.6032388663968"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.1376518218624"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.2793522267206"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.4939271255061"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -7081,7 +7056,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.4251012145749"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5303643724696"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -12032,7 +12007,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -12135,10 +12110,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.3522267206478"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.4574898785425"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.6356275303644"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.0647773279352"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="34.3846153846154"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>
@@ -15857,7 +15832,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="22.7085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.6032388663968"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
renaming BiomassReaction --> DfbaNetReaction, BiomassComponent --> DfbaNetComponent, adding constraint on ids of DfbaNetComponent
</commit_message>
<xml_diff>
--- a/tests/fixtures/example-model.xlsx
+++ b/tests/fixtures/example-model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="11"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,8 +20,8 @@
     <sheet name="dFBA objectives" sheetId="10" state="visible" r:id="rId11"/>
     <sheet name="Reactions" sheetId="11" state="visible" r:id="rId12"/>
     <sheet name="Rate laws" sheetId="12" state="visible" r:id="rId13"/>
-    <sheet name="Biomass reactions" sheetId="13" state="visible" r:id="rId14"/>
-    <sheet name="Biomass components" sheetId="14" state="visible" r:id="rId15"/>
+    <sheet name="dFBA net reactions" sheetId="13" state="visible" r:id="rId14"/>
+    <sheet name="dFBA net components" sheetId="14" state="visible" r:id="rId15"/>
     <sheet name="Parameters" sheetId="15" state="visible" r:id="rId16"/>
     <sheet name="Stop conditions" sheetId="16" state="visible" r:id="rId17"/>
     <sheet name="References" sheetId="17" state="visible" r:id="rId18"/>
@@ -31,8 +31,8 @@
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
     <definedName function="false" hidden="true" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">Concentrations!$C$1:$G$126</definedName>
     <definedName function="false" hidden="true" localSheetId="17" name="_xlnm._FilterDatabase" vbProcedure="false">'Database references'!$A$1:$J$20</definedName>
-    <definedName function="false" hidden="true" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$G$37</definedName>
-    <definedName function="false" hidden="true" localSheetId="11" name="_xlnm._FilterDatabase" vbProcedure="false">'Rate laws'!$A$1:$I$168</definedName>
+    <definedName function="false" hidden="true" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$G$6</definedName>
+    <definedName function="false" hidden="true" localSheetId="11" name="_xlnm._FilterDatabase" vbProcedure="false">'Rate laws'!$C$1:$I$168</definedName>
     <definedName function="false" hidden="true" localSheetId="10" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$I$176</definedName>
     <definedName function="false" hidden="true" localSheetId="16" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$Q$20</definedName>
     <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$I$144</definedName>
@@ -107,6 +107,9 @@
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Submodels!$A$1:$E$5</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Submodels!$A$1:$E$5</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Submodels!$A$1:$E$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Submodels!$A$1:$E$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Submodels!$A$1:$E$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Submodels!$A$1:$E$5</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
@@ -137,6 +140,9 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$F$3</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$I$144</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$I$144</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$144</definedName>
@@ -167,6 +173,9 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$144</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$144</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$144</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$144</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$144</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$I$144</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_FilterDatabase_0" vbProcedure="false">Concentrations!$C$1:$G$126</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_FilterDatabase_0_0" vbProcedure="false">Concentrations!$C$1:$G$126</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_FilterDatabase_0_0_0" vbProcedure="false">Concentrations!$C$1:$G$126</definedName>
@@ -197,6 +206,9 @@
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Concentrations!$C$1:$G$126</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Concentrations!$C$1:$G$126</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Concentrations!$C$1:$G$126</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Concentrations!$C$1:$G$126</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Concentrations!$C$1:$G$126</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Concentrations!$C$1:$G$126</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$I$176</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$I$176</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0_0" vbProcedure="false">Reactions!$A$1:$I$176</definedName>
@@ -227,6 +239,9 @@
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$I$176</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$I$176</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$I$176</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$I$176</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$I$176</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$I$176</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_FilterDatabase_0" vbProcedure="false">'Rate laws'!$C$1:$I$168</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_FilterDatabase_0_0" vbProcedure="false">'Rate laws'!$C$1:$I$168</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_FilterDatabase_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$I$168</definedName>
@@ -235,11 +250,11 @@
     <definedName function="false" hidden="false" localSheetId="11" name="_FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$I$168</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$I$168</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$I$168</definedName>
-    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase" vbProcedure="false">'Rate laws'!$C$1:$I$168</definedName>
-    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Rate laws'!$A$1:$I$168</definedName>
-    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Rate laws'!$C$1:$I$168</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase" vbProcedure="false">'Rate laws'!$A$1:$I$168</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Rate laws'!$C$1:$I$168</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Rate laws'!$A$1:$I$168</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$I$168</definedName>
-    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$I$168</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Rate laws'!$A$1:$I$168</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$I$168</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$I$168</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$I$168</definedName>
@@ -257,6 +272,9 @@
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$I$168</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$I$168</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$I$168</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$I$168</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$I$168</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$I$168</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$G$6</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$G$6</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$G$6</definedName>
@@ -265,11 +283,11 @@
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$G$6</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$G$6</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$G$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$G$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$G$37</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$G$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$G$37</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$G$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$G$37</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$G$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Parameters!$A$1:$G$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Parameters!$A$1:$G$37</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$G$6</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$G$6</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$G$6</definedName>
@@ -287,6 +305,9 @@
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$G$6</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$G$6</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$G$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$G$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$G$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$G$6</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_FilterDatabase_0" vbProcedure="false">References!$A$1:$Q$20</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_FilterDatabase_0_0" vbProcedure="false">References!$A$1:$Q$20</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_FilterDatabase_0_0_0" vbProcedure="false">References!$A$1:$Q$20</definedName>
@@ -317,6 +338,9 @@
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$Q$20</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$Q$20</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$Q$20</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$Q$20</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$Q$20</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$Q$20</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_FilterDatabase_0" vbProcedure="false">'Database references'!$A$1:$J$20</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_FilterDatabase_0_0" vbProcedure="false">'Database references'!$A$1:$J$20</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_FilterDatabase_0_0_0" vbProcedure="false">'Database references'!$A$1:$J$20</definedName>
@@ -347,6 +371,9 @@
     <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Database references'!$A$1:$J$20</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Database references'!$A$1:$J$20</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Database references'!$A$1:$J$20</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Database references'!$A$1:$J$20</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Database references'!$A$1:$J$20</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Database references'!$A$1:$J$20</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -358,7 +385,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3886" uniqueCount="1806">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3886" uniqueCount="1805">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -2517,7 +2544,7 @@
     <t xml:space="preserve">dfba-obj-Metabolism</t>
   </si>
   <si>
-    <t xml:space="preserve">Metabolism_biomass + AdnTransport</t>
+    <t xml:space="preserve">Metabolism_net_rxn + AdnTransport</t>
   </si>
   <si>
     <t xml:space="preserve">Participants</t>
@@ -4887,34 +4914,34 @@
     <t xml:space="preserve">ValAbcTransport-forward</t>
   </si>
   <si>
-    <t xml:space="preserve">Metabolism_biomass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Metabolism biomass reaction</t>
+    <t xml:space="preserve">Metabolism_net_rxn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metabolism net reaction</t>
   </si>
   <si>
     <t xml:space="preserve">No comment</t>
   </si>
   <si>
-    <t xml:space="preserve">Other_biomass</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other biomass</t>
+    <t xml:space="preserve">Other_net_rxn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other net reaction</t>
   </si>
   <si>
     <t xml:space="preserve">NA</t>
   </si>
   <si>
-    <t xml:space="preserve">Biomass reaction</t>
+    <t xml:space="preserve">dFBA net reaction</t>
   </si>
   <si>
     <t xml:space="preserve">Coefficient</t>
   </si>
   <si>
-    <t xml:space="preserve">biomass_id_001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ALA_biomass_comp</t>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-ALA[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALA net component</t>
   </si>
   <si>
     <t xml:space="preserve">test</t>
@@ -4923,202 +4950,202 @@
     <t xml:space="preserve">Ref_0004, Ref_0005</t>
   </si>
   <si>
-    <t xml:space="preserve">biomass_id_002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARG_biomass_comp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_id_003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASN_biomass_comp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_id_004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ASP_biomass_comp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_id_005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ATP_biomass_comp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_id_006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CTP_biomass_comp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_id_007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CYS_biomass_comp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_id_008</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GLN_biomass_comp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_id_009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GLU_biomass_comp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_id_010</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GLY_biomass_comp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_id_011</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GTP_biomass_comp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_id_012</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H2O_biomass_comp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_id_013</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HIS_biomass_comp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_id_014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ILE_biomass_comp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_id_015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LEU_biomass_comp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_id_016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LYS_biomass_comp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_id_017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MET_biomass_comp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_id_018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHE_biomass_comp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_id_019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRO_biomass_comp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_id_020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SER_biomass_comp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_id_021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">THR_biomass_comp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_id_022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TRP_biomass_comp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_id_023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TYR_biomass_comp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_id_024</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UTP_biomass_comp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_id_025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VAL_biomass_comp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_id_026</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AMP_biomass_comp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_id_027</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CMP_biomass_comp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_id_028</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GDP_biomass_comp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_id_029</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GMP_biomass_comp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_id_030</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H_biomass_comp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_id_031</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pi_biomass_comp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_id_032</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PPi_biomass_comp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_id_033</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UMP_biomass_comp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_id_034</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biomass_id_035</t>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-AMP[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMP net component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-ARG[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARG net component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-ASN[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASN net component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-ASP[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ASP net component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-ATP[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATP net component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-CMP[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CMP net component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-CTP[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CTP net component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-CYS[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CYS net component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-GDP[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GDP net component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-GLN[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GLN net component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-GLU[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GLU net component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-GLY[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GLY net component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-GMP[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GMP net component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-GTP[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GTP net component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-H2O[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H2O net component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-H[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H net component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-HIS[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HIS net component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-ILE[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ILE net component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-LEU[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LEU net component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-LYS[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LYS net component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-MET[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MET net component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-PHE[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PHE net component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-Pi[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pi net component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-PPi[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PPi net component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-PRO[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRO net component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-SER[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SER net component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-THR[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">THR net component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-TRP[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRP net component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-TYR[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TYR net component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-UMP[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UMP net component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-UTP[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UTP net component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-VAL[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VAL net component</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Other_net_rxn-PPi[c]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dfba-net-comp-Other_net_rxn-UMP[c]</t>
   </si>
   <si>
     <t xml:space="preserve">carbonExchangeRate</t>
@@ -5698,9 +5725,6 @@
   </si>
   <si>
     <t xml:space="preserve">Database</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ID</t>
   </si>
   <si>
     <t xml:space="preserve">Model</t>
@@ -6077,7 +6101,7 @@
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="44.1336032388664"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="45.0971659919028"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -6194,14 +6218,14 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="20.3522267206478"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="3" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="40.919028340081"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="41.8825910931174"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="3" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -6255,19 +6279,19 @@
   <dimension ref="A1:I176"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topRight" activeCell="O1" activeCellId="0" sqref="O1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
       <selection pane="bottomRight" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="30.2064777327935"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="30.8502024291498"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="56.3441295546559"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="57.8461538461538"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -9985,11 +10009,11 @@
   </sheetPr>
   <dimension ref="A1:I168"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B140" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A140" activeCellId="0" sqref="A140"/>
       <selection pane="bottomRight" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -13702,7 +13726,7 @@
       <c r="I168" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I168"/>
+  <autoFilter ref="C1:I168"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -13722,17 +13746,17 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="M1" activeCellId="0" sqref="M1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="9" width="17.995951417004"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="9" width="18.3157894736842"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="23.5668016194332"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="9" width="11.246963562753"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="9" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1020" min="6" style="9" width="8.78542510121457"/>
@@ -13807,20 +13831,20 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D35" activeCellId="0" sqref="D35"/>
+      <selection pane="bottomRight" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="11" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="11" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="11" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="18.8542510121457"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="11" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="11" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="11" width="8.78542510121457"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="11" width="16.497975708502"/>
     <col collapsed="false" hidden="false" max="1019" min="8" style="3" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="1020" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="1020" style="1" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13853,7 +13877,7 @@
       <c r="B2" s="11" t="s">
         <v>1518</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>1509</v>
       </c>
       <c r="D2" s="13" t="n">
@@ -13876,14 +13900,14 @@
       <c r="B3" s="11" t="s">
         <v>1522</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>1509</v>
       </c>
       <c r="D3" s="13" t="n">
-        <v>-40890.38</v>
+        <v>1035619</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13893,14 +13917,14 @@
       <c r="B4" s="11" t="s">
         <v>1524</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>1509</v>
       </c>
       <c r="D4" s="13" t="n">
-        <v>-23190.38</v>
+        <v>-40890.38</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13910,14 +13934,14 @@
       <c r="B5" s="11" t="s">
         <v>1526</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>1509</v>
       </c>
       <c r="D5" s="13" t="n">
-        <v>-24290.38</v>
+        <v>-23190.38</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13927,14 +13951,14 @@
       <c r="B6" s="11" t="s">
         <v>1528</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>1509</v>
       </c>
       <c r="D6" s="13" t="n">
-        <v>-1101856</v>
+        <v>-24290.38</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13944,14 +13968,14 @@
       <c r="B7" s="11" t="s">
         <v>1530</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>1509</v>
       </c>
       <c r="D7" s="13" t="n">
-        <v>-1164906</v>
+        <v>-1101856</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13961,14 +13985,14 @@
       <c r="B8" s="11" t="s">
         <v>1532</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="10" t="s">
         <v>1509</v>
       </c>
       <c r="D8" s="13" t="n">
-        <v>-22290.38</v>
+        <v>1098019</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13978,14 +14002,14 @@
       <c r="B9" s="11" t="s">
         <v>1534</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="10" t="s">
         <v>1509</v>
       </c>
       <c r="D9" s="13" t="n">
-        <v>-24690.38</v>
+        <v>-1164906</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>448</v>
+        <v>425</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13995,14 +14019,14 @@
       <c r="B10" s="11" t="s">
         <v>1536</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>1509</v>
       </c>
       <c r="D10" s="13" t="n">
-        <v>-22690.38</v>
+        <v>-22290.38</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>451</v>
+        <v>426</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14012,14 +14036,14 @@
       <c r="B11" s="11" t="s">
         <v>1538</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="10" t="s">
         <v>1509</v>
       </c>
       <c r="D11" s="13" t="n">
-        <v>-31190.38</v>
+        <v>581419.2</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>454</v>
+        <v>444</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14029,14 +14053,14 @@
       <c r="B12" s="11" t="s">
         <v>1540</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="10" t="s">
         <v>1509</v>
       </c>
       <c r="D12" s="13" t="n">
-        <v>-1728316</v>
+        <v>-24690.38</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>460</v>
+        <v>448</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14046,14 +14070,14 @@
       <c r="B13" s="11" t="s">
         <v>1542</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>1509</v>
       </c>
       <c r="D13" s="13" t="n">
-        <v>-1521617000</v>
+        <v>-22690.38</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>461</v>
+        <v>451</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14063,14 +14087,14 @@
       <c r="B14" s="11" t="s">
         <v>1544</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="10" t="s">
         <v>1509</v>
       </c>
       <c r="D14" s="13" t="n">
-        <v>-21590.38</v>
+        <v>-31190.38</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>465</v>
+        <v>454</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14080,14 +14104,14 @@
       <c r="B15" s="11" t="s">
         <v>1546</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="10" t="s">
         <v>1509</v>
       </c>
       <c r="D15" s="13" t="n">
-        <v>-29290.38</v>
+        <v>1052899</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>470</v>
+        <v>457</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14097,14 +14121,14 @@
       <c r="B16" s="11" t="s">
         <v>1548</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="10" t="s">
         <v>1509</v>
       </c>
       <c r="D16" s="13" t="n">
-        <v>-41190.38</v>
+        <v>-1728316</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>479</v>
+        <v>460</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14114,14 +14138,14 @@
       <c r="B17" s="11" t="s">
         <v>1550</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="10" t="s">
         <v>1509</v>
       </c>
       <c r="D17" s="13" t="n">
-        <v>-21990.38</v>
+        <v>-1521617000</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>482</v>
+        <v>461</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14131,14 +14155,14 @@
       <c r="B18" s="11" t="s">
         <v>1552</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="10" t="s">
         <v>1509</v>
       </c>
       <c r="D18" s="13" t="n">
-        <v>-21390.38</v>
+        <v>4972350</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>485</v>
+        <v>463</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14148,14 +14172,14 @@
       <c r="B19" s="11" t="s">
         <v>1554</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="10" t="s">
         <v>1509</v>
       </c>
       <c r="D19" s="13" t="n">
-        <v>-23890.38</v>
+        <v>-21590.38</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>506</v>
+        <v>465</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14165,14 +14189,14 @@
       <c r="B20" s="11" t="s">
         <v>1556</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="10" t="s">
         <v>1509</v>
       </c>
       <c r="D20" s="13" t="n">
-        <v>-34390.38</v>
+        <v>-29290.38</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>516</v>
+        <v>470</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14182,14 +14206,14 @@
       <c r="B21" s="11" t="s">
         <v>1558</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="10" t="s">
         <v>1509</v>
       </c>
       <c r="D21" s="13" t="n">
-        <v>-44490.38</v>
+        <v>-41190.38</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>540</v>
+        <v>479</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14199,14 +14223,14 @@
       <c r="B22" s="11" t="s">
         <v>1560</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="10" t="s">
         <v>1509</v>
       </c>
       <c r="D22" s="13" t="n">
-        <v>-36190.38</v>
+        <v>-21990.38</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>545</v>
+        <v>482</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14216,14 +14240,14 @@
       <c r="B23" s="11" t="s">
         <v>1562</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="10" t="s">
         <v>1509</v>
       </c>
       <c r="D23" s="13" t="n">
-        <v>-22190.38</v>
+        <v>-21390.38</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>552</v>
+        <v>485</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14233,14 +14257,14 @@
       <c r="B24" s="11" t="s">
         <v>1564</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="10" t="s">
         <v>1509</v>
       </c>
       <c r="D24" s="13" t="n">
-        <v>-21990.38</v>
+        <v>-23890.38</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>555</v>
+        <v>506</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14250,14 +14274,14 @@
       <c r="B25" s="11" t="s">
         <v>1566</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="10" t="s">
         <v>1509</v>
       </c>
       <c r="D25" s="13" t="n">
-        <v>-1132896</v>
+        <v>471096.2</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>567</v>
+        <v>509</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14267,14 +14291,14 @@
       <c r="B26" s="11" t="s">
         <v>1568</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="10" t="s">
         <v>1509</v>
       </c>
       <c r="D26" s="13" t="n">
-        <v>-33790.38</v>
+        <v>4381069</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>569</v>
+        <v>515</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14284,14 +14308,14 @@
       <c r="B27" s="11" t="s">
         <v>1570</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="10" t="s">
         <v>1509</v>
       </c>
       <c r="D27" s="13" t="n">
-        <v>1035619</v>
+        <v>-34390.38</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>406</v>
+        <v>516</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14301,14 +14325,14 @@
       <c r="B28" s="11" t="s">
         <v>1572</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="10" t="s">
         <v>1509</v>
       </c>
       <c r="D28" s="13" t="n">
-        <v>1098019</v>
+        <v>-44490.38</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>422</v>
+        <v>540</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14318,14 +14342,14 @@
       <c r="B29" s="11" t="s">
         <v>1574</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="10" t="s">
         <v>1509</v>
       </c>
       <c r="D29" s="13" t="n">
-        <v>581419.2</v>
+        <v>-36190.38</v>
       </c>
       <c r="E29" s="11" t="s">
-        <v>444</v>
+        <v>545</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14335,14 +14359,14 @@
       <c r="B30" s="11" t="s">
         <v>1576</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="10" t="s">
         <v>1509</v>
       </c>
       <c r="D30" s="13" t="n">
-        <v>1052899</v>
+        <v>-22190.38</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>457</v>
+        <v>552</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14352,14 +14376,14 @@
       <c r="B31" s="11" t="s">
         <v>1578</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="10" t="s">
         <v>1509</v>
       </c>
       <c r="D31" s="13" t="n">
-        <v>4972350</v>
+        <v>-21990.38</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>463</v>
+        <v>555</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14369,14 +14393,14 @@
       <c r="B32" s="11" t="s">
         <v>1580</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="10" t="s">
         <v>1509</v>
       </c>
       <c r="D32" s="13" t="n">
-        <v>471096.2</v>
+        <v>1066339</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>509</v>
+        <v>561</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14386,14 +14410,14 @@
       <c r="B33" s="11" t="s">
         <v>1582</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="10" t="s">
         <v>1509</v>
       </c>
       <c r="D33" s="13" t="n">
-        <v>4381069</v>
+        <v>-1132896</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>515</v>
+        <v>567</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14403,22 +14427,22 @@
       <c r="B34" s="11" t="s">
         <v>1584</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" s="10" t="s">
         <v>1509</v>
       </c>
       <c r="D34" s="13" t="n">
-        <v>1066339</v>
+        <v>-33790.38</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="11" t="s">
         <v>1585</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>1582</v>
+        <v>1568</v>
       </c>
       <c r="C35" s="10" t="s">
         <v>1512</v>
@@ -14430,12 +14454,12 @@
         <v>515</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="11" t="s">
         <v>1586</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>1584</v>
+        <v>1580</v>
       </c>
       <c r="C36" s="10" t="s">
         <v>1512</v>
@@ -15177,7 +15201,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G37"/>
+  <autoFilter ref="A1:G6"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -16003,12 +16027,12 @@
   </sheetPr>
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -16021,16 +16045,16 @@
         <v>1779</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1780</v>
+        <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>1780</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>1781</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>1782</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>717</v>
@@ -16045,15 +16069,15 @@
         <v>1249</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>1783</v>
+        <v>1782</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>1783</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>1784</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>1785</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -16068,10 +16092,10 @@
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1786</v>
+        <v>1785</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -16086,10 +16110,10 @@
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -16104,10 +16128,10 @@
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1788</v>
+        <v>1787</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -16122,10 +16146,10 @@
     </row>
     <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1789</v>
+        <v>1788</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -16140,10 +16164,10 @@
     </row>
     <row r="7" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1790</v>
+        <v>1789</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -16158,10 +16182,10 @@
     </row>
     <row r="8" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1791</v>
+        <v>1790</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -16176,10 +16200,10 @@
     </row>
     <row r="9" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -16194,10 +16218,10 @@
     </row>
     <row r="10" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1793</v>
+        <v>1792</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -16212,10 +16236,10 @@
     </row>
     <row r="11" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -16230,10 +16254,10 @@
     </row>
     <row r="12" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>1795</v>
+        <v>1794</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -16248,10 +16272,10 @@
     </row>
     <row r="13" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>1796</v>
+        <v>1795</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -16266,10 +16290,10 @@
     </row>
     <row r="14" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
+        <v>1796</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>1797</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>1798</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -16284,10 +16308,10 @@
     </row>
     <row r="15" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
+        <v>1798</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>1799</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>1800</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -16305,10 +16329,10 @@
         <v>6</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
@@ -16325,10 +16349,10 @@
         <v>6</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -16345,10 +16369,10 @@
         <v>6</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>1803</v>
+        <v>1802</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>1803</v>
+        <v>1802</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -16365,10 +16389,10 @@
         <v>6</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>1804</v>
+        <v>1803</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>1804</v>
+        <v>1803</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -16385,10 +16409,10 @@
         <v>6</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
@@ -16429,7 +16453,7 @@
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="25.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.3522267206478"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -16607,7 +16631,7 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.6396761133603"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.9595141700405"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="1" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.7813765182186"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.3562753036437"/>
@@ -16704,7 +16728,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.4574898785425"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -19724,7 +19748,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.7085020242915"/>
     <col collapsed="false" hidden="false" max="6" min="2" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="9.10526315789474"/>
   </cols>
@@ -21877,9 +21901,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.6356275303644"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="27.6356275303644"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -24057,7 +24081,7 @@
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="1" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="33.2064777327935"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="34.17004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -24147,7 +24171,7 @@
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="1" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.5303643724696"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="8.78542510121457"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
adding element/charge balance validation and option to toggle it off
</commit_message>
<xml_diff>
--- a/tests/fixtures/example-model.xlsx
+++ b/tests/fixtures/example-model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="16"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -29,8 +29,8 @@
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
     <definedName function="false" hidden="true" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">Concentrations!$C$1:$H$126</definedName>
-    <definedName function="false" hidden="true" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$H$37</definedName>
-    <definedName function="false" hidden="true" localSheetId="11" name="_xlnm._FilterDatabase" vbProcedure="false">'Rate laws'!$A$1:$J$168</definedName>
+    <definedName function="false" hidden="true" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$H$6</definedName>
+    <definedName function="false" hidden="true" localSheetId="11" name="_xlnm._FilterDatabase" vbProcedure="false">'Rate laws'!$C$1:$J$168</definedName>
     <definedName function="false" hidden="true" localSheetId="10" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$J$176</definedName>
     <definedName function="false" hidden="true" localSheetId="16" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$R$20</definedName>
     <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$J$144</definedName>
@@ -109,6 +109,7 @@
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Submodels!$A$1:$F$5</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Submodels!$A$1:$F$5</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Submodels!$A$1:$F$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Submodels!$A$1:$F$5</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
@@ -143,6 +144,7 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$G$3</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$J$144</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$J$144</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$144</definedName>
@@ -177,6 +179,7 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$144</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$144</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$144</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$J$144</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_FilterDatabase_0" vbProcedure="false">Concentrations!$C$1:$H$126</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_FilterDatabase_0_0" vbProcedure="false">Concentrations!$C$1:$H$126</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_FilterDatabase_0_0_0" vbProcedure="false">Concentrations!$C$1:$H$126</definedName>
@@ -211,6 +214,7 @@
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Concentrations!$C$1:$H$126</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Concentrations!$C$1:$H$126</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Concentrations!$C$1:$H$126</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Concentrations!$C$1:$H$126</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$J$176</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$J$176</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0_0" vbProcedure="false">Reactions!$A$1:$J$176</definedName>
@@ -245,6 +249,7 @@
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$J$176</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$J$176</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$J$176</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$J$176</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_FilterDatabase_0" vbProcedure="false">'Rate laws'!$C$1:$J$168</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_FilterDatabase_0_0" vbProcedure="false">'Rate laws'!$C$1:$J$168</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_FilterDatabase_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$J$168</definedName>
@@ -253,13 +258,13 @@
     <definedName function="false" hidden="false" localSheetId="11" name="_FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$J$168</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$J$168</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$J$168</definedName>
-    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase" vbProcedure="false">'Rate laws'!$C$1:$J$168</definedName>
-    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Rate laws'!$A$1:$J$168</definedName>
-    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Rate laws'!$C$1:$J$168</definedName>
-    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Rate laws'!$A$1:$J$168</definedName>
-    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$J$168</definedName>
-    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Rate laws'!$A$1:$J$168</definedName>
-    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$J$168</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase" vbProcedure="false">'Rate laws'!$A$1:$J$168</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Rate laws'!$C$1:$J$168</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Rate laws'!$A$1:$J$168</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$J$168</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Rate laws'!$A$1:$J$168</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$J$168</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$A$1:$J$168</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$J$168</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$J$168</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$J$168</definedName>
@@ -279,6 +284,7 @@
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$J$168</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$J$168</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$J$168</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$J$168</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$H$6</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$H$6</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$H$6</definedName>
@@ -287,13 +293,13 @@
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$H$6</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$H$6</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$H$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$H$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$H$37</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$H$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$H$37</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Parameters!$A$1:$H$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$H$37</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$H$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$H$37</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$H$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$H$37</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$H$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Parameters!$A$1:$H$37</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$H$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$H$37</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$H$6</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$H$6</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$H$6</definedName>
@@ -313,6 +319,7 @@
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$H$6</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$H$6</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$H$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$H$6</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_FilterDatabase_0" vbProcedure="false">References!$A$1:$R$20</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_FilterDatabase_0_0" vbProcedure="false">References!$A$1:$R$20</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_FilterDatabase_0_0_0" vbProcedure="false">References!$A$1:$R$20</definedName>
@@ -347,6 +354,7 @@
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$R$20</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$R$20</definedName>
     <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$R$20</definedName>
+    <definedName function="false" hidden="false" localSheetId="16" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$R$20</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -6046,13 +6054,13 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="A11" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topRight" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="45.5263157894737"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="45.9554655870445"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -6174,14 +6182,14 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="bottomRight" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="20.5668016194332"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="3" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="42.2064777327935"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="42.5263157894737"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="3" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -6242,15 +6250,15 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="bottomRight" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.17004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.4939271255061"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="58.3805668016194"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="58.8097165991903"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -10143,7 +10151,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A140" activeCellId="0" sqref="A140"/>
-      <selection pane="bottomRight" activeCell="H1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="bottomRight" activeCell="H1" activeCellId="0" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -14025,7 +14033,7 @@
       <c r="J168" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J168"/>
+  <autoFilter ref="C1:J168"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -14049,13 +14057,13 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="bottomRight" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="9" width="18.4251012145749"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="9" width="18.5303643724696"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="9" width="23.8866396761134"/>
     <col collapsed="false" hidden="false" max="5" min="3" style="9" width="11.246963562753"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="9" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1021" min="7" style="9" width="8.78542510121457"/>
@@ -14133,14 +14141,14 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="bottomRight" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="11" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="11" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="11" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="11" width="19.1740890688259"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="11" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="11" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="11" width="8.78542510121457"/>
@@ -14799,7 +14807,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
-      <selection pane="bottomRight" activeCell="F1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="bottomRight" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -14849,6 +14857,7 @@
       <c r="E2" s="3" t="s">
         <v>1590</v>
       </c>
+      <c r="F2" s="0"/>
       <c r="G2" s="3" t="s">
         <v>1591</v>
       </c>
@@ -14872,6 +14881,7 @@
       <c r="E3" s="3" t="s">
         <v>1594</v>
       </c>
+      <c r="F3" s="0"/>
       <c r="G3" s="0"/>
       <c r="H3" s="0"/>
     </row>
@@ -14891,6 +14901,7 @@
       <c r="E4" s="3" t="s">
         <v>1597</v>
       </c>
+      <c r="F4" s="0"/>
       <c r="G4" s="0"/>
       <c r="H4" s="3" t="s">
         <v>1598</v>
@@ -15539,7 +15550,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H37"/>
+  <autoFilter ref="A1:H6"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -15563,7 +15574,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D2" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="bottomRight" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -15629,12 +15640,12 @@
   </sheetPr>
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M23" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="bottomRight" activeCell="M23" activeCellId="0" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -16433,13 +16444,13 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="A4" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="topRight" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="26.7813765182186"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -16508,7 +16519,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D2" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="bottomRight" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -16624,13 +16635,13 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E2" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="bottomRight" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.1740890688259"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="1" width="14.1417004048583"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="1" width="11.7813765182186"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.3562753036437"/>
@@ -16722,17 +16733,17 @@
   </sheetPr>
   <dimension ref="A1:J144"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H2" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="bottomRight" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.6720647773279"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -16780,7 +16791,9 @@
       <c r="E2" s="3" t="n">
         <v>135.126</v>
       </c>
-      <c r="F2" s="3"/>
+      <c r="F2" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G2" s="3" t="s">
         <v>51</v>
       </c>
@@ -16806,7 +16819,9 @@
       <c r="E3" s="3" t="n">
         <v>11217.6918</v>
       </c>
-      <c r="F3" s="3"/>
+      <c r="F3" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G3" s="3" t="s">
         <v>57</v>
       </c>
@@ -16828,7 +16843,9 @@
       <c r="E4" s="3" t="n">
         <v>97629.5094</v>
       </c>
-      <c r="F4" s="3"/>
+      <c r="F4" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G4" s="3" t="s">
         <v>61</v>
       </c>
@@ -16848,7 +16865,9 @@
       <c r="E5" s="3" t="n">
         <v>424.177</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="F5" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G5" s="3" t="s">
         <v>51</v>
       </c>
@@ -16868,7 +16887,9 @@
       <c r="E6" s="3" t="n">
         <v>89.0929</v>
       </c>
-      <c r="F6" s="3"/>
+      <c r="F6" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G6" s="3" t="s">
         <v>51</v>
       </c>
@@ -16888,7 +16909,9 @@
       <c r="E7" s="3" t="n">
         <v>160.171</v>
       </c>
-      <c r="F7" s="3"/>
+      <c r="F7" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G7" s="3" t="s">
         <v>51</v>
       </c>
@@ -16912,7 +16935,9 @@
       <c r="E8" s="3" t="n">
         <v>345.205</v>
       </c>
-      <c r="F8" s="3"/>
+      <c r="F8" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G8" s="3" t="s">
         <v>51</v>
       </c>
@@ -16934,7 +16959,9 @@
       <c r="E9" s="3" t="n">
         <v>11598.2932</v>
       </c>
-      <c r="F9" s="3"/>
+      <c r="F9" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G9" s="3" t="s">
         <v>57</v>
       </c>
@@ -16956,7 +16983,9 @@
       <c r="E10" s="3" t="n">
         <v>96600.2544</v>
       </c>
-      <c r="F10" s="3"/>
+      <c r="F10" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G10" s="3" t="s">
         <v>61</v>
       </c>
@@ -16976,7 +17005,9 @@
       <c r="E11" s="3" t="n">
         <v>175.208</v>
       </c>
-      <c r="F11" s="3"/>
+      <c r="F11" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G11" s="3" t="s">
         <v>51</v>
       </c>
@@ -16996,7 +17027,9 @@
       <c r="E12" s="3" t="n">
         <v>332.401</v>
       </c>
-      <c r="F12" s="3"/>
+      <c r="F12" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G12" s="3" t="s">
         <v>51</v>
       </c>
@@ -17020,7 +17053,9 @@
       <c r="E13" s="3" t="n">
         <v>132.118</v>
       </c>
-      <c r="F13" s="3"/>
+      <c r="F13" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G13" s="3" t="s">
         <v>51</v>
       </c>
@@ -17040,7 +17075,9 @@
       <c r="E14" s="3" t="n">
         <v>246.22</v>
       </c>
-      <c r="F14" s="3"/>
+      <c r="F14" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G14" s="3" t="s">
         <v>51</v>
       </c>
@@ -17062,7 +17099,9 @@
       <c r="E15" s="3" t="n">
         <v>132.094</v>
       </c>
-      <c r="F15" s="3"/>
+      <c r="F15" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G15" s="3" t="s">
         <v>51</v>
       </c>
@@ -17082,7 +17121,9 @@
       <c r="E16" s="3" t="n">
         <v>246.174</v>
       </c>
-      <c r="F16" s="3"/>
+      <c r="F16" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G16" s="3" t="s">
         <v>51</v>
       </c>
@@ -17106,7 +17147,9 @@
       <c r="E17" s="3" t="n">
         <v>503.149</v>
       </c>
-      <c r="F17" s="3"/>
+      <c r="F17" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G17" s="3" t="s">
         <v>51</v>
       </c>
@@ -17126,7 +17169,9 @@
       <c r="E18" s="3" t="n">
         <v>400.152</v>
       </c>
-      <c r="F18" s="3"/>
+      <c r="F18" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G18" s="3" t="s">
         <v>51</v>
       </c>
@@ -17148,7 +17193,9 @@
       <c r="E19" s="3" t="n">
         <v>11298.8995</v>
       </c>
-      <c r="F19" s="3"/>
+      <c r="F19" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G19" s="3" t="s">
         <v>57</v>
       </c>
@@ -17170,7 +17217,9 @@
       <c r="E20" s="3" t="n">
         <v>97091.9214</v>
       </c>
-      <c r="F20" s="3"/>
+      <c r="F20" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G20" s="3" t="s">
         <v>61</v>
       </c>
@@ -17190,7 +17239,9 @@
       <c r="E21" s="3" t="n">
         <v>321.18</v>
       </c>
-      <c r="F21" s="3"/>
+      <c r="F21" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G21" s="3" t="s">
         <v>51</v>
       </c>
@@ -17210,7 +17261,9 @@
       <c r="E22" s="3" t="n">
         <v>44.0095</v>
       </c>
-      <c r="F22" s="3"/>
+      <c r="F22" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G22" s="3" t="s">
         <v>51</v>
       </c>
@@ -17234,7 +17287,9 @@
       <c r="E23" s="3" t="n">
         <v>479.124</v>
       </c>
-      <c r="F23" s="3"/>
+      <c r="F23" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G23" s="3" t="s">
         <v>51</v>
       </c>
@@ -17254,7 +17309,9 @@
       <c r="E24" s="3" t="n">
         <v>121.158</v>
       </c>
-      <c r="F24" s="3"/>
+      <c r="F24" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G24" s="3" t="s">
         <v>51</v>
       </c>
@@ -17274,7 +17331,9 @@
       <c r="E25" s="3" t="n">
         <v>224.301</v>
       </c>
-      <c r="F25" s="3"/>
+      <c r="F25" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G25" s="3" t="s">
         <v>51</v>
       </c>
@@ -17298,7 +17357,9 @@
       <c r="E26" s="3" t="n">
         <v>243.216</v>
       </c>
-      <c r="F26" s="3"/>
+      <c r="F26" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G26" s="3" t="s">
         <v>51</v>
       </c>
@@ -17320,7 +17381,9 @@
       <c r="E27" s="3" t="n">
         <v>262.005</v>
       </c>
-      <c r="F27" s="3"/>
+      <c r="F27" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G27" s="3" t="s">
         <v>51</v>
       </c>
@@ -17340,7 +17403,9 @@
       <c r="E28" s="3" t="n">
         <v>198.068</v>
       </c>
-      <c r="F28" s="3"/>
+      <c r="F28" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G28" s="3" t="s">
         <v>51</v>
       </c>
@@ -17362,7 +17427,9 @@
       <c r="E29" s="3" t="n">
         <v>11492.0791</v>
       </c>
-      <c r="F29" s="3"/>
+      <c r="F29" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G29" s="3" t="s">
         <v>57</v>
       </c>
@@ -17384,7 +17451,9 @@
       <c r="E30" s="3" t="n">
         <v>96912.9774</v>
       </c>
-      <c r="F30" s="3"/>
+      <c r="F30" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G30" s="3" t="s">
         <v>61</v>
       </c>
@@ -17404,7 +17473,9 @@
       <c r="E31" s="3" t="n">
         <v>258.12</v>
       </c>
-      <c r="F31" s="3"/>
+      <c r="F31" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G31" s="3" t="s">
         <v>51</v>
       </c>
@@ -17426,7 +17497,9 @@
       <c r="E32" s="3" t="n">
         <v>11272.1572</v>
       </c>
-      <c r="F32" s="3"/>
+      <c r="F32" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G32" s="3" t="s">
         <v>57</v>
       </c>
@@ -17448,7 +17521,9 @@
       <c r="E33" s="3" t="n">
         <v>96999.6024</v>
       </c>
-      <c r="F33" s="3"/>
+      <c r="F33" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G33" s="3" t="s">
         <v>61</v>
       </c>
@@ -17468,7 +17543,9 @@
       <c r="E34" s="3" t="n">
         <v>336.084</v>
       </c>
-      <c r="F34" s="3"/>
+      <c r="F34" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G34" s="3" t="s">
         <v>51</v>
       </c>
@@ -17488,7 +17565,9 @@
       <c r="E35" s="3" t="n">
         <v>183.033</v>
       </c>
-      <c r="F35" s="3"/>
+      <c r="F35" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G35" s="3" t="s">
         <v>51</v>
       </c>
@@ -17508,7 +17587,9 @@
       <c r="E36" s="3" t="n">
         <v>183.033</v>
       </c>
-      <c r="F36" s="3"/>
+      <c r="F36" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G36" s="3" t="s">
         <v>51</v>
       </c>
@@ -17528,7 +17609,9 @@
       <c r="E37" s="3" t="n">
         <v>258.12</v>
       </c>
-      <c r="F37" s="3"/>
+      <c r="F37" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G37" s="3" t="s">
         <v>51</v>
       </c>
@@ -17550,7 +17633,9 @@
       <c r="E38" s="3" t="n">
         <v>11569.3829</v>
       </c>
-      <c r="F38" s="3"/>
+      <c r="F38" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G38" s="3" t="s">
         <v>57</v>
       </c>
@@ -17572,7 +17657,9 @@
       <c r="E39" s="3" t="n">
         <v>96926.5024</v>
       </c>
-      <c r="F39" s="3"/>
+      <c r="F39" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G39" s="3" t="s">
         <v>61</v>
       </c>
@@ -17592,7 +17679,9 @@
       <c r="E40" s="3" t="n">
         <v>440.176</v>
       </c>
-      <c r="F40" s="3"/>
+      <c r="F40" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G40" s="3" t="s">
         <v>51</v>
       </c>
@@ -17614,7 +17703,9 @@
       <c r="E41" s="3" t="n">
         <v>10700.146</v>
       </c>
-      <c r="F41" s="3"/>
+      <c r="F41" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G41" s="3" t="s">
         <v>57</v>
       </c>
@@ -17636,7 +17727,9 @@
       <c r="E42" s="3" t="n">
         <v>96935.7124</v>
       </c>
-      <c r="F42" s="3"/>
+      <c r="F42" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G42" s="3" t="s">
         <v>61</v>
       </c>
@@ -17656,7 +17749,9 @@
       <c r="E43" s="3" t="n">
         <v>180.155</v>
       </c>
-      <c r="F43" s="3"/>
+      <c r="F43" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G43" s="3" t="s">
         <v>51</v>
       </c>
@@ -17680,7 +17775,9 @@
       <c r="E44" s="3" t="n">
         <v>146.144</v>
       </c>
-      <c r="F44" s="3"/>
+      <c r="F44" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G44" s="3" t="s">
         <v>51</v>
       </c>
@@ -17700,7 +17797,9 @@
       <c r="E45" s="3" t="n">
         <v>274.273</v>
       </c>
-      <c r="F45" s="3"/>
+      <c r="F45" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G45" s="3" t="s">
         <v>51</v>
       </c>
@@ -17724,7 +17823,9 @@
       <c r="E46" s="3" t="n">
         <v>146.121</v>
       </c>
-      <c r="F46" s="3"/>
+      <c r="F46" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G46" s="3" t="s">
         <v>51</v>
       </c>
@@ -17744,7 +17845,9 @@
       <c r="E47" s="3" t="n">
         <v>274.227</v>
       </c>
-      <c r="F47" s="3"/>
+      <c r="F47" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G47" s="3" t="s">
         <v>51</v>
       </c>
@@ -17768,7 +17871,9 @@
       <c r="E48" s="3" t="n">
         <v>75.0664</v>
       </c>
-      <c r="F48" s="3"/>
+      <c r="F48" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G48" s="3" t="s">
         <v>51</v>
       </c>
@@ -17788,7 +17893,9 @@
       <c r="E49" s="3" t="n">
         <v>132.118</v>
       </c>
-      <c r="F49" s="3"/>
+      <c r="F49" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G49" s="3" t="s">
         <v>51</v>
       </c>
@@ -17812,7 +17919,9 @@
       <c r="E50" s="3" t="n">
         <v>361.204</v>
       </c>
-      <c r="F50" s="3"/>
+      <c r="F50" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G50" s="3" t="s">
         <v>51</v>
       </c>
@@ -17832,7 +17941,9 @@
       <c r="E51" s="3" t="n">
         <v>151.126</v>
       </c>
-      <c r="F51" s="3"/>
+      <c r="F51" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G51" s="3" t="s">
         <v>51</v>
       </c>
@@ -17856,7 +17967,9 @@
       <c r="E52" s="3" t="n">
         <v>519.148</v>
       </c>
-      <c r="F52" s="3"/>
+      <c r="F52" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G52" s="3" t="s">
         <v>51</v>
       </c>
@@ -17876,7 +17989,9 @@
       <c r="E53" s="3" t="n">
         <v>1.0079</v>
       </c>
-      <c r="F53" s="3"/>
+      <c r="F53" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G53" s="3" t="s">
         <v>51</v>
       </c>
@@ -17898,7 +18013,9 @@
       <c r="E54" s="3" t="n">
         <v>18.0152</v>
       </c>
-      <c r="F54" s="3"/>
+      <c r="F54" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G54" s="3" t="s">
         <v>51</v>
       </c>
@@ -17922,7 +18039,9 @@
       <c r="E55" s="3" t="n">
         <v>155.154</v>
       </c>
-      <c r="F55" s="3"/>
+      <c r="F55" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G55" s="3" t="s">
         <v>51</v>
       </c>
@@ -17942,7 +18061,9 @@
       <c r="E56" s="3" t="n">
         <v>292.293</v>
       </c>
-      <c r="F56" s="3"/>
+      <c r="F56" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G56" s="3" t="s">
         <v>51</v>
       </c>
@@ -17968,7 +18089,9 @@
       <c r="E57" s="3" t="n">
         <v>11257.9285</v>
       </c>
-      <c r="F57" s="3"/>
+      <c r="F57" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G57" s="3" t="s">
         <v>57</v>
       </c>
@@ -17990,7 +18113,9 @@
       <c r="E58" s="3" t="n">
         <v>97473.0484</v>
       </c>
-      <c r="F58" s="3"/>
+      <c r="F58" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G58" s="3" t="s">
         <v>61</v>
       </c>
@@ -18010,7 +18135,9 @@
       <c r="E59" s="3" t="n">
         <v>131.172</v>
       </c>
-      <c r="F59" s="3"/>
+      <c r="F59" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G59" s="3" t="s">
         <v>51</v>
       </c>
@@ -18030,7 +18157,9 @@
       <c r="E60" s="3" t="n">
         <v>244.33</v>
       </c>
-      <c r="F60" s="3"/>
+      <c r="F60" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G60" s="3" t="s">
         <v>51</v>
       </c>
@@ -18054,7 +18183,9 @@
       <c r="E61" s="3" t="n">
         <v>89.0698</v>
       </c>
-      <c r="F61" s="3"/>
+      <c r="F61" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G61" s="3" t="s">
         <v>51</v>
       </c>
@@ -18076,7 +18207,9 @@
       <c r="E62" s="3" t="n">
         <v>10899.2893</v>
       </c>
-      <c r="F62" s="3"/>
+      <c r="F62" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G62" s="3" t="s">
         <v>57</v>
       </c>
@@ -18098,7 +18231,9 @@
       <c r="E63" s="3" t="n">
         <v>97211.0614</v>
       </c>
-      <c r="F63" s="3"/>
+      <c r="F63" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G63" s="3" t="s">
         <v>61</v>
       </c>
@@ -18120,7 +18255,9 @@
       <c r="E64" s="3" t="n">
         <v>11194.7491</v>
       </c>
-      <c r="F64" s="3"/>
+      <c r="F64" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G64" s="3" t="s">
         <v>57</v>
       </c>
@@ -18142,7 +18279,9 @@
       <c r="E65" s="3" t="n">
         <v>97143.8054</v>
       </c>
-      <c r="F65" s="3"/>
+      <c r="F65" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G65" s="3" t="s">
         <v>61</v>
       </c>
@@ -18162,7 +18301,9 @@
       <c r="E66" s="3" t="n">
         <v>131.172</v>
       </c>
-      <c r="F66" s="3"/>
+      <c r="F66" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G66" s="3" t="s">
         <v>51</v>
       </c>
@@ -18182,7 +18323,9 @@
       <c r="E67" s="3" t="n">
         <v>244.33</v>
       </c>
-      <c r="F67" s="3"/>
+      <c r="F67" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G67" s="3" t="s">
         <v>51</v>
       </c>
@@ -18206,7 +18349,9 @@
       <c r="E68" s="3" t="n">
         <v>147.195</v>
       </c>
-      <c r="F68" s="3"/>
+      <c r="F68" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G68" s="3" t="s">
         <v>51</v>
       </c>
@@ -18226,7 +18371,9 @@
       <c r="E69" s="3" t="n">
         <v>276.375</v>
       </c>
-      <c r="F69" s="3"/>
+      <c r="F69" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G69" s="3" t="s">
         <v>51</v>
       </c>
@@ -18250,7 +18397,9 @@
       <c r="E70" s="3" t="n">
         <v>149.211</v>
       </c>
-      <c r="F70" s="3"/>
+      <c r="F70" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G70" s="3" t="s">
         <v>51</v>
       </c>
@@ -18270,7 +18419,9 @@
       <c r="E71" s="3" t="n">
         <v>280.407</v>
       </c>
-      <c r="F71" s="3"/>
+      <c r="F71" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G71" s="3" t="s">
         <v>51</v>
       </c>
@@ -18294,7 +18445,9 @@
       <c r="E72" s="3" t="n">
         <v>662.416</v>
       </c>
-      <c r="F72" s="3"/>
+      <c r="F72" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G72" s="3" t="s">
         <v>51</v>
       </c>
@@ -18318,7 +18471,9 @@
       <c r="E73" s="3" t="n">
         <v>663.424</v>
       </c>
-      <c r="F73" s="3"/>
+      <c r="F73" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G73" s="3" t="s">
         <v>51</v>
       </c>
@@ -18340,7 +18495,9 @@
       <c r="E74" s="3" t="n">
         <v>11129.4153</v>
       </c>
-      <c r="F74" s="3"/>
+      <c r="F74" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G74" s="3" t="s">
         <v>57</v>
       </c>
@@ -18362,7 +18519,9 @@
       <c r="E75" s="3" t="n">
         <v>97015.7604</v>
       </c>
-      <c r="F75" s="3"/>
+      <c r="F75" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G75" s="3" t="s">
         <v>61</v>
       </c>
@@ -18382,7 +18541,9 @@
       <c r="E76" s="3" t="n">
         <v>31.9988</v>
       </c>
-      <c r="F76" s="3"/>
+      <c r="F76" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G76" s="3" t="s">
         <v>51</v>
       </c>
@@ -18406,7 +18567,9 @@
       <c r="E77" s="3" t="n">
         <v>165.018</v>
       </c>
-      <c r="F77" s="3"/>
+      <c r="F77" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G77" s="3" t="s">
         <v>51</v>
       </c>
@@ -18428,7 +18591,9 @@
       <c r="E78" s="3" t="n">
         <v>11256.6933</v>
       </c>
-      <c r="F78" s="3"/>
+      <c r="F78" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G78" s="3" t="s">
         <v>57</v>
       </c>
@@ -18450,7 +18615,9 @@
       <c r="E79" s="3" t="n">
         <v>97069.6674</v>
       </c>
-      <c r="F79" s="3"/>
+      <c r="F79" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G79" s="3" t="s">
         <v>61</v>
       </c>
@@ -18472,7 +18639,9 @@
       <c r="E80" s="3" t="n">
         <v>11426.8266</v>
       </c>
-      <c r="F80" s="3"/>
+      <c r="F80" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G80" s="3" t="s">
         <v>57</v>
       </c>
@@ -18494,7 +18663,9 @@
       <c r="E81" s="3" t="n">
         <v>96846.4144</v>
       </c>
-      <c r="F81" s="3"/>
+      <c r="F81" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G81" s="3" t="s">
         <v>61</v>
       </c>
@@ -18516,7 +18687,9 @@
       <c r="E82" s="3" t="n">
         <v>11164.5594</v>
       </c>
-      <c r="F82" s="3"/>
+      <c r="F82" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G82" s="3" t="s">
         <v>57</v>
       </c>
@@ -18538,7 +18711,9 @@
       <c r="E83" s="3" t="n">
         <v>97452.3234</v>
       </c>
-      <c r="F83" s="3"/>
+      <c r="F83" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G83" s="3" t="s">
         <v>61</v>
       </c>
@@ -18560,7 +18735,9 @@
       <c r="E84" s="3" t="n">
         <v>10839.3244</v>
       </c>
-      <c r="F84" s="3"/>
+      <c r="F84" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G84" s="3" t="s">
         <v>57</v>
       </c>
@@ -18582,7 +18759,9 @@
       <c r="E85" s="3" t="n">
         <v>96860.6824</v>
       </c>
-      <c r="F85" s="3"/>
+      <c r="F85" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G85" s="3" t="s">
         <v>61</v>
       </c>
@@ -18604,7 +18783,9 @@
       <c r="E86" s="3" t="n">
         <v>11422.9086</v>
       </c>
-      <c r="F86" s="3"/>
+      <c r="F86" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G86" s="3" t="s">
         <v>57</v>
       </c>
@@ -18626,7 +18807,9 @@
       <c r="E87" s="3" t="n">
         <v>96891.6954</v>
       </c>
-      <c r="F87" s="3"/>
+      <c r="F87" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G87" s="3" t="s">
         <v>61</v>
       </c>
@@ -18646,7 +18829,9 @@
       <c r="E88" s="3" t="n">
         <v>165.189</v>
       </c>
-      <c r="F88" s="3"/>
+      <c r="F88" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G88" s="3" t="s">
         <v>51</v>
       </c>
@@ -18666,7 +18851,9 @@
       <c r="E89" s="3" t="n">
         <v>312.362</v>
       </c>
-      <c r="F89" s="3"/>
+      <c r="F89" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G89" s="3" t="s">
         <v>51</v>
       </c>
@@ -18690,7 +18877,9 @@
       <c r="E90" s="3" t="n">
         <v>95.9793</v>
       </c>
-      <c r="F90" s="3"/>
+      <c r="F90" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G90" s="3" t="s">
         <v>51</v>
       </c>
@@ -18714,7 +18903,9 @@
       <c r="E91" s="3" t="n">
         <v>10816.122</v>
       </c>
-      <c r="F91" s="3"/>
+      <c r="F91" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G91" s="3" t="s">
         <v>57</v>
       </c>
@@ -18736,7 +18927,9 @@
       <c r="E92" s="3" t="n">
         <v>96985.7724</v>
       </c>
-      <c r="F92" s="3"/>
+      <c r="F92" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G92" s="3" t="s">
         <v>61</v>
       </c>
@@ -18758,7 +18951,9 @@
       <c r="E93" s="3" t="n">
         <v>11689.35</v>
       </c>
-      <c r="F93" s="3"/>
+      <c r="F93" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G93" s="3" t="s">
         <v>57</v>
       </c>
@@ -18780,7 +18975,9 @@
       <c r="E94" s="3" t="n">
         <v>96885.7984</v>
       </c>
-      <c r="F94" s="3"/>
+      <c r="F94" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G94" s="3" t="s">
         <v>61</v>
       </c>
@@ -18800,7 +18997,9 @@
       <c r="E95" s="3" t="n">
         <v>174.951</v>
       </c>
-      <c r="F95" s="3"/>
+      <c r="F95" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G95" s="3" t="s">
         <v>51</v>
       </c>
@@ -18820,7 +19019,9 @@
       <c r="E96" s="3" t="n">
         <v>115.13</v>
       </c>
-      <c r="F96" s="3"/>
+      <c r="F96" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G96" s="3" t="s">
         <v>51</v>
       </c>
@@ -18840,7 +19041,9 @@
       <c r="E97" s="3" t="n">
         <v>212.245</v>
       </c>
-      <c r="F97" s="3"/>
+      <c r="F97" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G97" s="3" t="s">
         <v>51</v>
       </c>
@@ -18864,7 +19067,9 @@
       <c r="E98" s="3" t="n">
         <v>385.03</v>
       </c>
-      <c r="F98" s="3"/>
+      <c r="F98" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G98" s="3" t="s">
         <v>51</v>
       </c>
@@ -18886,7 +19091,9 @@
       <c r="E99" s="3" t="n">
         <v>11101.9732</v>
       </c>
-      <c r="F99" s="3"/>
+      <c r="F99" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G99" s="3" t="s">
         <v>57</v>
       </c>
@@ -18908,7 +19115,9 @@
       <c r="E100" s="3" t="n">
         <v>97311.1414</v>
       </c>
-      <c r="F100" s="3"/>
+      <c r="F100" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G100" s="3" t="s">
         <v>61</v>
       </c>
@@ -18930,7 +19139,9 @@
       <c r="E101" s="3" t="n">
         <v>11031.3146</v>
       </c>
-      <c r="F101" s="3"/>
+      <c r="F101" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G101" s="3" t="s">
         <v>57</v>
       </c>
@@ -18952,7 +19163,9 @@
       <c r="E102" s="3" t="n">
         <v>96859.8964</v>
       </c>
-      <c r="F102" s="3"/>
+      <c r="F102" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G102" s="3" t="s">
         <v>61</v>
       </c>
@@ -18974,7 +19187,9 @@
       <c r="E103" s="3" t="n">
         <v>11201.3035</v>
       </c>
-      <c r="F103" s="3"/>
+      <c r="F103" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G103" s="3" t="s">
         <v>57</v>
       </c>
@@ -18996,7 +19211,9 @@
       <c r="E104" s="3" t="n">
         <v>97096.1004</v>
       </c>
-      <c r="F104" s="3"/>
+      <c r="F104" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G104" s="3" t="s">
         <v>61</v>
       </c>
@@ -19016,7 +19233,9 @@
       <c r="E105" s="3" t="n">
         <v>87.054</v>
       </c>
-      <c r="F105" s="3"/>
+      <c r="F105" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G105" s="3" t="s">
         <v>51</v>
       </c>
@@ -19038,7 +19257,9 @@
       <c r="E106" s="3" t="n">
         <v>11205.9319</v>
       </c>
-      <c r="F106" s="3"/>
+      <c r="F106" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G106" s="3" t="s">
         <v>57</v>
       </c>
@@ -19060,7 +19281,9 @@
       <c r="E107" s="3" t="n">
         <v>96495.5014</v>
       </c>
-      <c r="F107" s="3"/>
+      <c r="F107" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G107" s="3" t="s">
         <v>61</v>
       </c>
@@ -19080,7 +19303,9 @@
       <c r="E108" s="3" t="n">
         <v>228.094</v>
       </c>
-      <c r="F108" s="3"/>
+      <c r="F108" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G108" s="3" t="s">
         <v>51</v>
       </c>
@@ -19102,7 +19327,9 @@
       <c r="E109" s="3" t="n">
         <v>11189.0439</v>
       </c>
-      <c r="F109" s="3"/>
+      <c r="F109" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G109" s="3" t="s">
         <v>57</v>
       </c>
@@ -19124,7 +19351,9 @@
       <c r="E110" s="3" t="n">
         <v>96734.6074</v>
       </c>
-      <c r="F110" s="3"/>
+      <c r="F110" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G110" s="3" t="s">
         <v>61</v>
       </c>
@@ -19144,7 +19373,9 @@
       <c r="E111" s="3" t="n">
         <v>228.094</v>
       </c>
-      <c r="F111" s="3"/>
+      <c r="F111" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G111" s="3" t="s">
         <v>51</v>
       </c>
@@ -19166,7 +19397,9 @@
       <c r="E112" s="3" t="n">
         <v>12048.1694</v>
       </c>
-      <c r="F112" s="3"/>
+      <c r="F112" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G112" s="3" t="s">
         <v>57</v>
       </c>
@@ -19188,7 +19421,9 @@
       <c r="E113" s="3" t="n">
         <v>96965.7004</v>
       </c>
-      <c r="F113" s="3"/>
+      <c r="F113" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G113" s="3" t="s">
         <v>61</v>
       </c>
@@ -19210,7 +19445,9 @@
       <c r="E114" s="3" t="n">
         <v>11400.9224</v>
       </c>
-      <c r="F114" s="3"/>
+      <c r="F114" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G114" s="3" t="s">
         <v>57</v>
       </c>
@@ -19232,7 +19469,9 @@
       <c r="E115" s="3" t="n">
         <v>97136.8574</v>
       </c>
-      <c r="F115" s="3"/>
+      <c r="F115" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G115" s="3" t="s">
         <v>61</v>
       </c>
@@ -19254,7 +19493,9 @@
       <c r="E116" s="3" t="n">
         <v>11565.0949</v>
       </c>
-      <c r="F116" s="3"/>
+      <c r="F116" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G116" s="3" t="s">
         <v>57</v>
       </c>
@@ -19276,7 +19517,9 @@
       <c r="E117" s="3" t="n">
         <v>97588.6064</v>
       </c>
-      <c r="F117" s="3"/>
+      <c r="F117" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G117" s="3" t="s">
         <v>61</v>
       </c>
@@ -19296,7 +19539,9 @@
       <c r="E118" s="3" t="n">
         <v>288.145</v>
       </c>
-      <c r="F118" s="3"/>
+      <c r="F118" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G118" s="3" t="s">
         <v>51</v>
       </c>
@@ -19316,7 +19561,9 @@
       <c r="E119" s="3" t="n">
         <v>105.092</v>
       </c>
-      <c r="F119" s="3"/>
+      <c r="F119" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G119" s="3" t="s">
         <v>51</v>
       </c>
@@ -19336,7 +19583,9 @@
       <c r="E120" s="3" t="n">
         <v>192.169</v>
       </c>
-      <c r="F120" s="3"/>
+      <c r="F120" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G120" s="3" t="s">
         <v>51</v>
       </c>
@@ -19360,7 +19609,9 @@
       <c r="E121" s="3" t="n">
         <v>168.042</v>
       </c>
-      <c r="F121" s="3"/>
+      <c r="F121" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G121" s="3" t="s">
         <v>51</v>
       </c>
@@ -19380,7 +19631,9 @@
       <c r="E122" s="3" t="n">
         <v>168.042</v>
       </c>
-      <c r="F122" s="3"/>
+      <c r="F122" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G122" s="3" t="s">
         <v>51</v>
       </c>
@@ -19400,7 +19653,9 @@
       <c r="E123" s="3" t="n">
         <v>119.119</v>
       </c>
-      <c r="F123" s="3"/>
+      <c r="F123" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G123" s="3" t="s">
         <v>51</v>
       </c>
@@ -19420,7 +19675,9 @@
       <c r="E124" s="3" t="n">
         <v>220.222</v>
       </c>
-      <c r="F124" s="3"/>
+      <c r="F124" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G124" s="3" t="s">
         <v>51</v>
       </c>
@@ -19446,7 +19703,9 @@
       <c r="E125" s="3" t="n">
         <v>11440.1771</v>
       </c>
-      <c r="F125" s="3"/>
+      <c r="F125" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G125" s="3" t="s">
         <v>57</v>
       </c>
@@ -19468,7 +19727,9 @@
       <c r="E126" s="3" t="n">
         <v>97022.6024</v>
       </c>
-      <c r="F126" s="3"/>
+      <c r="F126" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G126" s="3" t="s">
         <v>61</v>
       </c>
@@ -19490,7 +19751,9 @@
       <c r="E127" s="3" t="n">
         <v>10896.0191</v>
       </c>
-      <c r="F127" s="3"/>
+      <c r="F127" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G127" s="3" t="s">
         <v>57</v>
       </c>
@@ -19512,7 +19775,9 @@
       <c r="E128" s="3" t="n">
         <v>96870.8244</v>
       </c>
-      <c r="F128" s="3"/>
+      <c r="F128" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G128" s="3" t="s">
         <v>61</v>
       </c>
@@ -19532,7 +19797,9 @@
       <c r="E129" s="3" t="n">
         <v>204.225</v>
       </c>
-      <c r="F129" s="3"/>
+      <c r="F129" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G129" s="3" t="s">
         <v>51</v>
       </c>
@@ -19552,7 +19819,9 @@
       <c r="E130" s="3" t="n">
         <v>390.434</v>
       </c>
-      <c r="F130" s="3"/>
+      <c r="F130" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G130" s="3" t="s">
         <v>51</v>
       </c>
@@ -19576,7 +19845,9 @@
       <c r="E131" s="3" t="n">
         <v>181.188</v>
       </c>
-      <c r="F131" s="3"/>
+      <c r="F131" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G131" s="3" t="s">
         <v>51</v>
       </c>
@@ -19596,7 +19867,9 @@
       <c r="E132" s="3" t="n">
         <v>344.361</v>
       </c>
-      <c r="F132" s="3"/>
+      <c r="F132" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G132" s="3" t="s">
         <v>51</v>
       </c>
@@ -19622,7 +19895,9 @@
       <c r="E133" s="3" t="n">
         <v>10812.4343</v>
       </c>
-      <c r="F133" s="3"/>
+      <c r="F133" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G133" s="3" t="s">
         <v>57</v>
       </c>
@@ -19644,7 +19919,9 @@
       <c r="E134" s="3" t="n">
         <v>97302.1834</v>
       </c>
-      <c r="F134" s="3"/>
+      <c r="F134" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G134" s="3" t="s">
         <v>61</v>
       </c>
@@ -19664,7 +19941,9 @@
       <c r="E135" s="3" t="n">
         <v>401.137</v>
       </c>
-      <c r="F135" s="3"/>
+      <c r="F135" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G135" s="3" t="s">
         <v>51</v>
       </c>
@@ -19684,7 +19963,9 @@
       <c r="E136" s="3" t="n">
         <v>322.165</v>
       </c>
-      <c r="F136" s="3"/>
+      <c r="F136" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G136" s="3" t="s">
         <v>51</v>
       </c>
@@ -19706,7 +19987,9 @@
       <c r="E137" s="3" t="n">
         <v>11169.4967</v>
       </c>
-      <c r="F137" s="3"/>
+      <c r="F137" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G137" s="3" t="s">
         <v>57</v>
       </c>
@@ -19728,7 +20011,9 @@
       <c r="E138" s="3" t="n">
         <v>96677.7454</v>
       </c>
-      <c r="F138" s="3"/>
+      <c r="F138" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G138" s="3" t="s">
         <v>61</v>
       </c>
@@ -19748,7 +20033,9 @@
       <c r="E139" s="3" t="n">
         <v>112.087</v>
       </c>
-      <c r="F139" s="3"/>
+      <c r="F139" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G139" s="3" t="s">
         <v>51</v>
       </c>
@@ -19772,7 +20059,9 @@
       <c r="E140" s="3" t="n">
         <v>244.201</v>
       </c>
-      <c r="F140" s="3"/>
+      <c r="F140" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G140" s="3" t="s">
         <v>51</v>
       </c>
@@ -19792,7 +20081,9 @@
       <c r="E141" s="3" t="n">
         <v>480.109</v>
       </c>
-      <c r="F141" s="3"/>
+      <c r="F141" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G141" s="3" t="s">
         <v>51</v>
       </c>
@@ -19816,7 +20107,9 @@
       <c r="E142" s="3" t="n">
         <v>117.146</v>
       </c>
-      <c r="F142" s="3"/>
+      <c r="F142" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G142" s="3" t="s">
         <v>51</v>
       </c>
@@ -19836,7 +20129,9 @@
       <c r="E143" s="3" t="n">
         <v>216.277</v>
       </c>
-      <c r="F143" s="3"/>
+      <c r="F143" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G143" s="3" t="s">
         <v>51</v>
       </c>
@@ -19860,7 +20155,9 @@
       <c r="E144" s="3" t="n">
         <v>228.094</v>
       </c>
-      <c r="F144" s="3"/>
+      <c r="F144" s="3" t="n">
+        <v>0</v>
+      </c>
       <c r="G144" s="3" t="s">
         <v>51</v>
       </c>
@@ -19893,12 +20190,12 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E2" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="bottomRight" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.9230769230769"/>
     <col collapsed="false" hidden="false" max="7" min="2" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="1" width="9.10526315789474"/>
   </cols>
@@ -22049,14 +22346,14 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="bottomRight" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.8502024291498"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="28.0647773279352"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="27.8502024291498"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="28.0647773279352"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -24356,13 +24653,13 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="bottomRight" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="1" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="34.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="34.7085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -24453,13 +24750,13 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D1" activeCellId="0" sqref="1:1048576"/>
+      <selection pane="bottomRight" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="1" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.7449392712551"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="8.78542510121457"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
adding units to DfbaNetComponent and renaming coefficient to value
</commit_message>
<xml_diff>
--- a/tests/fixtures/example-model.xlsx
+++ b/tests/fixtures/example-model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -407,7 +407,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3929" uniqueCount="1842">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3965" uniqueCount="1842">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -4987,7 +4987,7 @@
     <t xml:space="preserve">dFBA net reaction</t>
   </si>
   <si>
-    <t xml:space="preserve">Coefficient</t>
+    <t xml:space="preserve">Value</t>
   </si>
   <si>
     <t xml:space="preserve">dfba-net-comp-Metabolism_net_rxn-ALA[c]</t>
@@ -4996,6 +4996,9 @@
     <t xml:space="preserve">ALA net component</t>
   </si>
   <si>
+    <t xml:space="preserve">M s^-1</t>
+  </si>
+  <si>
     <t xml:space="preserve">test</t>
   </si>
   <si>
@@ -5198,9 +5201,6 @@
   </si>
   <si>
     <t xml:space="preserve">dfba-net-comp-Other_net_rxn-UMP[c]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Value</t>
   </si>
   <si>
     <t xml:space="preserve">carbonExchangeRate</t>
@@ -6233,7 +6233,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="topRight" activeCell="B16" activeCellId="1" sqref="F2:F36 B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -6361,7 +6361,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="bottomRight" activeCell="F1" activeCellId="1" sqref="F2:F36 F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -6432,7 +6432,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="bottomRight" activeCell="I1" activeCellId="1" sqref="F2:F36 I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -10503,7 +10503,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A140" activeCellId="0" sqref="A140"/>
-      <selection pane="bottomRight" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="bottomRight" activeCell="I1" activeCellId="1" sqref="F2:F36 I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -14579,7 +14579,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomRight" activeCell="D9" activeCellId="1" sqref="F2:F36 D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -14659,14 +14659,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B27" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
+      <selection pane="bottomRight" activeCell="F2" activeCellId="0" sqref="F2:F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -14674,12 +14674,14 @@
     <col collapsed="false" hidden="false" max="1" min="1" style="12" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="12" width="20.8866396761134"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="12" width="19.8178137651822"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="12" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="12" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="12" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="12" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="1021" min="10" style="3" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="1" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="12" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="12" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="12" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="12" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="12" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="1022" min="11" style="3" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1023" min="1023" style="1" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.78542510121457"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14693,21 +14695,24 @@
         <v>1525</v>
       </c>
       <c r="D1" s="13" t="s">
+        <v>578</v>
+      </c>
+      <c r="E1" s="13" t="s">
         <v>1526</v>
       </c>
-      <c r="E1" s="13" t="s">
-        <v>578</v>
-      </c>
       <c r="F1" s="13" t="s">
+        <v>581</v>
+      </c>
+      <c r="G1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>24</v>
       </c>
     </row>
@@ -14721,595 +14726,700 @@
       <c r="C2" s="11" t="s">
         <v>1519</v>
       </c>
-      <c r="D2" s="14" t="n">
+      <c r="D2" s="12" t="s">
+        <v>408</v>
+      </c>
+      <c r="E2" s="14" t="n">
         <v>-34190.38</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>408</v>
-      </c>
-      <c r="H2" s="12" t="s">
+      <c r="F2" s="14" t="s">
         <v>1529</v>
       </c>
       <c r="I2" s="12" t="s">
         <v>1530</v>
       </c>
+      <c r="J2" s="12" t="s">
+        <v>1531</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
-        <v>1531</v>
+        <v>1532</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>1532</v>
+        <v>1533</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>1519</v>
       </c>
-      <c r="D3" s="14" t="n">
+      <c r="D3" s="12" t="s">
+        <v>411</v>
+      </c>
+      <c r="E3" s="14" t="n">
         <v>1035619</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>411</v>
+      <c r="F3" s="14" t="s">
+        <v>1529</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="12" t="s">
-        <v>1533</v>
+        <v>1534</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>1534</v>
+        <v>1535</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>1519</v>
       </c>
-      <c r="D4" s="14" t="n">
+      <c r="D4" s="12" t="s">
+        <v>414</v>
+      </c>
+      <c r="E4" s="14" t="n">
         <v>-40890.38</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>414</v>
+      <c r="F4" s="14" t="s">
+        <v>1529</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="12" t="s">
-        <v>1535</v>
+        <v>1536</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>1536</v>
+        <v>1537</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>1519</v>
       </c>
-      <c r="D5" s="14" t="n">
+      <c r="D5" s="12" t="s">
+        <v>417</v>
+      </c>
+      <c r="E5" s="14" t="n">
         <v>-23190.38</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>417</v>
+      <c r="F5" s="14" t="s">
+        <v>1529</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="12" t="s">
-        <v>1537</v>
+        <v>1538</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>1538</v>
+        <v>1539</v>
       </c>
       <c r="C6" s="11" t="s">
         <v>1519</v>
       </c>
-      <c r="D6" s="14" t="n">
+      <c r="D6" s="12" t="s">
+        <v>420</v>
+      </c>
+      <c r="E6" s="14" t="n">
         <v>-24290.38</v>
       </c>
-      <c r="E6" s="12" t="s">
-        <v>420</v>
+      <c r="F6" s="14" t="s">
+        <v>1529</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="12" t="s">
-        <v>1539</v>
+        <v>1540</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="C7" s="11" t="s">
         <v>1519</v>
       </c>
-      <c r="D7" s="14" t="n">
+      <c r="D7" s="12" t="s">
+        <v>423</v>
+      </c>
+      <c r="E7" s="14" t="n">
         <v>-1101856</v>
       </c>
-      <c r="E7" s="12" t="s">
-        <v>423</v>
+      <c r="F7" s="14" t="s">
+        <v>1529</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="12" t="s">
-        <v>1541</v>
+        <v>1542</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>1542</v>
+        <v>1543</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>1519</v>
       </c>
-      <c r="D8" s="14" t="n">
+      <c r="D8" s="12" t="s">
+        <v>427</v>
+      </c>
+      <c r="E8" s="14" t="n">
         <v>1098019</v>
       </c>
-      <c r="E8" s="12" t="s">
-        <v>427</v>
+      <c r="F8" s="14" t="s">
+        <v>1529</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="12" t="s">
-        <v>1543</v>
+        <v>1544</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>1519</v>
       </c>
-      <c r="D9" s="14" t="n">
+      <c r="D9" s="12" t="s">
+        <v>430</v>
+      </c>
+      <c r="E9" s="14" t="n">
         <v>-1164906</v>
       </c>
-      <c r="E9" s="12" t="s">
-        <v>430</v>
+      <c r="F9" s="14" t="s">
+        <v>1529</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="12" t="s">
-        <v>1545</v>
+        <v>1546</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>1546</v>
+        <v>1547</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>1519</v>
       </c>
-      <c r="D10" s="14" t="n">
+      <c r="D10" s="12" t="s">
+        <v>431</v>
+      </c>
+      <c r="E10" s="14" t="n">
         <v>-22290.38</v>
       </c>
-      <c r="E10" s="12" t="s">
-        <v>431</v>
+      <c r="F10" s="14" t="s">
+        <v>1529</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="12" t="s">
-        <v>1547</v>
+        <v>1548</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>1548</v>
+        <v>1549</v>
       </c>
       <c r="C11" s="11" t="s">
         <v>1519</v>
       </c>
-      <c r="D11" s="14" t="n">
+      <c r="D11" s="12" t="s">
+        <v>449</v>
+      </c>
+      <c r="E11" s="14" t="n">
         <v>581419.2</v>
       </c>
-      <c r="E11" s="12" t="s">
-        <v>449</v>
+      <c r="F11" s="14" t="s">
+        <v>1529</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="12" t="s">
-        <v>1549</v>
+        <v>1550</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>1550</v>
+        <v>1551</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>1519</v>
       </c>
-      <c r="D12" s="14" t="n">
+      <c r="D12" s="12" t="s">
+        <v>453</v>
+      </c>
+      <c r="E12" s="14" t="n">
         <v>-24690.38</v>
       </c>
-      <c r="E12" s="12" t="s">
-        <v>453</v>
+      <c r="F12" s="14" t="s">
+        <v>1529</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="12" t="s">
-        <v>1551</v>
+        <v>1552</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>1552</v>
+        <v>1553</v>
       </c>
       <c r="C13" s="11" t="s">
         <v>1519</v>
       </c>
-      <c r="D13" s="14" t="n">
+      <c r="D13" s="12" t="s">
+        <v>456</v>
+      </c>
+      <c r="E13" s="14" t="n">
         <v>-22690.38</v>
       </c>
-      <c r="E13" s="12" t="s">
-        <v>456</v>
+      <c r="F13" s="14" t="s">
+        <v>1529</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="12" t="s">
-        <v>1553</v>
+        <v>1554</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>1554</v>
+        <v>1555</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>1519</v>
       </c>
-      <c r="D14" s="14" t="n">
+      <c r="D14" s="12" t="s">
+        <v>459</v>
+      </c>
+      <c r="E14" s="14" t="n">
         <v>-31190.38</v>
       </c>
-      <c r="E14" s="12" t="s">
-        <v>459</v>
+      <c r="F14" s="14" t="s">
+        <v>1529</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="12" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>1556</v>
+        <v>1557</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>1519</v>
       </c>
-      <c r="D15" s="14" t="n">
+      <c r="D15" s="12" t="s">
+        <v>462</v>
+      </c>
+      <c r="E15" s="14" t="n">
         <v>1052899</v>
       </c>
-      <c r="E15" s="12" t="s">
-        <v>462</v>
+      <c r="F15" s="14" t="s">
+        <v>1529</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="12" t="s">
-        <v>1557</v>
+        <v>1558</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>1558</v>
+        <v>1559</v>
       </c>
       <c r="C16" s="11" t="s">
         <v>1519</v>
       </c>
-      <c r="D16" s="14" t="n">
+      <c r="D16" s="12" t="s">
+        <v>465</v>
+      </c>
+      <c r="E16" s="14" t="n">
         <v>-1728316</v>
       </c>
-      <c r="E16" s="12" t="s">
-        <v>465</v>
+      <c r="F16" s="14" t="s">
+        <v>1529</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="12" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>1560</v>
+        <v>1561</v>
       </c>
       <c r="C17" s="11" t="s">
         <v>1519</v>
       </c>
-      <c r="D17" s="14" t="n">
+      <c r="D17" s="12" t="s">
+        <v>466</v>
+      </c>
+      <c r="E17" s="14" t="n">
         <v>-1521617000</v>
       </c>
-      <c r="E17" s="12" t="s">
-        <v>466</v>
+      <c r="F17" s="14" t="s">
+        <v>1529</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="12" t="s">
-        <v>1561</v>
+        <v>1562</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>1562</v>
+        <v>1563</v>
       </c>
       <c r="C18" s="11" t="s">
         <v>1519</v>
       </c>
-      <c r="D18" s="14" t="n">
+      <c r="D18" s="12" t="s">
+        <v>468</v>
+      </c>
+      <c r="E18" s="14" t="n">
         <v>4972350</v>
       </c>
-      <c r="E18" s="12" t="s">
-        <v>468</v>
+      <c r="F18" s="14" t="s">
+        <v>1529</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="12" t="s">
-        <v>1563</v>
+        <v>1564</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>1564</v>
+        <v>1565</v>
       </c>
       <c r="C19" s="11" t="s">
         <v>1519</v>
       </c>
-      <c r="D19" s="14" t="n">
+      <c r="D19" s="12" t="s">
+        <v>470</v>
+      </c>
+      <c r="E19" s="14" t="n">
         <v>-21590.38</v>
       </c>
-      <c r="E19" s="12" t="s">
-        <v>470</v>
+      <c r="F19" s="14" t="s">
+        <v>1529</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="12" t="s">
-        <v>1565</v>
+        <v>1566</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>1519</v>
       </c>
-      <c r="D20" s="14" t="n">
+      <c r="D20" s="12" t="s">
+        <v>475</v>
+      </c>
+      <c r="E20" s="14" t="n">
         <v>-29290.38</v>
       </c>
-      <c r="E20" s="12" t="s">
-        <v>475</v>
+      <c r="F20" s="14" t="s">
+        <v>1529</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="12" t="s">
-        <v>1567</v>
+        <v>1568</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>1568</v>
+        <v>1569</v>
       </c>
       <c r="C21" s="11" t="s">
         <v>1519</v>
       </c>
-      <c r="D21" s="14" t="n">
+      <c r="D21" s="12" t="s">
+        <v>484</v>
+      </c>
+      <c r="E21" s="14" t="n">
         <v>-41190.38</v>
       </c>
-      <c r="E21" s="12" t="s">
-        <v>484</v>
+      <c r="F21" s="14" t="s">
+        <v>1529</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="12" t="s">
-        <v>1569</v>
+        <v>1570</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>1570</v>
+        <v>1571</v>
       </c>
       <c r="C22" s="11" t="s">
         <v>1519</v>
       </c>
-      <c r="D22" s="14" t="n">
+      <c r="D22" s="12" t="s">
+        <v>487</v>
+      </c>
+      <c r="E22" s="14" t="n">
         <v>-21990.38</v>
       </c>
-      <c r="E22" s="12" t="s">
-        <v>487</v>
+      <c r="F22" s="14" t="s">
+        <v>1529</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="12" t="s">
-        <v>1571</v>
+        <v>1572</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>1572</v>
+        <v>1573</v>
       </c>
       <c r="C23" s="11" t="s">
         <v>1519</v>
       </c>
-      <c r="D23" s="14" t="n">
+      <c r="D23" s="12" t="s">
+        <v>490</v>
+      </c>
+      <c r="E23" s="14" t="n">
         <v>-21390.38</v>
       </c>
-      <c r="E23" s="12" t="s">
-        <v>490</v>
+      <c r="F23" s="14" t="s">
+        <v>1529</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="12" t="s">
-        <v>1573</v>
+        <v>1574</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>1574</v>
+        <v>1575</v>
       </c>
       <c r="C24" s="11" t="s">
         <v>1519</v>
       </c>
-      <c r="D24" s="14" t="n">
+      <c r="D24" s="12" t="s">
+        <v>511</v>
+      </c>
+      <c r="E24" s="14" t="n">
         <v>-23890.38</v>
       </c>
-      <c r="E24" s="12" t="s">
-        <v>511</v>
+      <c r="F24" s="14" t="s">
+        <v>1529</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="12" t="s">
-        <v>1575</v>
+        <v>1576</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>1576</v>
+        <v>1577</v>
       </c>
       <c r="C25" s="11" t="s">
         <v>1519</v>
       </c>
-      <c r="D25" s="14" t="n">
+      <c r="D25" s="12" t="s">
+        <v>514</v>
+      </c>
+      <c r="E25" s="14" t="n">
         <v>471096.2</v>
       </c>
-      <c r="E25" s="12" t="s">
-        <v>514</v>
+      <c r="F25" s="14" t="s">
+        <v>1529</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="12" t="s">
-        <v>1577</v>
+        <v>1578</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>1578</v>
+        <v>1579</v>
       </c>
       <c r="C26" s="11" t="s">
         <v>1519</v>
       </c>
-      <c r="D26" s="14" t="n">
+      <c r="D26" s="12" t="s">
+        <v>520</v>
+      </c>
+      <c r="E26" s="14" t="n">
         <v>4381069</v>
       </c>
-      <c r="E26" s="12" t="s">
-        <v>520</v>
+      <c r="F26" s="14" t="s">
+        <v>1529</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="12" t="s">
-        <v>1579</v>
+        <v>1580</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>1580</v>
+        <v>1581</v>
       </c>
       <c r="C27" s="11" t="s">
         <v>1519</v>
       </c>
-      <c r="D27" s="14" t="n">
+      <c r="D27" s="12" t="s">
+        <v>521</v>
+      </c>
+      <c r="E27" s="14" t="n">
         <v>-34390.38</v>
       </c>
-      <c r="E27" s="12" t="s">
-        <v>521</v>
+      <c r="F27" s="14" t="s">
+        <v>1529</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="12" t="s">
-        <v>1581</v>
+        <v>1582</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>1582</v>
+        <v>1583</v>
       </c>
       <c r="C28" s="11" t="s">
         <v>1519</v>
       </c>
-      <c r="D28" s="14" t="n">
+      <c r="D28" s="12" t="s">
+        <v>545</v>
+      </c>
+      <c r="E28" s="14" t="n">
         <v>-44490.38</v>
       </c>
-      <c r="E28" s="12" t="s">
-        <v>545</v>
+      <c r="F28" s="14" t="s">
+        <v>1529</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="12" t="s">
-        <v>1583</v>
+        <v>1584</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>1584</v>
+        <v>1585</v>
       </c>
       <c r="C29" s="11" t="s">
         <v>1519</v>
       </c>
-      <c r="D29" s="14" t="n">
+      <c r="D29" s="12" t="s">
+        <v>550</v>
+      </c>
+      <c r="E29" s="14" t="n">
         <v>-36190.38</v>
       </c>
-      <c r="E29" s="12" t="s">
-        <v>550</v>
+      <c r="F29" s="14" t="s">
+        <v>1529</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="12" t="s">
-        <v>1585</v>
+        <v>1586</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>1586</v>
+        <v>1587</v>
       </c>
       <c r="C30" s="11" t="s">
         <v>1519</v>
       </c>
-      <c r="D30" s="14" t="n">
+      <c r="D30" s="12" t="s">
+        <v>557</v>
+      </c>
+      <c r="E30" s="14" t="n">
         <v>-22190.38</v>
       </c>
-      <c r="E30" s="12" t="s">
-        <v>557</v>
+      <c r="F30" s="14" t="s">
+        <v>1529</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="12" t="s">
-        <v>1587</v>
+        <v>1588</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>1588</v>
+        <v>1589</v>
       </c>
       <c r="C31" s="11" t="s">
         <v>1519</v>
       </c>
-      <c r="D31" s="14" t="n">
+      <c r="D31" s="12" t="s">
+        <v>560</v>
+      </c>
+      <c r="E31" s="14" t="n">
         <v>-21990.38</v>
       </c>
-      <c r="E31" s="12" t="s">
-        <v>560</v>
+      <c r="F31" s="14" t="s">
+        <v>1529</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="12" t="s">
-        <v>1589</v>
+        <v>1590</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>1590</v>
+        <v>1591</v>
       </c>
       <c r="C32" s="11" t="s">
         <v>1519</v>
       </c>
-      <c r="D32" s="14" t="n">
+      <c r="D32" s="12" t="s">
+        <v>566</v>
+      </c>
+      <c r="E32" s="14" t="n">
         <v>1066339</v>
       </c>
-      <c r="E32" s="12" t="s">
-        <v>566</v>
+      <c r="F32" s="14" t="s">
+        <v>1529</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="12" t="s">
-        <v>1591</v>
+        <v>1592</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>1592</v>
+        <v>1593</v>
       </c>
       <c r="C33" s="11" t="s">
         <v>1519</v>
       </c>
-      <c r="D33" s="14" t="n">
+      <c r="D33" s="12" t="s">
+        <v>572</v>
+      </c>
+      <c r="E33" s="14" t="n">
         <v>-1132896</v>
       </c>
-      <c r="E33" s="12" t="s">
-        <v>572</v>
+      <c r="F33" s="14" t="s">
+        <v>1529</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="12" t="s">
-        <v>1593</v>
+        <v>1594</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="C34" s="11" t="s">
         <v>1519</v>
       </c>
-      <c r="D34" s="14" t="n">
+      <c r="D34" s="12" t="s">
+        <v>574</v>
+      </c>
+      <c r="E34" s="14" t="n">
         <v>-33790.38</v>
       </c>
-      <c r="E34" s="12" t="s">
-        <v>574</v>
+      <c r="F34" s="14" t="s">
+        <v>1529</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="12" t="s">
-        <v>1595</v>
+        <v>1596</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>1578</v>
+        <v>1579</v>
       </c>
       <c r="C35" s="11" t="s">
         <v>1522</v>
       </c>
-      <c r="D35" s="14" t="n">
+      <c r="D35" s="12" t="s">
+        <v>520</v>
+      </c>
+      <c r="E35" s="14" t="n">
         <v>4381069</v>
       </c>
-      <c r="E35" s="12" t="s">
-        <v>520</v>
+      <c r="F35" s="14" t="s">
+        <v>1529</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="12" t="s">
-        <v>1596</v>
+        <v>1597</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>1590</v>
+        <v>1591</v>
       </c>
       <c r="C36" s="11" t="s">
         <v>1522</v>
       </c>
-      <c r="D36" s="14" t="n">
+      <c r="D36" s="12" t="s">
+        <v>566</v>
+      </c>
+      <c r="E36" s="14" t="n">
         <v>1066339</v>
       </c>
-      <c r="E36" s="12" t="s">
-        <v>566</v>
+      <c r="F36" s="14" t="s">
+        <v>1529</v>
       </c>
     </row>
   </sheetData>
@@ -15335,7 +15445,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
-      <selection pane="bottomRight" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="bottomRight" activeCell="G1" activeCellId="1" sqref="F2:F36 G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -15354,7 +15464,7 @@
         <v>35</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1597</v>
+        <v>1526</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>581</v>
@@ -15394,7 +15504,7 @@
         <v>1601</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16094,7 +16204,7 @@
         <v>1671</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>1530</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16139,7 +16249,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomRight" activeCell="E1" activeCellId="1" sqref="F2:F36 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -16215,7 +16325,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="bottomRight" activeCell="D8" activeCellId="1" sqref="F2:F36 D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -16233,7 +16343,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>1597</v>
+        <v>1526</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>581</v>
@@ -16459,7 +16569,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M23" activeCellId="0" sqref="M23"/>
+      <selection pane="bottomRight" activeCell="M23" activeCellId="1" sqref="F2:F36 M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -17258,7 +17368,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B23" activeCellId="0" sqref="B23"/>
+      <selection pane="topRight" activeCell="B23" activeCellId="1" sqref="F2:F36 B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -17333,7 +17443,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomRight" activeCell="E1" activeCellId="1" sqref="F2:F36 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -17450,12 +17560,12 @@
   </sheetPr>
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="bottomRight" activeCell="E8" activeCellId="1" sqref="F2:F36 E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -17581,7 +17691,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="bottomRight" activeCell="I1" activeCellId="1" sqref="F2:F36 I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -21179,7 +21289,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="bottomRight" activeCell="F1" activeCellId="1" sqref="F2:F36 F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -23338,7 +23448,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="C2" activeCellId="1" sqref="F2:F36 C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -26159,7 +26269,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomRight" activeCell="E1" activeCellId="1" sqref="F2:F36 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -26263,7 +26373,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomRight" activeCell="E1" activeCellId="1" sqref="F2:F36 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>

</xml_diff>

<commit_message>
adding stop condition units
</commit_message>
<xml_diff>
--- a/tests/fixtures/example-model.xlsx
+++ b/tests/fixtures/example-model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -30,8 +30,8 @@
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">Compartments!$A$1:$J$3</definedName>
     <definedName function="false" hidden="true" localSheetId="6" name="_xlnm._FilterDatabase" vbProcedure="false">Concentrations!$C$1:$J$126</definedName>
-    <definedName function="false" hidden="true" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="true" localSheetId="11" name="_xlnm._FilterDatabase" vbProcedure="false">'Rate laws'!$C$1:$K$168</definedName>
+    <definedName function="false" hidden="true" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$I$37</definedName>
+    <definedName function="false" hidden="true" localSheetId="11" name="_xlnm._FilterDatabase" vbProcedure="false">'Rate laws'!$A$1:$K$168</definedName>
     <definedName function="false" hidden="true" localSheetId="10" name="_xlnm._FilterDatabase" vbProcedure="false">Reactions!$A$1:$L$176</definedName>
     <definedName function="false" hidden="true" localSheetId="17" name="_xlnm._FilterDatabase" vbProcedure="false">References!$A$1:$R$20</definedName>
     <definedName function="false" hidden="true" localSheetId="4" name="_xlnm._FilterDatabase" vbProcedure="false">'Species types'!$A$1:$K$144</definedName>
@@ -119,6 +119,7 @@
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Submodels!$A$1:$G$5</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Submodels!$A$1:$G$5</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Submodels!$A$1:$G$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Submodels!$A$1:$G$5</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0" vbProcedure="false">Compartments!$A$1:$J$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0" vbProcedure="false">Compartments!$A$1:$J$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_FilterDatabase_0_0_0" vbProcedure="false">Compartments!$A$1:$J$3</definedName>
@@ -162,6 +163,7 @@
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$J$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$J$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$J$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Compartments!$A$1:$J$3</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0" vbProcedure="false">'Species types'!$A$1:$K$144</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0" vbProcedure="false">'Species types'!$A$1:$K$144</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_FilterDatabase_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$144</definedName>
@@ -205,6 +207,7 @@
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$144</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$144</definedName>
     <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$144</definedName>
+    <definedName function="false" hidden="false" localSheetId="4" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Species types'!$A$1:$K$144</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_FilterDatabase_0" vbProcedure="false">Concentrations!$C$1:$J$126</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_FilterDatabase_0_0" vbProcedure="false">Concentrations!$C$1:$J$126</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_FilterDatabase_0_0_0" vbProcedure="false">Concentrations!$C$1:$J$126</definedName>
@@ -248,6 +251,7 @@
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Concentrations!$C$1:$J$126</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Concentrations!$C$1:$J$126</definedName>
     <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Concentrations!$C$1:$J$126</definedName>
+    <definedName function="false" hidden="false" localSheetId="6" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Concentrations!$C$1:$J$126</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0" vbProcedure="false">Reactions!$A$1:$L$176</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0" vbProcedure="false">Reactions!$A$1:$L$176</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_FilterDatabase_0_0_0" vbProcedure="false">Reactions!$A$1:$L$176</definedName>
@@ -291,6 +295,7 @@
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$L$176</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$L$176</definedName>
     <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$L$176</definedName>
+    <definedName function="false" hidden="false" localSheetId="10" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Reactions!$A$1:$L$176</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_FilterDatabase_0" vbProcedure="false">'Rate laws'!$C$1:$K$168</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_FilterDatabase_0_0" vbProcedure="false">'Rate laws'!$C$1:$K$168</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_FilterDatabase_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$K$168</definedName>
@@ -299,22 +304,22 @@
     <definedName function="false" hidden="false" localSheetId="11" name="_FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$K$168</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$K$168</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$K$168</definedName>
-    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase" vbProcedure="false">'Rate laws'!$A$1:$K$168</definedName>
-    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Rate laws'!$C$1:$K$168</definedName>
-    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Rate laws'!$A$1:$K$168</definedName>
-    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$K$168</definedName>
-    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Rate laws'!$A$1:$K$168</definedName>
-    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$K$168</definedName>
-    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$A$1:$K$168</definedName>
-    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$K$168</definedName>
-    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$A$1:$K$168</definedName>
-    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$K$168</definedName>
-    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$A$1:$K$168</definedName>
-    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$K$168</definedName>
-    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$A$1:$K$168</definedName>
-    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$K$168</definedName>
-    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$A$1:$K$168</definedName>
-    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$K$168</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase" vbProcedure="false">'Rate laws'!$C$1:$K$168</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Rate laws'!$A$1:$K$168</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Rate laws'!$C$1:$K$168</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'Rate laws'!$A$1:$K$168</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$K$168</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'Rate laws'!$A$1:$K$168</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$K$168</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$A$1:$K$168</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$K$168</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$A$1:$K$168</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$K$168</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$A$1:$K$168</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$K$168</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$A$1:$K$168</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$K$168</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$A$1:$K$168</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$K$168</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$K$168</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$K$168</definedName>
@@ -334,6 +339,7 @@
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$K$168</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$K$168</definedName>
     <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$K$168</definedName>
+    <definedName function="false" hidden="false" localSheetId="11" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Rate laws'!$C$1:$K$168</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$I$6</definedName>
@@ -342,22 +348,22 @@
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$I$37</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$I$37</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Parameters!$A$1:$I$37</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$I$37</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$I$37</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$I$37</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$I$37</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$I$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$I$37</definedName>
-    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase" vbProcedure="false">Parameters!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0" vbProcedure="false">Parameters!$A$1:$I$37</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Parameters!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Parameters!$A$1:$I$37</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Parameters!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$I$37</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$I$37</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$I$37</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$I$37</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$I$37</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$I$37</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$I$6</definedName>
@@ -377,6 +383,7 @@
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$I$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="14" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Parameters!$A$1:$I$6</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_FilterDatabase_0" vbProcedure="false">References!$A$1:$R$20</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_FilterDatabase_0_0" vbProcedure="false">References!$A$1:$R$20</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_FilterDatabase_0_0_0" vbProcedure="false">References!$A$1:$R$20</definedName>
@@ -420,6 +427,7 @@
     <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$R$20</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$R$20</definedName>
     <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$R$20</definedName>
+    <definedName function="false" hidden="false" localSheetId="17" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">References!$A$1:$R$20</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -431,7 +439,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3968" uniqueCount="1844">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3971" uniqueCount="1844">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -6263,13 +6271,13 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topRight" activeCell="A12" activeCellId="1" sqref="D3 A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="49.0607287449393"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="49.4898785425101"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -6401,14 +6409,14 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="bottomRight" activeCell="F1" activeCellId="1" sqref="D3 F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="21.7449392712551"/>
     <col collapsed="false" hidden="false" max="3" min="2" style="3" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="45.417004048583"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="45.8461538461538"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="3" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -6467,20 +6475,20 @@
   </sheetPr>
   <dimension ref="A1:L176"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H2" activeCellId="0" sqref="H2"/>
+      <selection pane="bottomRight" activeCell="H2" activeCellId="1" sqref="D3 H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="33.2064777327935"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="33.5263157894737"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="62.8785425101215"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="63.412955465587"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="1" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -10713,7 +10721,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A140" activeCellId="0" sqref="A140"/>
-      <selection pane="bottomRight" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="bottomRight" activeCell="I1" activeCellId="1" sqref="D3 I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -14765,7 +14773,7 @@
       <c r="K168" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="C1:K168"/>
+  <autoFilter ref="A1:K168"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -14789,13 +14797,13 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="bottomRight" activeCell="D9" activeCellId="1" sqref="D3 D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="19.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="10" width="19.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="10" width="25.6032388663968"/>
     <col collapsed="false" hidden="false" max="6" min="3" style="10" width="11.246963562753"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="10" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1022" min="8" style="10" width="8.78542510121457"/>
@@ -14876,14 +14884,14 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A27" activeCellId="0" sqref="A27"/>
-      <selection pane="bottomRight" activeCell="F2" activeCellId="0" sqref="F2"/>
+      <selection pane="bottomRight" activeCell="F2" activeCellId="1" sqref="D3 F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="12" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="12" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="12" width="20.246963562753"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="12" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="12" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="12" width="9.10526315789474"/>
@@ -15655,7 +15663,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
-      <selection pane="bottomRight" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="bottomRight" activeCell="G1" activeCellId="1" sqref="D3 G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -16435,7 +16443,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I6"/>
+  <autoFilter ref="A1:I37"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -16452,14 +16460,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomRight" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -16478,15 +16486,18 @@
         <v>714</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>26</v>
       </c>
     </row>
@@ -16498,8 +16509,11 @@
       <c r="C2" s="3" t="s">
         <v>724</v>
       </c>
-      <c r="D2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>1609</v>
+      </c>
       <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="15.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
@@ -16509,8 +16523,11 @@
       <c r="C3" s="3" t="s">
         <v>726</v>
       </c>
-      <c r="D3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>1609</v>
+      </c>
       <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -16535,12 +16552,12 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="bottomRight" activeCell="D8" activeCellId="1" sqref="D3 D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="3" width="13.2834008097166"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="3" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="3" width="9.10526315789474"/>
   </cols>
@@ -16779,7 +16796,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M23" activeCellId="0" sqref="M23"/>
+      <selection pane="bottomRight" activeCell="M23" activeCellId="1" sqref="D3 M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -17578,13 +17595,13 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B23" activeCellId="0" sqref="B23"/>
+      <selection pane="topRight" activeCell="B23" activeCellId="1" sqref="D3 B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="28.7085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="1" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -17653,7 +17670,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomRight" activeCell="E1" activeCellId="1" sqref="D3 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -17775,7 +17792,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E8" activeCellId="0" sqref="E8"/>
+      <selection pane="bottomRight" activeCell="E8" activeCellId="1" sqref="D3 E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -17901,12 +17918,12 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="bottomRight" activeCell="I1" activeCellId="1" sqref="D3 I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.4939271255061"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -21499,12 +21516,12 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="bottomRight" activeCell="F1" activeCellId="1" sqref="D3 F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.6356275303644"/>
     <col collapsed="false" hidden="false" max="8" min="2" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="9.10526315789474"/>
   </cols>
@@ -23658,14 +23675,14 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="C2" activeCellId="1" sqref="D3 C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="29.9919028340081"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="29.7773279352227"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="29.9919028340081"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -26479,13 +26496,13 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomRight" activeCell="E1" activeCellId="1" sqref="D3 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="1" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="36.8502024291498"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="37.17004048583"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="8.78542510121457"/>
   </cols>
   <sheetData>
@@ -26583,13 +26600,13 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomRight" activeCell="E1" activeCellId="1" sqref="D3 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="1" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.8178137651822"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.9230769230769"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="1" width="8.78542510121457"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
testing compartment evalation in expressions; adding species to StopConditionExpression.valid_models; renaming RateLawExpression.modifiers to RateLawExpression.species
</commit_message>
<xml_diff>
--- a/tests/fixtures/example-model.xlsx
+++ b/tests/fixtures/example-model.xlsx
@@ -1709,7 +1709,7 @@
     <t xml:space="preserve">AD[c]</t>
   </si>
   <si>
-    <t xml:space="preserve">molecule cell^-1</t>
+    <t xml:space="preserve">molecule</t>
   </si>
   <si>
     <t xml:space="preserve">AD[e]</t>
@@ -4301,7 +4301,7 @@
     <t xml:space="preserve">k_cat_rev_ak * func_1() * AXP_c * Adk_Protein[c]</t>
   </si>
   <si>
-    <t xml:space="preserve">reaction cell^-1 s^-1</t>
+    <t xml:space="preserve">reaction s^-1</t>
   </si>
   <si>
     <t xml:space="preserve">AK_AMP-forward</t>
@@ -5813,7 +5813,7 @@
     <t xml:space="preserve">k_cat_rev_ak</t>
   </si>
   <si>
-    <t xml:space="preserve">reaction molecule^-2 cell s^-1</t>
+    <t xml:space="preserve">reaction molecule^-2 s^-1</t>
   </si>
   <si>
     <t xml:space="preserve">k_cat_rev_aprt</t>
@@ -15847,11 +15847,11 @@
   <dimension ref="A1:J93"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B45" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B49" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
-      <selection pane="bottomRight" activeCell="F61" activeCellId="0" sqref="F61"/>
+      <selection pane="bottomLeft" activeCell="A49" activeCellId="0" sqref="A49"/>
+      <selection pane="bottomRight" activeCell="I71" activeCellId="0" sqref="I71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -22607,11 +22607,11 @@
   <dimension ref="A1:I176"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B150" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A150" activeCellId="0" sqref="A150"/>
-      <selection pane="bottomRight" activeCell="E150" activeCellId="0" sqref="E150"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -28119,7 +28119,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H32" activeCellId="0" sqref="H32"/>
+      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>

</xml_diff>

<commit_message>
removing () suffix from functions in expressions
</commit_message>
<xml_diff>
--- a/tests/fixtures/example-model.xlsx
+++ b/tests/fixtures/example-model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="14"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" state="visible" r:id="rId2"/>
@@ -4298,7 +4298,7 @@
     <t xml:space="preserve">other</t>
   </si>
   <si>
-    <t xml:space="preserve">k_cat_rev_ak * func_1() * AXP_c * Adk_Protein[c]</t>
+    <t xml:space="preserve">k_cat_rev_ak * func_1 * AXP_c * Adk_Protein[c]</t>
   </si>
   <si>
     <t xml:space="preserve">reaction s^-1</t>
@@ -11221,12 +11221,12 @@
   </sheetPr>
   <dimension ref="A1:K168"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F4" activeCellId="0" sqref="F4"/>
+      <selection pane="bottomRight" activeCell="F3" activeCellId="0" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -15846,12 +15846,12 @@
   </sheetPr>
   <dimension ref="A1:J93"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B49" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A49" activeCellId="0" sqref="A49"/>
-      <selection pane="bottomRight" activeCell="I71" activeCellId="0" sqref="I71"/>
+      <selection pane="bottomRight" activeCell="K80" activeCellId="0" sqref="K80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
simplifying dFBA flux units to facilitate composability
</commit_message>
<xml_diff>
--- a/tests/fixtures/example-model.xlsx
+++ b/tests/fixtures/example-model.xlsx
@@ -390,7 +390,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4550" uniqueCount="2011">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4552" uniqueCount="2012">
   <si>
     <t>Id</t>
   </si>
@@ -5162,6 +5162,9 @@
   </si>
   <si>
     <t>k_cat_for_val_abc * PeptAbcTransporter_Protein[c]</t>
+  </si>
+  <si>
+    <t>Reaction rate units</t>
   </si>
   <si>
     <t>Coefficient units</t>
@@ -6433,10 +6436,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -6483,6 +6486,13 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -6491,16 +6501,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6508,21 +6510,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6552,22 +6539,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -6582,6 +6553,52 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
@@ -6590,21 +6607,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6633,19 +6636,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6663,7 +6666,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6675,25 +6756,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6705,37 +6786,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6747,73 +6816,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6842,15 +6845,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -6866,6 +6860,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -6877,17 +6886,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -6910,8 +6913,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -6919,140 +6922,140 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -7641,11 +7644,11 @@
   <dimension ref="A1:L176"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -15619,14 +15622,14 @@
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
@@ -15634,10 +15637,10 @@
     <col min="1" max="1" width="22.6" style="3"/>
     <col min="2" max="3" width="9.10833333333333" style="3"/>
     <col min="4" max="4" width="47.5666666666667" style="3"/>
-    <col min="5" max="1026" width="9.10833333333333" style="3"/>
+    <col min="5" max="1027" width="9.10833333333333" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.1" customHeight="1" spans="1:10">
+    <row r="1" ht="15.1" customHeight="1" spans="1:11">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -15657,32 +15660,38 @@
         <v>1590</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>1591</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:6">
+    <row r="2" ht="15.1" customHeight="1" spans="1:7">
       <c r="A2" s="3" t="s">
-        <v>1591</v>
+        <v>1592</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>1592</v>
+        <v>1593</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>742</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>1284</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -15732,7 +15741,7 @@
         <v>420</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>1593</v>
+        <v>1594</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>18</v>
@@ -15749,10 +15758,10 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:8">
       <c r="A2" s="9" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>1595</v>
+        <v>1596</v>
       </c>
       <c r="C2" s="11" t="s">
         <v>29</v>
@@ -15764,15 +15773,15 @@
         <v>56</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>1596</v>
+        <v>1597</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:8">
       <c r="A3" s="9" t="s">
-        <v>1597</v>
+        <v>1598</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>1598</v>
+        <v>1599</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>29</v>
@@ -15784,7 +15793,7 @@
         <v>56</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>1599</v>
+        <v>1600</v>
       </c>
     </row>
   </sheetData>
@@ -15830,13 +15839,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>1600</v>
+        <v>1601</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>597</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>1601</v>
+        <v>1602</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>420</v>
@@ -15856,13 +15865,13 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:10">
       <c r="A2" s="7" t="s">
-        <v>1602</v>
+        <v>1603</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>1603</v>
+        <v>1604</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>427</v>
@@ -15871,24 +15880,24 @@
         <v>-34190.38</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>1605</v>
+        <v>1606</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>1606</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:6">
       <c r="A3" s="7" t="s">
-        <v>1607</v>
+        <v>1608</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>1608</v>
+        <v>1609</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>430</v>
@@ -15897,18 +15906,18 @@
         <v>1035619</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:6">
       <c r="A4" s="7" t="s">
-        <v>1609</v>
+        <v>1610</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>1610</v>
+        <v>1611</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>433</v>
@@ -15917,18 +15926,18 @@
         <v>-40890.38</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:6">
       <c r="A5" s="7" t="s">
-        <v>1611</v>
+        <v>1612</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>1612</v>
+        <v>1613</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>436</v>
@@ -15937,18 +15946,18 @@
         <v>-23190.38</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:6">
       <c r="A6" s="7" t="s">
-        <v>1613</v>
+        <v>1614</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>1614</v>
+        <v>1615</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>439</v>
@@ -15957,18 +15966,18 @@
         <v>-24290.38</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:6">
       <c r="A7" s="7" t="s">
-        <v>1615</v>
+        <v>1616</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>1616</v>
+        <v>1617</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>442</v>
@@ -15977,18 +15986,18 @@
         <v>-1101856</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:6">
       <c r="A8" s="7" t="s">
-        <v>1617</v>
+        <v>1618</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>1618</v>
+        <v>1619</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>446</v>
@@ -15997,18 +16006,18 @@
         <v>1098019</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="9" ht="15.1" customHeight="1" spans="1:6">
       <c r="A9" s="7" t="s">
-        <v>1619</v>
+        <v>1620</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>1620</v>
+        <v>1621</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>449</v>
@@ -16017,18 +16026,18 @@
         <v>-1164906</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="10" ht="15.1" customHeight="1" spans="1:6">
       <c r="A10" s="7" t="s">
-        <v>1621</v>
+        <v>1622</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>1622</v>
+        <v>1623</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>450</v>
@@ -16037,18 +16046,18 @@
         <v>-22290.38</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="11" ht="15.1" customHeight="1" spans="1:6">
       <c r="A11" s="7" t="s">
-        <v>1623</v>
+        <v>1624</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>1624</v>
+        <v>1625</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>468</v>
@@ -16057,18 +16066,18 @@
         <v>581419.2</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="12" ht="15.1" customHeight="1" spans="1:6">
       <c r="A12" s="7" t="s">
-        <v>1625</v>
+        <v>1626</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>1626</v>
+        <v>1627</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>472</v>
@@ -16077,18 +16086,18 @@
         <v>-24690.38</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="13" ht="15.1" customHeight="1" spans="1:6">
       <c r="A13" s="7" t="s">
-        <v>1627</v>
+        <v>1628</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>1628</v>
+        <v>1629</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>475</v>
@@ -16097,18 +16106,18 @@
         <v>-22690.38</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="14" ht="15.1" customHeight="1" spans="1:6">
       <c r="A14" s="7" t="s">
-        <v>1629</v>
+        <v>1630</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>1630</v>
+        <v>1631</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>478</v>
@@ -16117,18 +16126,18 @@
         <v>-31190.38</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="15" ht="15.1" customHeight="1" spans="1:6">
       <c r="A15" s="7" t="s">
-        <v>1631</v>
+        <v>1632</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>1632</v>
+        <v>1633</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>481</v>
@@ -16137,18 +16146,18 @@
         <v>1052899</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="16" ht="15.1" customHeight="1" spans="1:6">
       <c r="A16" s="7" t="s">
-        <v>1633</v>
+        <v>1634</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>1634</v>
+        <v>1635</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>484</v>
@@ -16157,18 +16166,18 @@
         <v>-1728316</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="17" ht="15.1" customHeight="1" spans="1:6">
       <c r="A17" s="7" t="s">
-        <v>1635</v>
+        <v>1636</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>1636</v>
+        <v>1637</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>485</v>
@@ -16177,18 +16186,18 @@
         <v>-1521617000</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="18" ht="15.1" customHeight="1" spans="1:6">
       <c r="A18" s="7" t="s">
-        <v>1637</v>
+        <v>1638</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>1638</v>
+        <v>1639</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>487</v>
@@ -16197,18 +16206,18 @@
         <v>4972350</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="19" ht="15.1" customHeight="1" spans="1:6">
       <c r="A19" s="7" t="s">
-        <v>1639</v>
+        <v>1640</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>1640</v>
+        <v>1641</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>489</v>
@@ -16217,18 +16226,18 @@
         <v>-21590.38</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="20" ht="15.1" customHeight="1" spans="1:6">
       <c r="A20" s="7" t="s">
-        <v>1641</v>
+        <v>1642</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>1642</v>
+        <v>1643</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>494</v>
@@ -16237,18 +16246,18 @@
         <v>-29290.38</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="21" ht="15.1" customHeight="1" spans="1:6">
       <c r="A21" s="7" t="s">
-        <v>1643</v>
+        <v>1644</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>1644</v>
+        <v>1645</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>503</v>
@@ -16257,18 +16266,18 @@
         <v>-41190.38</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="22" ht="15.1" customHeight="1" spans="1:6">
       <c r="A22" s="7" t="s">
-        <v>1645</v>
+        <v>1646</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>1646</v>
+        <v>1647</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>506</v>
@@ -16277,18 +16286,18 @@
         <v>-21990.38</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="23" ht="15.1" customHeight="1" spans="1:6">
       <c r="A23" s="7" t="s">
-        <v>1647</v>
+        <v>1648</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>1648</v>
+        <v>1649</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>509</v>
@@ -16297,18 +16306,18 @@
         <v>-21390.38</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="24" ht="15.1" customHeight="1" spans="1:6">
       <c r="A24" s="7" t="s">
-        <v>1649</v>
+        <v>1650</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>1650</v>
+        <v>1651</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>530</v>
@@ -16317,18 +16326,18 @@
         <v>-23890.38</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="25" ht="15.1" customHeight="1" spans="1:6">
       <c r="A25" s="7" t="s">
-        <v>1651</v>
+        <v>1652</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>1652</v>
+        <v>1653</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>533</v>
@@ -16337,18 +16346,18 @@
         <v>471096.2</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="26" ht="15.1" customHeight="1" spans="1:6">
       <c r="A26" s="7" t="s">
-        <v>1653</v>
+        <v>1654</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>1654</v>
+        <v>1655</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>539</v>
@@ -16357,18 +16366,18 @@
         <v>4381069</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="27" ht="15.1" customHeight="1" spans="1:6">
       <c r="A27" s="7" t="s">
-        <v>1655</v>
+        <v>1656</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>1656</v>
+        <v>1657</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>540</v>
@@ -16377,18 +16386,18 @@
         <v>-34390.38</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="28" ht="15.1" customHeight="1" spans="1:6">
       <c r="A28" s="7" t="s">
-        <v>1657</v>
+        <v>1658</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>1658</v>
+        <v>1659</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>564</v>
@@ -16397,18 +16406,18 @@
         <v>-44490.38</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="29" ht="15.1" customHeight="1" spans="1:6">
       <c r="A29" s="7" t="s">
-        <v>1659</v>
+        <v>1660</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>1660</v>
+        <v>1661</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>569</v>
@@ -16417,18 +16426,18 @@
         <v>-36190.38</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="30" ht="15.1" customHeight="1" spans="1:6">
       <c r="A30" s="7" t="s">
-        <v>1661</v>
+        <v>1662</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>1662</v>
+        <v>1663</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>576</v>
@@ -16437,18 +16446,18 @@
         <v>-22190.38</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="31" ht="15.1" customHeight="1" spans="1:6">
       <c r="A31" s="7" t="s">
-        <v>1663</v>
+        <v>1664</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>1664</v>
+        <v>1665</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D31" s="7" t="s">
         <v>579</v>
@@ -16457,18 +16466,18 @@
         <v>-21990.38</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="32" ht="15.1" customHeight="1" spans="1:6">
       <c r="A32" s="7" t="s">
-        <v>1665</v>
+        <v>1666</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>1666</v>
+        <v>1667</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D32" s="7" t="s">
         <v>585</v>
@@ -16477,18 +16486,18 @@
         <v>1066339</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="33" ht="15.1" customHeight="1" spans="1:6">
       <c r="A33" s="7" t="s">
-        <v>1667</v>
+        <v>1668</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>1668</v>
+        <v>1669</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>591</v>
@@ -16497,18 +16506,18 @@
         <v>-1132896</v>
       </c>
       <c r="F33" s="10" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="34" ht="15.1" customHeight="1" spans="1:6">
       <c r="A34" s="7" t="s">
-        <v>1669</v>
+        <v>1670</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>1670</v>
+        <v>1671</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>1594</v>
+        <v>1595</v>
       </c>
       <c r="D34" s="7" t="s">
         <v>593</v>
@@ -16517,18 +16526,18 @@
         <v>-33790.38</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="35" ht="15.1" customHeight="1" spans="1:6">
       <c r="A35" s="7" t="s">
-        <v>1671</v>
+        <v>1672</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>1654</v>
+        <v>1655</v>
       </c>
       <c r="C35" s="9" t="s">
-        <v>1597</v>
+        <v>1598</v>
       </c>
       <c r="D35" s="7" t="s">
         <v>539</v>
@@ -16537,18 +16546,18 @@
         <v>4381069</v>
       </c>
       <c r="F35" s="10" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="36" ht="15.1" customHeight="1" spans="1:6">
       <c r="A36" s="7" t="s">
-        <v>1672</v>
+        <v>1673</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>1666</v>
+        <v>1667</v>
       </c>
       <c r="C36" s="9" t="s">
-        <v>1597</v>
+        <v>1598</v>
       </c>
       <c r="D36" s="7" t="s">
         <v>585</v>
@@ -16557,7 +16566,7 @@
         <v>1066339</v>
       </c>
       <c r="F36" s="10" t="s">
-        <v>1604</v>
+        <v>1605</v>
       </c>
     </row>
   </sheetData>
@@ -16597,10 +16606,10 @@
         <v>69</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1601</v>
+        <v>1602</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>1673</v>
+        <v>1674</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>420</v>
@@ -16620,10 +16629,10 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:10">
       <c r="A2" s="3" t="s">
-        <v>1674</v>
+        <v>1675</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1675</v>
+        <v>1676</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>1282</v>
@@ -16632,23 +16641,23 @@
         <v>12</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1676</v>
+        <v>1677</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="3" t="s">
-        <v>1677</v>
+        <v>1678</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>1606</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:10">
       <c r="A3" s="3" t="s">
-        <v>1678</v>
+        <v>1679</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1679</v>
+        <v>1680</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>1282</v>
@@ -16666,10 +16675,10 @@
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:10">
       <c r="A4" s="3" t="s">
-        <v>1680</v>
+        <v>1681</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1681</v>
+        <v>1682</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>1282</v>
@@ -16684,12 +16693,12 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="3" t="s">
-        <v>1682</v>
+        <v>1683</v>
       </c>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:10">
       <c r="A5" s="3" t="s">
-        <v>1683</v>
+        <v>1684</v>
       </c>
       <c r="B5"/>
       <c r="C5" s="3" t="s">
@@ -16706,7 +16715,7 @@
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:10">
       <c r="A6" s="3" t="s">
-        <v>1684</v>
+        <v>1685</v>
       </c>
       <c r="B6"/>
       <c r="C6" s="3" t="s">
@@ -16723,1519 +16732,1519 @@
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:10">
       <c r="A7" s="3" t="s">
-        <v>1685</v>
+        <v>1686</v>
       </c>
       <c r="B7"/>
       <c r="C7" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D7" s="3">
         <v>1</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I7"/>
       <c r="J7"/>
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:10">
       <c r="A8" s="3" t="s">
-        <v>1688</v>
+        <v>1689</v>
       </c>
       <c r="B8"/>
       <c r="C8" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D8" s="3">
         <v>1</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I8"/>
       <c r="J8"/>
     </row>
     <row r="9" ht="15.1" customHeight="1" spans="1:10">
       <c r="A9" s="3" t="s">
-        <v>1689</v>
+        <v>1690</v>
       </c>
       <c r="B9"/>
       <c r="C9" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D9" s="3">
         <v>1</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I9"/>
       <c r="J9"/>
     </row>
     <row r="10" ht="15.1" customHeight="1" spans="1:10">
       <c r="A10" s="3" t="s">
-        <v>1690</v>
+        <v>1691</v>
       </c>
       <c r="B10"/>
       <c r="C10" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D10" s="3">
         <v>1</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I10"/>
       <c r="J10"/>
     </row>
     <row r="11" ht="15.1" customHeight="1" spans="1:10">
       <c r="A11" s="3" t="s">
-        <v>1691</v>
+        <v>1692</v>
       </c>
       <c r="B11"/>
       <c r="C11" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D11" s="3">
         <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I11"/>
       <c r="J11"/>
     </row>
     <row r="12" ht="15.1" customHeight="1" spans="1:10">
       <c r="A12" s="3" t="s">
-        <v>1692</v>
+        <v>1693</v>
       </c>
       <c r="B12"/>
       <c r="C12" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D12" s="3">
         <v>1</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I12"/>
       <c r="J12"/>
     </row>
     <row r="13" ht="15.1" customHeight="1" spans="1:10">
       <c r="A13" s="3" t="s">
-        <v>1693</v>
+        <v>1694</v>
       </c>
       <c r="B13"/>
       <c r="C13" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D13" s="3">
         <v>1</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I13"/>
       <c r="J13"/>
     </row>
     <row r="14" ht="15.1" customHeight="1" spans="1:10">
       <c r="A14" s="3" t="s">
-        <v>1694</v>
+        <v>1695</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>1695</v>
+        <v>1696</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D14" s="3">
         <v>250</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I14"/>
       <c r="J14" s="3" t="s">
-        <v>1696</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="15" ht="15.1" customHeight="1" spans="1:10">
       <c r="A15" s="3" t="s">
-        <v>1697</v>
+        <v>1698</v>
       </c>
       <c r="B15"/>
       <c r="C15" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D15" s="3">
         <v>1</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I15"/>
       <c r="J15"/>
     </row>
     <row r="16" ht="15.1" customHeight="1" spans="1:10">
       <c r="A16" s="3" t="s">
-        <v>1698</v>
+        <v>1699</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>1699</v>
+        <v>1700</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D16" s="3">
         <v>180</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I16"/>
       <c r="J16" s="3" t="s">
-        <v>1696</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="17" ht="15.1" customHeight="1" spans="1:10">
       <c r="A17" s="3" t="s">
-        <v>1700</v>
+        <v>1701</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>1701</v>
+        <v>1702</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D17" s="3">
         <v>1005.6</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>1702</v>
+        <v>1703</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>1703</v>
+        <v>1704</v>
       </c>
     </row>
     <row r="18" ht="15.1" customHeight="1" spans="1:10">
       <c r="A18" s="3" t="s">
-        <v>1704</v>
+        <v>1705</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>1705</v>
+        <v>1706</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D18" s="3">
         <v>4200</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>1706</v>
+        <v>1707</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>1707</v>
+        <v>1708</v>
       </c>
     </row>
     <row r="19" ht="15.1" customHeight="1" spans="1:10">
       <c r="A19" s="3" t="s">
-        <v>1708</v>
+        <v>1709</v>
       </c>
       <c r="B19"/>
       <c r="C19" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D19" s="3">
         <v>1</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I19"/>
       <c r="J19"/>
     </row>
     <row r="20" ht="15.1" customHeight="1" spans="1:10">
       <c r="A20" s="3" t="s">
-        <v>1709</v>
+        <v>1710</v>
       </c>
       <c r="B20"/>
       <c r="C20" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D20" s="3">
         <v>1</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I20"/>
       <c r="J20"/>
     </row>
     <row r="21" ht="15.1" customHeight="1" spans="1:10">
       <c r="A21" s="3" t="s">
-        <v>1710</v>
+        <v>1711</v>
       </c>
       <c r="B21"/>
       <c r="C21" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D21" s="3">
         <v>1</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I21"/>
       <c r="J21"/>
     </row>
     <row r="22" ht="15.1" customHeight="1" spans="1:10">
       <c r="A22" s="3" t="s">
-        <v>1711</v>
+        <v>1712</v>
       </c>
       <c r="B22"/>
       <c r="C22" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D22" s="3">
         <v>1</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I22"/>
       <c r="J22"/>
     </row>
     <row r="23" ht="15.1" customHeight="1" spans="1:10">
       <c r="A23" s="3" t="s">
-        <v>1712</v>
+        <v>1713</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>1713</v>
+        <v>1714</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D23" s="3">
         <v>13200</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>1714</v>
+        <v>1715</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>1696</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="24" ht="15.1" customHeight="1" spans="1:10">
       <c r="A24" s="3" t="s">
-        <v>1715</v>
+        <v>1716</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>1716</v>
+        <v>1717</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D24" s="3">
         <v>0.276</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>1717</v>
+        <v>1718</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>1696</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="25" ht="15.1" customHeight="1" spans="1:10">
       <c r="A25" s="3" t="s">
-        <v>1718</v>
+        <v>1719</v>
       </c>
       <c r="B25"/>
       <c r="C25" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D25" s="3">
         <v>1</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I25"/>
       <c r="J25"/>
     </row>
     <row r="26" ht="15.1" customHeight="1" spans="1:10">
       <c r="A26" s="3" t="s">
-        <v>1719</v>
+        <v>1720</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>1720</v>
+        <v>1721</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D26" s="3">
         <v>628.8</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>1721</v>
+        <v>1722</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>1696</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="27" ht="15.1" customHeight="1" spans="1:10">
       <c r="A27" s="3" t="s">
-        <v>1722</v>
+        <v>1723</v>
       </c>
       <c r="B27"/>
       <c r="C27" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D27" s="3">
         <v>1</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I27"/>
       <c r="J27"/>
     </row>
     <row r="28" ht="15.1" customHeight="1" spans="1:10">
       <c r="A28" s="3" t="s">
-        <v>1723</v>
+        <v>1724</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>1724</v>
+        <v>1725</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D28" s="3">
         <v>4140</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>1725</v>
+        <v>1726</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>1696</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="29" ht="15.1" customHeight="1" spans="1:10">
       <c r="A29" s="3" t="s">
-        <v>1726</v>
+        <v>1727</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>1727</v>
+        <v>1728</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D29" s="3">
         <v>220</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>1728</v>
+        <v>1729</v>
       </c>
       <c r="J29" s="3" t="s">
-        <v>1696</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="30" ht="15.1" customHeight="1" spans="1:10">
       <c r="A30" s="3" t="s">
-        <v>1729</v>
+        <v>1730</v>
       </c>
       <c r="B30"/>
       <c r="C30" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D30" s="3">
         <v>1</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I30"/>
       <c r="J30"/>
     </row>
     <row r="31" ht="15.1" customHeight="1" spans="1:10">
       <c r="A31" s="3" t="s">
-        <v>1730</v>
+        <v>1731</v>
       </c>
       <c r="B31"/>
       <c r="C31" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D31" s="3">
         <v>1</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I31"/>
       <c r="J31"/>
     </row>
     <row r="32" ht="15.1" customHeight="1" spans="1:10">
       <c r="A32" s="3" t="s">
-        <v>1731</v>
+        <v>1732</v>
       </c>
       <c r="B32"/>
       <c r="C32" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D32" s="3">
         <v>1</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I32"/>
       <c r="J32"/>
     </row>
     <row r="33" ht="15.1" customHeight="1" spans="1:10">
       <c r="A33" s="3" t="s">
-        <v>1732</v>
+        <v>1733</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>1733</v>
+        <v>1734</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D33" s="3">
         <v>21667.02</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>1734</v>
+        <v>1735</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>1696</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="34" ht="15.1" customHeight="1" spans="1:10">
       <c r="A34" s="3" t="s">
-        <v>1735</v>
+        <v>1736</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>1736</v>
+        <v>1737</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D34" s="3">
         <v>10020</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>1737</v>
+        <v>1738</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>1696</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="35" ht="15.1" customHeight="1" spans="1:10">
       <c r="A35" s="3" t="s">
-        <v>1738</v>
+        <v>1739</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>1739</v>
+        <v>1740</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D35" s="3">
         <v>30.6</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>1740</v>
+        <v>1741</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>1696</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="36" ht="15.1" customHeight="1" spans="1:10">
       <c r="A36" s="3" t="s">
-        <v>1741</v>
+        <v>1742</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>1742</v>
+        <v>1743</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D36" s="3">
         <v>12</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>1743</v>
+        <v>1744</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>1696</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="37" ht="15.1" customHeight="1" spans="1:10">
       <c r="A37" s="3" t="s">
-        <v>1744</v>
+        <v>1745</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>1745</v>
+        <v>1746</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D37" s="3">
         <v>1511</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>1746</v>
+        <v>1747</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>1696</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="38" ht="15.1" customHeight="1" spans="1:10">
       <c r="A38" s="3" t="s">
-        <v>1747</v>
+        <v>1748</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>1748</v>
+        <v>1749</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D38" s="3">
         <v>88800</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>1749</v>
+        <v>1750</v>
       </c>
       <c r="J38" s="3" t="s">
-        <v>1696</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="39" ht="15.1" customHeight="1" spans="1:10">
       <c r="A39" s="3" t="s">
-        <v>1750</v>
+        <v>1751</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>1751</v>
+        <v>1752</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D39" s="3">
         <v>340</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>1752</v>
+        <v>1753</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>1696</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="40" ht="15.1" customHeight="1" spans="1:10">
       <c r="A40" s="3" t="s">
-        <v>1753</v>
+        <v>1754</v>
       </c>
       <c r="B40"/>
       <c r="C40" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D40" s="3">
         <v>1</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I40"/>
       <c r="J40"/>
     </row>
     <row r="41" ht="15.1" customHeight="1" spans="1:10">
       <c r="A41" s="3" t="s">
-        <v>1754</v>
+        <v>1755</v>
       </c>
       <c r="B41"/>
       <c r="C41" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D41" s="3">
         <v>1</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I41"/>
       <c r="J41"/>
     </row>
     <row r="42" ht="15.1" customHeight="1" spans="1:10">
       <c r="A42" s="3" t="s">
-        <v>1755</v>
+        <v>1756</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>1756</v>
+        <v>1757</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D42" s="3">
         <v>213000</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>1757</v>
+        <v>1758</v>
       </c>
       <c r="J42" s="3" t="s">
-        <v>1696</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="43" ht="15.1" customHeight="1" spans="1:10">
       <c r="A43" s="3" t="s">
-        <v>1758</v>
+        <v>1759</v>
       </c>
       <c r="B43"/>
       <c r="C43" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D43" s="3">
         <v>1</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I43"/>
       <c r="J43"/>
     </row>
     <row r="44" ht="15.1" customHeight="1" spans="1:10">
       <c r="A44" s="3" t="s">
-        <v>1759</v>
+        <v>1760</v>
       </c>
       <c r="B44"/>
       <c r="C44" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D44" s="3">
         <v>1</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I44"/>
       <c r="J44"/>
     </row>
     <row r="45" ht="15.1" customHeight="1" spans="1:10">
       <c r="A45" s="3" t="s">
-        <v>1760</v>
+        <v>1761</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>1761</v>
+        <v>1762</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D45" s="3">
         <v>9600</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>1762</v>
+        <v>1763</v>
       </c>
       <c r="J45" s="3" t="s">
-        <v>1696</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="46" ht="15.1" customHeight="1" spans="1:10">
       <c r="A46" s="3" t="s">
-        <v>1763</v>
+        <v>1764</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>1764</v>
+        <v>1765</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D46" s="3">
         <v>47</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>1765</v>
+        <v>1766</v>
       </c>
       <c r="J46" s="3" t="s">
-        <v>1696</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="47" ht="15.1" customHeight="1" spans="1:10">
       <c r="A47" s="3" t="s">
-        <v>1766</v>
+        <v>1767</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>1767</v>
+        <v>1768</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D47" s="3">
         <v>200</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I47" s="3" t="s">
-        <v>1768</v>
+        <v>1769</v>
       </c>
       <c r="J47" s="3" t="s">
-        <v>1696</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="48" ht="15.1" customHeight="1" spans="1:10">
       <c r="A48" s="3" t="s">
-        <v>1769</v>
+        <v>1770</v>
       </c>
       <c r="B48"/>
       <c r="C48" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D48" s="3">
         <v>1</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I48"/>
       <c r="J48"/>
     </row>
     <row r="49" ht="15.1" customHeight="1" spans="1:10">
       <c r="A49" s="3" t="s">
-        <v>1770</v>
+        <v>1771</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>1771</v>
+        <v>1772</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D49" s="3">
         <v>120</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>1772</v>
+        <v>1773</v>
       </c>
       <c r="J49" s="3" t="s">
-        <v>1696</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="50" ht="15.1" customHeight="1" spans="1:10">
       <c r="A50" s="3" t="s">
-        <v>1773</v>
+        <v>1774</v>
       </c>
       <c r="B50"/>
       <c r="C50" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D50" s="3">
         <v>1</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I50"/>
       <c r="J50"/>
     </row>
     <row r="51" ht="15.1" customHeight="1" spans="1:10">
       <c r="A51" s="3" t="s">
-        <v>1774</v>
+        <v>1775</v>
       </c>
       <c r="B51"/>
       <c r="C51" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D51" s="3">
         <v>1</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I51"/>
       <c r="J51"/>
     </row>
     <row r="52" ht="15.1" customHeight="1" spans="1:10">
       <c r="A52" s="3" t="s">
-        <v>1775</v>
+        <v>1776</v>
       </c>
       <c r="B52"/>
       <c r="C52" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D52" s="3">
         <v>1</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I52"/>
       <c r="J52"/>
     </row>
     <row r="53" ht="15.1" customHeight="1" spans="1:10">
       <c r="A53" s="3" t="s">
-        <v>1776</v>
+        <v>1777</v>
       </c>
       <c r="B53"/>
       <c r="C53" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D53" s="3">
         <v>1</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I53"/>
       <c r="J53"/>
     </row>
     <row r="54" ht="15.1" customHeight="1" spans="1:10">
       <c r="A54" s="3" t="s">
-        <v>1777</v>
+        <v>1778</v>
       </c>
       <c r="B54"/>
       <c r="C54" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D54" s="3">
         <v>1</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I54"/>
       <c r="J54"/>
     </row>
     <row r="55" ht="15.1" customHeight="1" spans="1:10">
       <c r="A55" s="3" t="s">
-        <v>1778</v>
+        <v>1779</v>
       </c>
       <c r="B55"/>
       <c r="C55" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D55" s="3">
         <v>1</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I55"/>
       <c r="J55"/>
     </row>
     <row r="56" ht="15.1" customHeight="1" spans="1:10">
       <c r="A56" s="3" t="s">
-        <v>1779</v>
+        <v>1780</v>
       </c>
       <c r="B56"/>
       <c r="C56" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D56" s="3">
         <v>1</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I56"/>
       <c r="J56"/>
     </row>
     <row r="57" ht="15.1" customHeight="1" spans="1:10">
       <c r="A57" s="3" t="s">
-        <v>1780</v>
+        <v>1781</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>1781</v>
+        <v>1782</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D57" s="3">
         <v>6.5</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>1782</v>
+        <v>1783</v>
       </c>
       <c r="J57" s="3" t="s">
-        <v>1696</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="58" ht="15.1" customHeight="1" spans="1:10">
       <c r="A58" s="3" t="s">
-        <v>1783</v>
+        <v>1784</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>1784</v>
+        <v>1785</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D58" s="3">
         <v>1.58</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I58" s="3" t="s">
-        <v>1785</v>
+        <v>1786</v>
       </c>
       <c r="J58" s="3" t="s">
-        <v>1696</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="59" ht="15.1" customHeight="1" spans="1:10">
       <c r="A59" s="3" t="s">
-        <v>1786</v>
+        <v>1787</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>1787</v>
+        <v>1788</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D59" s="3">
         <v>52</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>1788</v>
+        <v>1789</v>
       </c>
       <c r="J59" s="3" t="s">
-        <v>1696</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="60" ht="15.1" customHeight="1" spans="1:10">
       <c r="A60" s="3" t="s">
-        <v>1789</v>
+        <v>1790</v>
       </c>
       <c r="B60"/>
       <c r="C60" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D60" s="3">
         <v>1</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I60"/>
       <c r="J60"/>
     </row>
     <row r="61" ht="15.1" customHeight="1" spans="1:10">
       <c r="A61" s="3" t="s">
-        <v>1790</v>
+        <v>1791</v>
       </c>
       <c r="B61"/>
       <c r="C61" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D61" s="3">
         <v>1</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I61"/>
       <c r="J61"/>
     </row>
     <row r="62" ht="15.1" customHeight="1" spans="1:10">
       <c r="A62" s="3" t="s">
-        <v>1791</v>
+        <v>1792</v>
       </c>
       <c r="B62"/>
       <c r="C62" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D62" s="3">
         <v>1</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I62"/>
       <c r="J62"/>
     </row>
     <row r="63" ht="15.1" customHeight="1" spans="1:10">
       <c r="A63" s="3" t="s">
-        <v>1792</v>
+        <v>1793</v>
       </c>
       <c r="B63" s="6"/>
       <c r="C63" s="3" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D63" s="3">
         <v>1247</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>1793</v>
+        <v>1794</v>
       </c>
       <c r="I63" s="6"/>
       <c r="J63" s="3" t="s">
-        <v>1696</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="64" ht="15.1" customHeight="1" spans="1:10">
       <c r="A64" s="3" t="s">
-        <v>1794</v>
+        <v>1795</v>
       </c>
       <c r="B64"/>
       <c r="C64" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D64" s="3">
         <v>1</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I64"/>
       <c r="J64"/>
     </row>
     <row r="65" ht="15.1" customHeight="1" spans="1:10">
       <c r="A65" s="3" t="s">
-        <v>1795</v>
+        <v>1796</v>
       </c>
       <c r="B65"/>
       <c r="C65" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D65" s="3">
         <v>1</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I65"/>
       <c r="J65"/>
     </row>
     <row r="66" ht="15.1" customHeight="1" spans="1:10">
       <c r="A66" s="3" t="s">
-        <v>1796</v>
+        <v>1797</v>
       </c>
       <c r="B66"/>
       <c r="C66" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D66" s="3">
         <v>1</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I66"/>
       <c r="J66"/>
     </row>
     <row r="67" ht="15.1" customHeight="1" spans="1:10">
       <c r="A67" s="3" t="s">
-        <v>1797</v>
+        <v>1798</v>
       </c>
       <c r="B67"/>
       <c r="C67" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D67" s="3">
         <v>1</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I67"/>
       <c r="J67"/>
     </row>
     <row r="68" ht="15.1" customHeight="1" spans="1:10">
       <c r="A68" s="3" t="s">
-        <v>1798</v>
+        <v>1799</v>
       </c>
       <c r="B68"/>
       <c r="C68" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D68" s="3">
         <v>1</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I68"/>
       <c r="J68"/>
     </row>
     <row r="69" ht="15.1" customHeight="1" spans="1:10">
       <c r="A69" s="3" t="s">
-        <v>1799</v>
+        <v>1800</v>
       </c>
       <c r="B69"/>
       <c r="C69" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D69" s="3">
         <v>1</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I69"/>
       <c r="J69"/>
     </row>
     <row r="70" ht="15.1" customHeight="1" spans="1:10">
       <c r="A70" s="3" t="s">
-        <v>1800</v>
+        <v>1801</v>
       </c>
       <c r="B70"/>
       <c r="C70" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D70" s="3">
         <v>1</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I70"/>
       <c r="J70"/>
     </row>
     <row r="71" ht="15.1" customHeight="1" spans="1:10">
       <c r="A71" s="3" t="s">
-        <v>1801</v>
+        <v>1802</v>
       </c>
       <c r="B71"/>
       <c r="C71" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D71" s="3">
         <v>1</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I71"/>
       <c r="J71"/>
     </row>
     <row r="72" ht="15.1" customHeight="1" spans="1:10">
       <c r="A72" s="3" t="s">
-        <v>1802</v>
+        <v>1803</v>
       </c>
       <c r="B72"/>
       <c r="C72" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D72" s="3">
         <v>1</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I72"/>
       <c r="J72"/>
     </row>
     <row r="73" ht="15.1" customHeight="1" spans="1:10">
       <c r="A73" s="3" t="s">
-        <v>1803</v>
+        <v>1804</v>
       </c>
       <c r="B73"/>
       <c r="C73" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D73" s="3">
         <v>1</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I73"/>
       <c r="J73"/>
     </row>
     <row r="74" ht="15.1" customHeight="1" spans="1:10">
       <c r="A74" s="3" t="s">
-        <v>1804</v>
+        <v>1805</v>
       </c>
       <c r="B74"/>
       <c r="C74" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D74" s="3">
         <v>1</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I74"/>
       <c r="J74"/>
     </row>
     <row r="75" ht="15.1" customHeight="1" spans="1:10">
       <c r="A75" s="3" t="s">
-        <v>1805</v>
+        <v>1806</v>
       </c>
       <c r="B75"/>
       <c r="C75" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D75" s="3">
         <v>1</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I75"/>
       <c r="J75"/>
     </row>
     <row r="76" ht="15.1" customHeight="1" spans="1:10">
       <c r="A76" s="3" t="s">
-        <v>1806</v>
+        <v>1807</v>
       </c>
       <c r="B76"/>
       <c r="C76" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D76" s="3">
         <v>1</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I76"/>
       <c r="J76"/>
     </row>
     <row r="77" ht="15.1" customHeight="1" spans="1:10">
       <c r="A77" s="3" t="s">
-        <v>1807</v>
+        <v>1808</v>
       </c>
       <c r="B77"/>
       <c r="C77" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D77" s="3">
         <v>1</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I77"/>
       <c r="J77"/>
     </row>
     <row r="78" ht="15.1" customHeight="1" spans="1:10">
       <c r="A78" s="3" t="s">
-        <v>1808</v>
+        <v>1809</v>
       </c>
       <c r="B78"/>
       <c r="C78" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D78" s="3">
         <v>1</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I78"/>
       <c r="J78"/>
     </row>
     <row r="79" ht="15.1" customHeight="1" spans="1:10">
       <c r="A79" s="3" t="s">
-        <v>1809</v>
+        <v>1810</v>
       </c>
       <c r="B79"/>
       <c r="C79" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D79" s="3">
         <v>1</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I79"/>
       <c r="J79"/>
     </row>
     <row r="80" ht="15.1" customHeight="1" spans="1:10">
       <c r="A80" s="3" t="s">
-        <v>1810</v>
+        <v>1811</v>
       </c>
       <c r="B80"/>
       <c r="C80" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D80" s="3">
         <v>1</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I80"/>
       <c r="J80"/>
     </row>
     <row r="81" ht="15.1" customHeight="1" spans="1:10">
       <c r="A81" s="3" t="s">
-        <v>1811</v>
+        <v>1812</v>
       </c>
       <c r="B81"/>
       <c r="C81" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D81" s="3">
         <v>1</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I81"/>
       <c r="J81"/>
     </row>
     <row r="82" ht="15.1" customHeight="1" spans="1:10">
       <c r="A82" s="3" t="s">
-        <v>1812</v>
+        <v>1813</v>
       </c>
       <c r="B82"/>
       <c r="C82" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D82" s="3">
         <v>1</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I82"/>
       <c r="J82"/>
     </row>
     <row r="83" ht="15.1" customHeight="1" spans="1:10">
       <c r="A83" s="3" t="s">
-        <v>1813</v>
+        <v>1814</v>
       </c>
       <c r="B83"/>
       <c r="C83" s="1" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D83" s="3">
         <v>1</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I83"/>
       <c r="J83"/>
     </row>
     <row r="84" ht="15.1" customHeight="1" spans="1:10">
       <c r="A84" s="3" t="s">
-        <v>1814</v>
+        <v>1815</v>
       </c>
       <c r="B84" s="6"/>
       <c r="C84" s="3" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D84" s="3">
         <v>0.000231049060186648</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I84" s="3" t="s">
-        <v>1815</v>
+        <v>1816</v>
       </c>
       <c r="J84" s="6"/>
     </row>
     <row r="85" ht="15.1" customHeight="1" spans="1:10">
       <c r="A85" s="3" t="s">
-        <v>1816</v>
+        <v>1817</v>
       </c>
       <c r="B85" s="6"/>
       <c r="C85" s="3" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D85" s="3">
         <v>265.521194884729</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>1793</v>
+        <v>1794</v>
       </c>
       <c r="I85" s="3" t="s">
-        <v>1817</v>
+        <v>1818</v>
       </c>
       <c r="J85" s="6"/>
     </row>
     <row r="86" ht="15.1" customHeight="1" spans="1:10">
       <c r="A86" s="3" t="s">
-        <v>1818</v>
+        <v>1819</v>
       </c>
       <c r="B86" s="6"/>
       <c r="C86" s="3" t="s">
-        <v>1686</v>
+        <v>1687</v>
       </c>
       <c r="D86" s="3">
         <v>0.000233455821230259</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>1687</v>
+        <v>1688</v>
       </c>
       <c r="I86" s="3" t="s">
-        <v>1817</v>
+        <v>1818</v>
       </c>
       <c r="J86" s="6"/>
     </row>
     <row r="87" ht="15.1" customHeight="1" spans="1:10">
       <c r="A87" s="3" t="s">
-        <v>1819</v>
+        <v>1820</v>
       </c>
       <c r="B87" s="6"/>
       <c r="C87" s="3" t="s">
-        <v>1820</v>
+        <v>1821</v>
       </c>
       <c r="D87" s="3">
         <v>1.81285794880199e-7</v>
@@ -18244,17 +18253,17 @@
         <v>422</v>
       </c>
       <c r="I87" s="3" t="s">
-        <v>1815</v>
+        <v>1816</v>
       </c>
       <c r="J87" s="6"/>
     </row>
     <row r="88" ht="15.1" customHeight="1" spans="1:10">
       <c r="A88" s="3" t="s">
-        <v>1821</v>
+        <v>1822</v>
       </c>
       <c r="B88" s="6"/>
       <c r="C88" s="3" t="s">
-        <v>1820</v>
+        <v>1821</v>
       </c>
       <c r="D88" s="3">
         <v>0.0005</v>
@@ -18263,17 +18272,17 @@
         <v>422</v>
       </c>
       <c r="I88" s="3" t="s">
-        <v>1817</v>
+        <v>1818</v>
       </c>
       <c r="J88" s="6"/>
     </row>
     <row r="89" ht="15.1" customHeight="1" spans="1:10">
       <c r="A89" s="3" t="s">
-        <v>1822</v>
+        <v>1823</v>
       </c>
       <c r="B89" s="6"/>
       <c r="C89" s="3" t="s">
-        <v>1820</v>
+        <v>1821</v>
       </c>
       <c r="D89" s="3">
         <v>0.001</v>
@@ -18282,16 +18291,16 @@
         <v>422</v>
       </c>
       <c r="I89" s="3" t="s">
-        <v>1817</v>
+        <v>1818</v>
       </c>
       <c r="J89" s="6"/>
     </row>
     <row r="90" ht="15.1" customHeight="1" spans="1:10">
       <c r="A90" s="3" t="s">
-        <v>1823</v>
+        <v>1824</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>1824</v>
+        <v>1825</v>
       </c>
       <c r="C90" s="3" t="s">
         <v>1282</v>
@@ -18300,21 +18309,21 @@
         <v>20</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>1676</v>
+        <v>1677</v>
       </c>
       <c r="I90" s="3" t="s">
-        <v>1825</v>
+        <v>1826</v>
       </c>
       <c r="J90" s="3" t="s">
-        <v>1606</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="91" ht="15.1" customHeight="1" spans="1:6">
       <c r="A91" s="3" t="s">
-        <v>1826</v>
+        <v>1827</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>1827</v>
+        <v>1828</v>
       </c>
       <c r="C91" s="3" t="s">
         <v>1282</v>
@@ -18328,7 +18337,7 @@
     </row>
     <row r="92" ht="15.1" customHeight="1" spans="1:6">
       <c r="A92" s="3" t="s">
-        <v>1828</v>
+        <v>1829</v>
       </c>
       <c r="C92" s="3" t="s">
         <v>1282</v>
@@ -18342,7 +18351,7 @@
     </row>
     <row r="93" ht="15.1" customHeight="1" spans="1:6">
       <c r="A93" s="3" t="s">
-        <v>1829</v>
+        <v>1830</v>
       </c>
       <c r="C93" s="3" t="s">
         <v>1282</v>
@@ -18411,11 +18420,11 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:6">
       <c r="A2" s="3" t="s">
-        <v>1830</v>
+        <v>1831</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>1831</v>
+        <v>1832</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>742</v>
@@ -18425,11 +18434,11 @@
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:6">
       <c r="A3" s="3" t="s">
-        <v>1832</v>
+        <v>1833</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>1833</v>
+        <v>1834</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>742</v>
@@ -18474,7 +18483,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>1601</v>
+        <v>1602</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>420</v>
@@ -18483,19 +18492,19 @@
         <v>69</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>1834</v>
+        <v>1835</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>1835</v>
+        <v>1836</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>1836</v>
+        <v>1837</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>1837</v>
+        <v>1838</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>1838</v>
+        <v>1839</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>18</v>
@@ -18515,19 +18524,19 @@
         <v>603</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1839</v>
+        <v>1840</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>1840</v>
+        <v>1841</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>602</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>1841</v>
+        <v>1842</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>1842</v>
+        <v>1843</v>
       </c>
       <c r="H2" s="3">
         <v>37</v>
@@ -18536,88 +18545,88 @@
         <v>7.5</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>1843</v>
+        <v>1844</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1844</v>
+        <v>1845</v>
       </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:8">
       <c r="A3" s="3" t="s">
-        <v>1845</v>
+        <v>1846</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1846</v>
+        <v>1847</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>1847</v>
+        <v>1848</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>602</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>1841</v>
+        <v>1842</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>1842</v>
+        <v>1843</v>
       </c>
       <c r="H3" s="1"/>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:8">
       <c r="A4" s="3" t="s">
-        <v>1848</v>
+        <v>1849</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1849</v>
+        <v>1850</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>1850</v>
+        <v>1851</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>602</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>1841</v>
+        <v>1842</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>1842</v>
+        <v>1843</v>
       </c>
       <c r="H4" s="1"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:8">
       <c r="A5" s="3" t="s">
-        <v>1851</v>
+        <v>1852</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1852</v>
+        <v>1853</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>1853</v>
+        <v>1854</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>602</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>1841</v>
+        <v>1842</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>1842</v>
+        <v>1843</v>
       </c>
       <c r="H5" s="1"/>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:8">
       <c r="A6" s="3" t="s">
-        <v>1854</v>
+        <v>1855</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1855</v>
+        <v>1856</v>
       </c>
       <c r="C6" s="5"/>
       <c r="E6" s="3" t="s">
-        <v>1856</v>
+        <v>1857</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>1857</v>
+        <v>1858</v>
       </c>
       <c r="H6" s="3">
         <v>37</v>
@@ -18628,14 +18637,14 @@
         <v>607</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1858</v>
+        <v>1859</v>
       </c>
       <c r="C7" s="5"/>
       <c r="E7" s="3" t="s">
-        <v>1859</v>
+        <v>1860</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>1860</v>
+        <v>1861</v>
       </c>
       <c r="H7" s="3">
         <v>30</v>
@@ -18643,17 +18652,17 @@
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:8">
       <c r="A8" s="3" t="s">
-        <v>1861</v>
+        <v>1862</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1862</v>
+        <v>1863</v>
       </c>
       <c r="C8" s="5"/>
       <c r="E8" s="3" t="s">
-        <v>1863</v>
+        <v>1864</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>1864</v>
+        <v>1865</v>
       </c>
       <c r="H8" s="3">
         <v>37</v>
@@ -18661,17 +18670,17 @@
     </row>
     <row r="9" ht="15.1" customHeight="1" spans="1:8">
       <c r="A9" s="3" t="s">
-        <v>1865</v>
+        <v>1866</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>1866</v>
+        <v>1867</v>
       </c>
       <c r="C9" s="5"/>
       <c r="E9" s="3" t="s">
         <v>1282</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>1867</v>
+        <v>1868</v>
       </c>
       <c r="H9" s="3">
         <v>40</v>
@@ -18713,46 +18722,46 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1868</v>
+        <v>1869</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>1869</v>
+        <v>1870</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>1870</v>
+        <v>1871</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>69</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>1871</v>
+        <v>1872</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>1872</v>
+        <v>1873</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>1873</v>
+        <v>1874</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>41</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>1874</v>
+        <v>1875</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>1875</v>
+        <v>1876</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>1876</v>
+        <v>1877</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>1877</v>
+        <v>1878</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>1878</v>
+        <v>1879</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>18</v>
@@ -18763,68 +18772,68 @@
     </row>
     <row r="2" ht="15.1" customHeight="1" spans="1:18">
       <c r="A2" s="3" t="s">
-        <v>1879</v>
+        <v>1880</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1880</v>
+        <v>1881</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>1881</v>
+        <v>1882</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>1882</v>
+        <v>1883</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3">
         <v>2008</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>1883</v>
+        <v>1884</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1884</v>
+        <v>1885</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3" t="s">
-        <v>1840</v>
+        <v>1841</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>1840</v>
+        <v>1841</v>
       </c>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3" t="s">
-        <v>1885</v>
+        <v>1886</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>1886</v>
+        <v>1887</v>
       </c>
       <c r="R2" s="3"/>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:18">
       <c r="A3" s="3" t="s">
-        <v>1887</v>
+        <v>1888</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1888</v>
+        <v>1889</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>1889</v>
+        <v>1890</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>1890</v>
+        <v>1891</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3">
         <v>2014</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>1883</v>
+        <v>1884</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>1891</v>
+        <v>1892</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
@@ -18834,160 +18843,160 @@
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3" t="s">
-        <v>1892</v>
+        <v>1893</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>1893</v>
+        <v>1894</v>
       </c>
       <c r="R3" s="3"/>
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:18">
       <c r="A4" s="3" t="s">
-        <v>1894</v>
+        <v>1895</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1895</v>
+        <v>1896</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>1896</v>
+        <v>1897</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>1897</v>
+        <v>1898</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3">
         <v>2004</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>1883</v>
+        <v>1884</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>1891</v>
+        <v>1892</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3" t="s">
-        <v>1898</v>
+        <v>1899</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>1899</v>
+        <v>1900</v>
       </c>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3" t="s">
-        <v>1900</v>
+        <v>1901</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>1901</v>
+        <v>1902</v>
       </c>
       <c r="R4" s="3"/>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="1:18">
       <c r="A5" s="3" t="s">
-        <v>1902</v>
+        <v>1903</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>1903</v>
+        <v>1904</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>1904</v>
+        <v>1905</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>1905</v>
+        <v>1906</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3">
         <v>2009</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>1883</v>
+        <v>1884</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>1906</v>
+        <v>1907</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3" t="s">
-        <v>1907</v>
+        <v>1908</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>1908</v>
+        <v>1909</v>
       </c>
       <c r="M5" s="3"/>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3" t="s">
-        <v>1909</v>
+        <v>1910</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>1910</v>
+        <v>1911</v>
       </c>
       <c r="R5" s="3"/>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:18">
       <c r="A6" s="3" t="s">
-        <v>1911</v>
+        <v>1912</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>1912</v>
+        <v>1913</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>1913</v>
+        <v>1914</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>1914</v>
+        <v>1915</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3">
         <v>2007</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>1883</v>
+        <v>1884</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>1915</v>
+        <v>1916</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="3" t="s">
-        <v>1916</v>
+        <v>1917</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>1840</v>
+        <v>1841</v>
       </c>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
       <c r="Q6" s="3" t="s">
-        <v>1917</v>
+        <v>1918</v>
       </c>
       <c r="R6" s="3"/>
     </row>
     <row r="7" ht="15.1" customHeight="1" spans="1:18">
       <c r="A7" s="3" t="s">
-        <v>1682</v>
+        <v>1683</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>1918</v>
+        <v>1919</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>1919</v>
+        <v>1920</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>1920</v>
+        <v>1921</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3">
         <v>2001</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>1921</v>
+        <v>1922</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3" t="s">
-        <v>1922</v>
+        <v>1923</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -18997,35 +19006,35 @@
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
       <c r="Q7" s="3" t="s">
-        <v>1923</v>
+        <v>1924</v>
       </c>
       <c r="R7" s="3"/>
     </row>
     <row r="8" ht="15.1" customHeight="1" spans="1:18">
       <c r="A8" s="3" t="s">
-        <v>1696</v>
+        <v>1697</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>1924</v>
+        <v>1925</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>1925</v>
+        <v>1926</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>1926</v>
+        <v>1927</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3">
         <v>2006</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>1927</v>
+        <v>1928</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>1928</v>
+        <v>1929</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>1929</v>
+        <v>1930</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
@@ -19035,217 +19044,217 @@
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3" t="s">
-        <v>1930</v>
+        <v>1931</v>
       </c>
       <c r="R8" s="3"/>
     </row>
     <row r="9" ht="15.1" customHeight="1" spans="1:18">
       <c r="A9" s="3" t="s">
-        <v>1931</v>
+        <v>1932</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>1932</v>
+        <v>1933</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>1933</v>
+        <v>1934</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>1934</v>
+        <v>1935</v>
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="3">
         <v>1993</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>1883</v>
+        <v>1884</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>1935</v>
+        <v>1936</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3" t="s">
-        <v>1936</v>
+        <v>1937</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>1840</v>
+        <v>1841</v>
       </c>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
       <c r="P9" s="3" t="s">
-        <v>1937</v>
+        <v>1938</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>1938</v>
+        <v>1939</v>
       </c>
       <c r="R9" s="3"/>
     </row>
     <row r="10" ht="15.1" customHeight="1" spans="1:18">
       <c r="A10" s="3" t="s">
-        <v>1939</v>
+        <v>1940</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>1940</v>
+        <v>1941</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>1941</v>
+        <v>1942</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>1942</v>
+        <v>1943</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3">
         <v>2010</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>1883</v>
+        <v>1884</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>1943</v>
+        <v>1944</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3" t="s">
-        <v>1944</v>
+        <v>1945</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>1916</v>
+        <v>1917</v>
       </c>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
       <c r="P10" s="3" t="s">
-        <v>1945</v>
+        <v>1946</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>1946</v>
+        <v>1947</v>
       </c>
       <c r="R10" s="3"/>
     </row>
     <row r="11" ht="15.1" customHeight="1" spans="1:18">
       <c r="A11" s="3" t="s">
-        <v>1947</v>
+        <v>1948</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>1948</v>
+        <v>1949</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>1949</v>
+        <v>1950</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>1950</v>
+        <v>1951</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3">
         <v>2000</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>1883</v>
+        <v>1884</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>1951</v>
+        <v>1952</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3" t="s">
-        <v>1952</v>
+        <v>1953</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>1953</v>
+        <v>1954</v>
       </c>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3" t="s">
-        <v>1954</v>
+        <v>1955</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>1955</v>
+        <v>1956</v>
       </c>
       <c r="R11" s="3"/>
     </row>
     <row r="12" ht="15.1" customHeight="1" spans="1:18">
       <c r="A12" s="3" t="s">
-        <v>1956</v>
+        <v>1957</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>1957</v>
+        <v>1958</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>1958</v>
+        <v>1959</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>1959</v>
+        <v>1960</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3">
         <v>1999</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>1883</v>
+        <v>1884</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>1960</v>
+        <v>1961</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3" t="s">
-        <v>1840</v>
+        <v>1841</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>1916</v>
+        <v>1917</v>
       </c>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3" t="s">
-        <v>1961</v>
+        <v>1962</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>1962</v>
+        <v>1963</v>
       </c>
       <c r="R12" s="3"/>
     </row>
     <row r="13" ht="15.1" customHeight="1" spans="1:18">
       <c r="A13" s="3" t="s">
-        <v>1963</v>
+        <v>1964</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>1964</v>
+        <v>1965</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>1965</v>
+        <v>1966</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>1966</v>
+        <v>1967</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3">
         <v>1979</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>1883</v>
+        <v>1884</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>1951</v>
+        <v>1952</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3" t="s">
-        <v>1967</v>
+        <v>1968</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>1968</v>
+        <v>1969</v>
       </c>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3" t="s">
-        <v>1969</v>
+        <v>1970</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>1970</v>
+        <v>1971</v>
       </c>
       <c r="R13" s="3"/>
     </row>
@@ -19254,40 +19263,40 @@
         <v>74</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>1971</v>
+        <v>1972</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>1972</v>
+        <v>1973</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>1973</v>
+        <v>1974</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3">
         <v>2012</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>1883</v>
+        <v>1884</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>1974</v>
+        <v>1975</v>
       </c>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3" t="s">
-        <v>1975</v>
+        <v>1976</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>1908</v>
+        <v>1909</v>
       </c>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
       <c r="P14" s="3" t="s">
-        <v>1976</v>
+        <v>1977</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>1977</v>
+        <v>1978</v>
       </c>
       <c r="R14" s="3"/>
     </row>
@@ -19296,56 +19305,56 @@
         <v>187</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>1978</v>
+        <v>1979</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>1979</v>
+        <v>1980</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>1980</v>
+        <v>1981</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="3">
         <v>2009</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>1883</v>
+        <v>1884</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>1981</v>
+        <v>1982</v>
       </c>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3" t="s">
-        <v>1982</v>
+        <v>1983</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>1983</v>
+        <v>1984</v>
       </c>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
       <c r="P15" s="3" t="s">
-        <v>1984</v>
+        <v>1985</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>1985</v>
+        <v>1986</v>
       </c>
       <c r="R15" s="3"/>
     </row>
     <row r="16" ht="15.1" customHeight="1" spans="1:18">
       <c r="A16" s="3" t="s">
-        <v>1986</v>
+        <v>1987</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>1987</v>
+        <v>1988</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3" t="s">
-        <v>1988</v>
+        <v>1989</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
@@ -19357,23 +19366,23 @@
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
       <c r="Q16" s="3" t="s">
-        <v>1989</v>
+        <v>1990</v>
       </c>
       <c r="R16" s="3"/>
     </row>
     <row r="17" ht="15.1" customHeight="1" spans="1:18">
       <c r="A17" s="3" t="s">
-        <v>1990</v>
+        <v>1991</v>
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="3" t="s">
-        <v>1991</v>
+        <v>1992</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3" t="s">
-        <v>1988</v>
+        <v>1989</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
@@ -19385,23 +19394,23 @@
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
       <c r="Q17" s="3" t="s">
-        <v>1992</v>
+        <v>1993</v>
       </c>
       <c r="R17" s="3"/>
     </row>
     <row r="18" ht="15.1" customHeight="1" spans="1:18">
       <c r="A18" s="3" t="s">
-        <v>1993</v>
+        <v>1994</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3" t="s">
-        <v>1994</v>
+        <v>1995</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3" t="s">
-        <v>1988</v>
+        <v>1989</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
@@ -19413,23 +19422,23 @@
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>
       <c r="Q18" s="3" t="s">
-        <v>1995</v>
+        <v>1996</v>
       </c>
       <c r="R18" s="3"/>
     </row>
     <row r="19" ht="15.1" customHeight="1" spans="1:18">
       <c r="A19" s="3" t="s">
-        <v>1996</v>
+        <v>1997</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3" t="s">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3" t="s">
-        <v>1988</v>
+        <v>1989</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
@@ -19441,7 +19450,7 @@
       <c r="O19" s="3"/>
       <c r="P19" s="3"/>
       <c r="Q19" s="3" t="s">
-        <v>1998</v>
+        <v>1999</v>
       </c>
       <c r="R19" s="3"/>
     </row>
@@ -19451,13 +19460,13 @@
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
-        <v>1999</v>
+        <v>2000</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3" t="s">
-        <v>1988</v>
+        <v>1989</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
@@ -19469,54 +19478,54 @@
       <c r="O20" s="3"/>
       <c r="P20" s="3"/>
       <c r="Q20" s="3" t="s">
-        <v>2000</v>
+        <v>2001</v>
       </c>
       <c r="R20" s="3"/>
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="1" t="s">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="F21" s="1">
         <v>2015</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>1988</v>
+        <v>1989</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>2005</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="1" t="s">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="F22" s="1">
         <v>2018</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>1988</v>
+        <v>1989</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>2010</v>
+        <v>2011</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Renamed DfbaNetReaction --> DfbaObjReaction, DfbaNetSpecies --> DfbaObjSpecies
</commit_message>
<xml_diff>
--- a/tests/fixtures/example-model.xlsx
+++ b/tests/fixtures/example-model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="19800" windowHeight="6840" tabRatio="993" activeTab="2"/>
+    <workbookView windowWidth="28200" windowHeight="14070" tabRatio="993" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,8 @@
     <sheet name="Reactions" sheetId="10" r:id="rId11"/>
     <sheet name="Rate laws" sheetId="11" r:id="rId12"/>
     <sheet name="dFBA objectives" sheetId="12" r:id="rId13"/>
-    <sheet name="dFBA net reactions" sheetId="13" r:id="rId14"/>
-    <sheet name="dFBA net species" sheetId="14" r:id="rId15"/>
+    <sheet name="dFBA objective reactions" sheetId="13" r:id="rId14"/>
+    <sheet name="dFBA objective species" sheetId="14" r:id="rId15"/>
     <sheet name="Parameters" sheetId="15" r:id="rId16"/>
     <sheet name="Stop conditions" sheetId="16" r:id="rId17"/>
     <sheet name="Evidence" sheetId="17" r:id="rId18"/>
@@ -5225,7 +5225,7 @@
     <t>NA</t>
   </si>
   <si>
-    <t>dFBA net reaction</t>
+    <t>dFBA objective reaction</t>
   </si>
   <si>
     <t>Value</t>
@@ -6472,11 +6472,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -6512,10 +6512,15 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -6526,18 +6531,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -6564,6 +6576,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -6580,36 +6600,10 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
     </font>
     <font>
       <b/>
@@ -6629,30 +6623,36 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6679,13 +6679,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6697,31 +6703,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6739,7 +6721,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6751,7 +6751,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6769,7 +6775,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6781,43 +6811,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6835,19 +6829,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6909,15 +6909,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
@@ -6964,143 +6955,152 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="18" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="18" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="18" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="18" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -7150,9 +7150,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -16179,12 +16176,12 @@
   <sheetPr/>
   <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -19958,7 +19955,7 @@
     <col min="1" max="1" width="10.3916666666667" style="3"/>
     <col min="2" max="2" width="29.775" style="3"/>
     <col min="3" max="1025" width="8.78333333333333" style="3"/>
-    <col min="1026" max="16384" width="9" style="18"/>
+    <col min="1026" max="16384" width="9" style="6"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.1" customHeight="1" spans="1:2">
@@ -20012,7 +20009,7 @@
   <sheetPr/>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection/>
       <selection pane="topRight" activeCell="G6" sqref="G6"/>

</xml_diff>

<commit_message>
starting to migrate enum types to ontologies
</commit_message>
<xml_diff>
--- a/tests/fixtures/example-model.xlsx
+++ b/tests/fixtures/example-model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="19800" windowHeight="6945" tabRatio="993" firstSheet="10" activeTab="17"/>
+    <workbookView windowWidth="28695" windowHeight="14070" tabRatio="993" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -565,13 +565,13 @@
     <t>Cytoplasm</t>
   </si>
   <si>
-    <t>cellular</t>
-  </si>
-  <si>
-    <t>fluid</t>
-  </si>
-  <si>
-    <t>3d</t>
+    <t>WCM:0000003 ! cellular compartment</t>
+  </si>
+  <si>
+    <t>WCM:0000006 ! fluid compartment</t>
+  </si>
+  <si>
+    <t>WCM:0000009 ! 3d compartment</t>
   </si>
   <si>
     <t>e</t>
@@ -599,7 +599,7 @@
     <t>Extracellular space</t>
   </si>
   <si>
-    <t>extracellular</t>
+    <t>WCM:0000004 ! extracellular compartment</t>
   </si>
   <si>
     <t>density_e</t>
@@ -6515,11 +6515,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -6567,25 +6567,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -6612,6 +6596,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -6619,8 +6619,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6634,22 +6642,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6657,22 +6650,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6700,6 +6692,14 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -6716,19 +6716,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6740,7 +6734,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6752,37 +6782,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6800,25 +6812,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6830,7 +6836,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6842,13 +6878,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6860,43 +6896,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6907,21 +6907,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -6943,6 +6928,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -6954,6 +6950,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -6975,11 +6986,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -6998,144 +7007,135 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -19097,7 +19097,7 @@
   <sheetPr/>
   <dimension ref="A1:V9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
@@ -19461,8 +19461,6 @@
       <c r="F2" s="3" t="s">
         <v>1889</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
       <c r="I2" s="3" t="s">
         <v>1862</v>
       </c>
@@ -19486,8 +19484,6 @@
       <c r="F3" s="3" t="s">
         <v>1892</v>
       </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
       <c r="I3" s="3" t="s">
         <v>1893</v>
       </c>
@@ -20652,18 +20648,20 @@
   <sheetPr/>
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="O2" sqref="O2"/>
+      <selection pane="bottomRight" activeCell="D7" sqref="D7:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2"/>
   <cols>
     <col min="1" max="1" width="6.10833333333333" style="9"/>
-    <col min="2" max="4" width="16.3916666666667" style="9"/>
+    <col min="2" max="2" width="16.3916666666667" style="9"/>
+    <col min="3" max="3" width="24.125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="17.5" style="9" customWidth="1"/>
     <col min="5" max="7" width="14.1416666666667" style="9"/>
     <col min="8" max="16" width="11.7833333333333" style="9"/>
     <col min="17" max="17" width="11.3583333333333" style="9"/>

</xml_diff>

<commit_message>
replacing SubmodelAlgorithm with ontology
</commit_message>
<xml_diff>
--- a/tests/fixtures/example-model.xlsx
+++ b/tests/fixtures/example-model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="14070" tabRatio="993" activeTab="4"/>
+    <workbookView windowWidth="28695" windowHeight="14070" tabRatio="993" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -508,7 +508,7 @@
     <t>Metabolism</t>
   </si>
   <si>
-    <t>dfba</t>
+    <t>WCM:0000013 ! dFBA</t>
   </si>
   <si>
     <t>E.g., obj. fn.</t>
@@ -520,7 +520,7 @@
     <t>RNA degradation</t>
   </si>
   <si>
-    <t>ssa</t>
+    <t>WCM:0000011 ! SSA</t>
   </si>
   <si>
     <t>Transcription</t>
@@ -20524,12 +20524,12 @@
   <sheetPr/>
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="7"/>
@@ -20648,7 +20648,7 @@
   <sheetPr/>
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>

</xml_diff>

<commit_message>
simplifying units with pint and UnitAttribute
</commit_message>
<xml_diff>
--- a/tests/fixtures/example-model.xlsx
+++ b/tests/fixtures/example-model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="14070" tabRatio="993" activeTab="3"/>
+    <workbookView windowWidth="28695" windowHeight="13965" tabRatio="993"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -445,7 +445,7 @@
     <t>Time units</t>
   </si>
   <si>
-    <t>s</t>
+    <t>second</t>
   </si>
   <si>
     <t>Database references</t>
@@ -484,7 +484,7 @@
     <t>Temperature units</t>
   </si>
   <si>
-    <t>C</t>
+    <t>degC</t>
   </si>
   <si>
     <t>pH</t>
@@ -577,13 +577,13 @@
     <t>e</t>
   </si>
   <si>
-    <t>g</t>
+    <t>gram</t>
   </si>
   <si>
     <t>normal_distribution</t>
   </si>
   <si>
-    <t>l</t>
+    <t>liter</t>
   </si>
   <si>
     <t>density_c</t>
@@ -2223,7 +2223,7 @@
     <t>dist-init-conc-AD[e]</t>
   </si>
   <si>
-    <t>M</t>
+    <t>molar</t>
   </si>
   <si>
     <t>evidence_001</t>
@@ -2697,7 +2697,7 @@
     <t>AD[e] + H[e] ==&gt; AD[c] + H[c]</t>
   </si>
   <si>
-    <t>s^-1</t>
+    <t>1 / second</t>
   </si>
   <si>
     <t>AK_AMP</t>
@@ -5241,7 +5241,7 @@
     <t>ALA net component</t>
   </si>
   <si>
-    <t>M s^-1</t>
+    <t>molar / second</t>
   </si>
   <si>
     <t>test</t>
@@ -5454,7 +5454,7 @@
     <t>Avogadro</t>
   </si>
   <si>
-    <t>molecule mol^-1</t>
+    <t>molecule / mole</t>
   </si>
   <si>
     <t>carbonExchangeRate</t>
@@ -5463,7 +5463,7 @@
     <t>Carbon-containing metabolite exchange rate</t>
   </si>
   <si>
-    <t>mmol/gDCW/h</t>
+    <t>millimole / gDCW / hour</t>
   </si>
   <si>
     <t>Exchange rate upper bound for carbon-containing metabolites (mmol/gDCW/h). Maranas et al. used 5 mmol/gDCW/h for all carbon-containing metabolites [Ref_0004]. Feist et al. used 11.2 mmol/gDCW/h for glucose [Ref_0005].</t>
@@ -5475,7 +5475,7 @@
     <t>Cell cycle length</t>
   </si>
   <si>
-    <t>g l^-1</t>
+    <t>gram / liter</t>
   </si>
   <si>
     <t>fractionDryWeight</t>
@@ -5499,7 +5499,7 @@
     <t>k_cat</t>
   </si>
   <si>
-    <t>molecule^-1 s^-1</t>
+    <t>1 / molecule / second</t>
   </si>
   <si>
     <t>k_cat_for_ak</t>
@@ -5817,7 +5817,7 @@
     <t>k_cat_rev_ak</t>
   </si>
   <si>
-    <t>molecule^-2 s^-1</t>
+    <t>1 / molecule ** 2 / second</t>
   </si>
   <si>
     <t>k_cat_rev_aprt</t>
@@ -6509,10 +6509,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="25">
@@ -6557,7 +6557,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6565,27 +6565,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6598,9 +6586,43 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6615,7 +6637,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6623,43 +6645,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6674,6 +6667,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -6681,17 +6689,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -6710,31 +6710,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6746,13 +6728,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6770,19 +6800,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6794,7 +6854,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6806,91 +6890,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6901,21 +6901,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -6938,7 +6923,46 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -6950,15 +6974,6 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -6986,153 +7001,138 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -7593,10 +7593,10 @@
   <sheetPr/>
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="A8" sqref="A8"/>
+      <selection pane="topRight" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1"/>
@@ -7731,7 +7731,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5"/>
@@ -7860,7 +7860,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L1" sqref="L1"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -12790,11 +12790,11 @@
   <dimension ref="A1:L168"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D100" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E100" sqref="E100"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2:G168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -15715,7 +15715,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J1" sqref="J1"/>
+      <selection pane="bottomRight" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="1"/>
@@ -15804,7 +15804,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2"/>
@@ -15905,7 +15905,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2:F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -16677,11 +16677,11 @@
   <dimension ref="A1:K96"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C90" sqref="C90:C92"/>
+      <selection pane="bottomRight" activeCell="F97" sqref="F97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1"/>
@@ -18563,7 +18563,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomRight" activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -18680,7 +18680,7 @@
         <v>1861</v>
       </c>
     </row>
-    <row r="3" ht="15.1" customHeight="1" spans="1:10">
+    <row r="3" ht="15.1" customHeight="1" spans="1:9">
       <c r="A3" s="4" t="s">
         <v>1862</v>
       </c>
@@ -18701,9 +18701,8 @@
         <v>1859</v>
       </c>
       <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
-    </row>
-    <row r="4" ht="15.1" customHeight="1" spans="1:10">
+    </row>
+    <row r="4" ht="15.1" customHeight="1" spans="1:9">
       <c r="A4" s="4" t="s">
         <v>1865</v>
       </c>
@@ -18724,9 +18723,8 @@
         <v>1859</v>
       </c>
       <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-    </row>
-    <row r="5" ht="15.1" customHeight="1" spans="1:10">
+    </row>
+    <row r="5" ht="15.1" customHeight="1" spans="1:9">
       <c r="A5" s="4" t="s">
         <v>1868</v>
       </c>
@@ -18747,7 +18745,6 @@
         <v>1859</v>
       </c>
       <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
     </row>
     <row r="6" ht="15.1" customHeight="1" spans="1:10">
       <c r="A6" s="4" t="s">
@@ -18851,7 +18848,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -18987,7 +18984,7 @@
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="C8" sqref="$A1:$XFD1048576"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="1"/>
@@ -19901,7 +19898,7 @@
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection/>
-      <selection pane="topRight" activeCell="E12" sqref="E12"/>
+      <selection pane="topRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelCol="1"/>
@@ -19984,7 +19981,7 @@
   <sheetPr/>
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
@@ -20113,7 +20110,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H2" sqref="H2:H3"/>
+      <selection pane="bottomRight" activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2"/>
@@ -26716,11 +26713,11 @@
   <dimension ref="A1:L127"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B74" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D84" sqref="D84"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2:G126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1"/>
@@ -30172,7 +30169,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G1" sqref="G1"/>
+      <selection pane="bottomRight" activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4"/>

</xml_diff>

<commit_message>
removing Author.orcid; renaming DatabaseReference --> Identifier
</commit_message>
<xml_diff>
--- a/tests/fixtures/example-model.xlsx
+++ b/tests/fixtures/example-model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13965" tabRatio="993"/>
+    <workbookView windowWidth="20295" windowHeight="6945" tabRatio="993" firstSheet="13" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="Table of contents" sheetId="23" r:id="rId1"/>
@@ -396,7 +396,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4682" uniqueCount="2068">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4681" uniqueCount="2067">
   <si>
     <t>Table</t>
   </si>
@@ -518,7 +518,7 @@
     <t>second</t>
   </si>
   <si>
-    <t>Database references</t>
+    <t>Identifiers</t>
   </si>
   <si>
     <t>Comments</t>
@@ -6575,9 +6575,6 @@
   </si>
   <si>
     <t>Address</t>
-  </si>
-  <si>
-    <t>ORCID</t>
   </si>
   <si>
     <t>Target</t>
@@ -6609,13 +6606,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -6681,7 +6678,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6696,6 +6701,67 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -6703,7 +6769,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6717,24 +6783,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6749,67 +6799,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6836,7 +6826,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6852,174 +7010,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -7030,11 +7020,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -7042,8 +7038,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -7073,6 +7069,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -7083,21 +7094,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -7113,149 +7109,143 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="27" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="27" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -7736,7 +7726,7 @@
   <sheetPr/>
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -20376,14 +20366,14 @@
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1"/>
@@ -20391,7 +20381,7 @@
     <col min="1" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:13">
+    <row r="1" customHeight="1" spans="1:12">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -20423,12 +20413,9 @@
         <v>2058</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>2059</v>
+        <v>40</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="M1" s="2" t="s">
         <v>41</v>
       </c>
     </row>
@@ -20467,25 +20454,25 @@
         <v>96</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>2059</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>2060</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>2061</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>2062</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>2063</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>2064</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>2065</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>2066</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>40</v>
@@ -20506,7 +20493,7 @@
         <v>23</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>2067</v>
+        <v>2066</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
renaming interpretation-->conclusion; renaming Method-->process; adding date to Conclusion
</commit_message>
<xml_diff>
--- a/tests/fixtures/example-model.xlsx
+++ b/tests/fixtures/example-model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13965" tabRatio="993" activeTab="6"/>
+    <workbookView windowWidth="28695" windowHeight="13965" tabRatio="993"/>
   </bookViews>
   <sheets>
     <sheet name="Table of contents" sheetId="23" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <sheet name="Parameters" sheetId="15" r:id="rId17"/>
     <sheet name="Stop conditions" sheetId="16" r:id="rId18"/>
     <sheet name="Evidence" sheetId="17" r:id="rId19"/>
-    <sheet name="Interpretations" sheetId="20" r:id="rId20"/>
+    <sheet name="Conclusions" sheetId="20" r:id="rId20"/>
     <sheet name="References" sheetId="18" r:id="rId21"/>
     <sheet name="Authors" sheetId="21" r:id="rId22"/>
     <sheet name="Changes" sheetId="22" r:id="rId23"/>
@@ -396,7 +396,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4635" uniqueCount="2009">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4636" uniqueCount="2009">
   <si>
     <t>Table</t>
   </si>
@@ -461,7 +461,7 @@
     <t>Evidence</t>
   </si>
   <si>
-    <t>Interpretations</t>
+    <t>Conclusions</t>
   </si>
   <si>
     <t>References</t>
@@ -5815,10 +5815,10 @@
     <t>Genotype</t>
   </si>
   <si>
-    <t>Measurement method</t>
-  </si>
-  <si>
-    <t>Analysis method</t>
+    <t>Data generation process</t>
+  </si>
+  <si>
+    <t>Data analysis process</t>
   </si>
   <si>
     <t>Variant</t>
@@ -5923,13 +5923,16 @@
     <t>Homo sapiens</t>
   </si>
   <si>
-    <t>Method</t>
-  </si>
-  <si>
-    <t>interpretation_001</t>
-  </si>
-  <si>
-    <t>Interpretation 001</t>
+    <t>Process</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>conclusion_001</t>
+  </si>
+  <si>
+    <t>Conclusion 001</t>
   </si>
   <si>
     <t>0.1</t>
@@ -5938,7 +5941,7 @@
     <t>assumption</t>
   </si>
   <si>
-    <t>interpretation_002</t>
+    <t>conclusion_002</t>
   </si>
   <si>
     <t>10</t>
@@ -6422,9 +6425,6 @@
   </si>
   <si>
     <t>Intention type</t>
-  </si>
-  <si>
-    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -6433,10 +6433,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -6503,17 +6503,23 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6527,16 +6533,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6551,33 +6588,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -6588,22 +6601,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6617,17 +6617,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -6652,7 +6652,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6664,13 +6706,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6682,151 +6820,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6846,6 +6846,24 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -6861,22 +6879,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -6898,9 +6911,20 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -6919,159 +6943,135 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -7552,10 +7552,10 @@
   <sheetPr/>
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1" outlineLevelCol="2"/>
@@ -7797,7 +7797,7 @@
     <hyperlink ref="A17" location="'Parameters'!A1" display="Parameters" tooltip="Click to view parameters"/>
     <hyperlink ref="A18" location="'Stop conditions'!A1" display="Stop conditions" tooltip="Click to view stop conditions"/>
     <hyperlink ref="A19" location="'Evidence'!A1" display="Evidence" tooltip="Click to view evidence"/>
-    <hyperlink ref="A20" location="'Interpretations'!A1" display="Interpretations" tooltip="Click to view interpretations"/>
+    <hyperlink ref="A20" location="'Interpretations'!A1" display="Conclusions" tooltip="Click to view interpretations"/>
     <hyperlink ref="A21" location="'References'!A1" display="References" tooltip="Click to view references"/>
     <hyperlink ref="A22" location="'Authors'!A1" display="Authors" tooltip="Click to view authors"/>
     <hyperlink ref="A23" location="'Changes'!A1" display="Changes" tooltip="Click to view changes"/>
@@ -18782,7 +18782,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J2" sqref="J2"/>
+      <selection pane="bottomRight" activeCell="Q1" sqref="Q1:T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -19209,14 +19209,14 @@
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomRight" activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -19235,7 +19235,7 @@
       </c>
       <c r="H1" s="7"/>
     </row>
-    <row r="2" ht="15.1" customHeight="1" spans="1:13">
+    <row r="2" ht="15.1" customHeight="1" spans="1:14">
       <c r="A2" s="5" t="s">
         <v>25</v>
       </c>
@@ -19275,25 +19275,28 @@
       <c r="M2" s="5" t="s">
         <v>23</v>
       </c>
+      <c r="N2" s="5" t="s">
+        <v>1842</v>
+      </c>
     </row>
     <row r="3" ht="15.1" customHeight="1" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>1842</v>
+        <v>1843</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1843</v>
+        <v>1844</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>1814</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>1844</v>
+        <v>1845</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>566</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>1845</v>
+        <v>1846</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>1818</v>
@@ -19301,13 +19304,13 @@
     </row>
     <row r="4" ht="15.1" customHeight="1" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>1846</v>
+        <v>1847</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1843</v>
+        <v>1844</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>1847</v>
+        <v>1848</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>1814</v>
@@ -19316,10 +19319,10 @@
         <v>39</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1848</v>
+        <v>1849</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>1849</v>
+        <v>1850</v>
       </c>
     </row>
     <row r="5" ht="15.1" customHeight="1" spans="3:4">
@@ -19388,46 +19391,46 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1850</v>
+        <v>1851</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1851</v>
+        <v>1852</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>1852</v>
+        <v>1853</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>1853</v>
+        <v>1854</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>98</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>1854</v>
+        <v>1855</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>1855</v>
+        <v>1856</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>1856</v>
+        <v>1857</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>1857</v>
+        <v>1858</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>1858</v>
+        <v>1859</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>1859</v>
+        <v>1860</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>1860</v>
+        <v>1861</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>1861</v>
+        <v>1862</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>1862</v>
+        <v>1863</v>
       </c>
       <c r="Q1" s="2" t="s">
         <v>40</v>
@@ -19438,26 +19441,26 @@
     </row>
     <row r="2" customHeight="1" spans="1:18">
       <c r="A2" s="1" t="s">
-        <v>1863</v>
+        <v>1864</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1864</v>
+        <v>1865</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>1865</v>
+        <v>1866</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>1866</v>
+        <v>1867</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1">
         <v>2008</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>1867</v>
+        <v>1868</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>1868</v>
+        <v>1869</v>
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -19471,35 +19474,35 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1" t="s">
-        <v>1869</v>
+        <v>1870</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>1870</v>
+        <v>1871</v>
       </c>
       <c r="R2" s="1"/>
     </row>
     <row r="3" customHeight="1" spans="1:18">
       <c r="A3" s="1" t="s">
-        <v>1871</v>
+        <v>1872</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1872</v>
+        <v>1873</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1873</v>
+        <v>1874</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>1874</v>
+        <v>1875</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1">
         <v>2014</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>1867</v>
+        <v>1868</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1875</v>
+        <v>1876</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -19509,124 +19512,124 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1" t="s">
-        <v>1876</v>
+        <v>1877</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>1877</v>
+        <v>1878</v>
       </c>
       <c r="R3" s="1"/>
     </row>
     <row r="4" customHeight="1" spans="1:18">
       <c r="A4" s="1" t="s">
-        <v>1878</v>
+        <v>1879</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1879</v>
+        <v>1880</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1880</v>
+        <v>1881</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>1881</v>
+        <v>1882</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1">
         <v>2004</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>1867</v>
+        <v>1868</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>1875</v>
+        <v>1876</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1" t="s">
-        <v>1882</v>
+        <v>1883</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>1883</v>
+        <v>1884</v>
       </c>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1" t="s">
-        <v>1884</v>
+        <v>1885</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>1885</v>
+        <v>1886</v>
       </c>
       <c r="R4" s="1"/>
     </row>
     <row r="5" customHeight="1" spans="1:18">
       <c r="A5" s="1" t="s">
-        <v>1886</v>
+        <v>1887</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1887</v>
+        <v>1888</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1888</v>
+        <v>1889</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>1889</v>
+        <v>1890</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1">
         <v>2009</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>1867</v>
+        <v>1868</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>1890</v>
+        <v>1891</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1" t="s">
-        <v>1891</v>
+        <v>1892</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>1892</v>
+        <v>1893</v>
       </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1" t="s">
-        <v>1893</v>
+        <v>1894</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>1894</v>
+        <v>1895</v>
       </c>
       <c r="R5" s="1"/>
     </row>
     <row r="6" customHeight="1" spans="1:18">
       <c r="A6" s="1" t="s">
-        <v>1895</v>
+        <v>1896</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1896</v>
+        <v>1897</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1897</v>
+        <v>1898</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>1898</v>
+        <v>1899</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1">
         <v>2007</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>1867</v>
+        <v>1868</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>1899</v>
+        <v>1900</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1" t="s">
-        <v>1900</v>
+        <v>1901</v>
       </c>
       <c r="L6" s="1" t="s">
         <v>1814</v>
@@ -19636,7 +19639,7 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1" t="s">
-        <v>1901</v>
+        <v>1902</v>
       </c>
       <c r="R6" s="1"/>
     </row>
@@ -19645,24 +19648,24 @@
         <v>1652</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1902</v>
+        <v>1903</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1903</v>
+        <v>1904</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>1904</v>
+        <v>1905</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1">
         <v>2001</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>1905</v>
+        <v>1906</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1" t="s">
-        <v>1906</v>
+        <v>1907</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -19672,7 +19675,7 @@
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1" t="s">
-        <v>1907</v>
+        <v>1908</v>
       </c>
       <c r="R7" s="1"/>
     </row>
@@ -19681,26 +19684,26 @@
         <v>1666</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>1908</v>
+        <v>1909</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1909</v>
+        <v>1910</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>1910</v>
+        <v>1911</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1">
         <v>2006</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>1905</v>
+        <v>1906</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>1911</v>
+        <v>1912</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>1912</v>
+        <v>1913</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -19710,37 +19713,37 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1" t="s">
-        <v>1913</v>
+        <v>1914</v>
       </c>
       <c r="R8" s="1"/>
     </row>
     <row r="9" customHeight="1" spans="1:18">
       <c r="A9" s="1" t="s">
-        <v>1914</v>
+        <v>1915</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1915</v>
+        <v>1916</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1916</v>
+        <v>1917</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>1917</v>
+        <v>1918</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1">
         <v>1993</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1867</v>
+        <v>1868</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>1918</v>
+        <v>1919</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1" t="s">
-        <v>1919</v>
+        <v>1920</v>
       </c>
       <c r="L9" s="1" t="s">
         <v>1814</v>
@@ -19749,119 +19752,119 @@
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1" t="s">
-        <v>1920</v>
+        <v>1921</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>1921</v>
+        <v>1922</v>
       </c>
       <c r="R9" s="1"/>
     </row>
     <row r="10" customHeight="1" spans="1:18">
       <c r="A10" s="1" t="s">
-        <v>1922</v>
+        <v>1923</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1923</v>
+        <v>1924</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1924</v>
+        <v>1925</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>1925</v>
+        <v>1926</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1">
         <v>2010</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>1867</v>
+        <v>1868</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>1926</v>
+        <v>1927</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1" t="s">
-        <v>1927</v>
+        <v>1928</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>1900</v>
+        <v>1901</v>
       </c>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1" t="s">
-        <v>1928</v>
+        <v>1929</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>1929</v>
+        <v>1930</v>
       </c>
       <c r="R10" s="1"/>
     </row>
     <row r="11" customHeight="1" spans="1:18">
       <c r="A11" s="1" t="s">
-        <v>1930</v>
+        <v>1931</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>1931</v>
+        <v>1932</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1932</v>
+        <v>1933</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>1933</v>
+        <v>1934</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1">
         <v>2000</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>1867</v>
+        <v>1868</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>1934</v>
+        <v>1935</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1" t="s">
-        <v>1935</v>
+        <v>1936</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>1936</v>
+        <v>1937</v>
       </c>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1" t="s">
-        <v>1937</v>
+        <v>1938</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>1938</v>
+        <v>1939</v>
       </c>
       <c r="R11" s="1"/>
     </row>
     <row r="12" customHeight="1" spans="1:18">
       <c r="A12" s="1" t="s">
-        <v>1939</v>
+        <v>1940</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>1940</v>
+        <v>1941</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1941</v>
+        <v>1942</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>1942</v>
+        <v>1943</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1">
         <v>1999</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>1867</v>
+        <v>1868</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>1943</v>
+        <v>1944</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -19869,58 +19872,58 @@
         <v>1814</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>1900</v>
+        <v>1901</v>
       </c>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1" t="s">
-        <v>1944</v>
+        <v>1945</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>1945</v>
+        <v>1946</v>
       </c>
       <c r="R12" s="1"/>
     </row>
     <row r="13" customHeight="1" spans="1:18">
       <c r="A13" s="1" t="s">
-        <v>1946</v>
+        <v>1947</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>1947</v>
+        <v>1948</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1948</v>
+        <v>1949</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>1949</v>
+        <v>1950</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1">
         <v>1979</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>1867</v>
+        <v>1868</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>1934</v>
+        <v>1935</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1" t="s">
-        <v>1950</v>
+        <v>1951</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>1951</v>
+        <v>1952</v>
       </c>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1" t="s">
-        <v>1952</v>
+        <v>1953</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>1953</v>
+        <v>1954</v>
       </c>
       <c r="R13" s="1"/>
     </row>
@@ -19929,40 +19932,40 @@
         <v>103</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>1954</v>
+        <v>1955</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1955</v>
+        <v>1956</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>1956</v>
+        <v>1957</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1">
         <v>2012</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>1867</v>
+        <v>1868</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>1957</v>
+        <v>1958</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1" t="s">
-        <v>1958</v>
+        <v>1959</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>1892</v>
+        <v>1893</v>
       </c>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1" t="s">
-        <v>1959</v>
+        <v>1960</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>1960</v>
+        <v>1961</v>
       </c>
       <c r="R14" s="1"/>
     </row>
@@ -19971,56 +19974,56 @@
         <v>202</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>1961</v>
+        <v>1962</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1962</v>
+        <v>1963</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>1963</v>
+        <v>1964</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1">
         <v>2009</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>1867</v>
+        <v>1868</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>1964</v>
+        <v>1965</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1" t="s">
-        <v>1965</v>
+        <v>1966</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>1966</v>
+        <v>1967</v>
       </c>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1" t="s">
-        <v>1967</v>
+        <v>1968</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>1968</v>
+        <v>1969</v>
       </c>
       <c r="R15" s="1"/>
     </row>
     <row r="16" customHeight="1" spans="1:18">
       <c r="A16" s="1" t="s">
-        <v>1969</v>
+        <v>1970</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>1970</v>
+        <v>1971</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
-        <v>1971</v>
+        <v>1972</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -20032,23 +20035,23 @@
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1" t="s">
-        <v>1972</v>
+        <v>1973</v>
       </c>
       <c r="R16" s="1"/>
     </row>
     <row r="17" customHeight="1" spans="1:18">
       <c r="A17" s="1" t="s">
-        <v>1973</v>
+        <v>1974</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>1974</v>
+        <v>1975</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>1971</v>
+        <v>1972</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -20060,23 +20063,23 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1" t="s">
-        <v>1975</v>
+        <v>1976</v>
       </c>
       <c r="R17" s="1"/>
     </row>
     <row r="18" customHeight="1" spans="1:18">
       <c r="A18" s="1" t="s">
-        <v>1976</v>
+        <v>1977</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>1977</v>
+        <v>1978</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
-        <v>1971</v>
+        <v>1972</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -20088,23 +20091,23 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1" t="s">
-        <v>1978</v>
+        <v>1979</v>
       </c>
       <c r="R18" s="1"/>
     </row>
     <row r="19" customHeight="1" spans="1:18">
       <c r="A19" s="1" t="s">
-        <v>1979</v>
+        <v>1980</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>1980</v>
+        <v>1981</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
-        <v>1971</v>
+        <v>1972</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -20116,7 +20119,7 @@
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1" t="s">
-        <v>1981</v>
+        <v>1982</v>
       </c>
       <c r="R19" s="1"/>
     </row>
@@ -20126,13 +20129,13 @@
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>1982</v>
+        <v>1983</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
-        <v>1971</v>
+        <v>1972</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -20144,54 +20147,54 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1" t="s">
-        <v>1983</v>
+        <v>1984</v>
       </c>
       <c r="R20" s="1"/>
     </row>
     <row r="21" customHeight="1" spans="1:17">
       <c r="A21" s="3" t="s">
-        <v>1984</v>
+        <v>1985</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>1985</v>
+        <v>1986</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>1986</v>
+        <v>1987</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>1987</v>
+        <v>1988</v>
       </c>
       <c r="F21" s="3">
         <v>2015</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>1971</v>
+        <v>1972</v>
       </c>
       <c r="Q21" s="3" t="s">
-        <v>1988</v>
+        <v>1989</v>
       </c>
     </row>
     <row r="22" customHeight="1" spans="1:17">
       <c r="A22" s="3" t="s">
-        <v>1989</v>
+        <v>1990</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>1990</v>
+        <v>1991</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>1991</v>
+        <v>1992</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>1992</v>
+        <v>1993</v>
       </c>
       <c r="F22" s="3">
         <v>2018</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>1971</v>
+        <v>1972</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>1993</v>
+        <v>1994</v>
       </c>
     </row>
   </sheetData>
@@ -20234,28 +20237,28 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1994</v>
+        <v>1995</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1995</v>
+        <v>1996</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>1996</v>
+        <v>1997</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>1850</v>
+        <v>1851</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>1998</v>
+        <v>1999</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>1999</v>
+        <v>2000</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>2000</v>
+        <v>2001</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>40</v>
@@ -20299,25 +20302,25 @@
         <v>98</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>2002</v>
+        <v>2003</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>2005</v>
+        <v>2006</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>2006</v>
+        <v>2007</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>2007</v>
+        <v>2008</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>40</v>
@@ -20338,7 +20341,7 @@
         <v>23</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>2008</v>
+        <v>1842</v>
       </c>
     </row>
   </sheetData>
@@ -20846,12 +20849,12 @@
   <sheetPr/>
   <dimension ref="A1:N145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B137" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C3" sqref="C3:G152"/>
+      <selection pane="bottomRight" activeCell="E150" sqref="E150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
updating for changes to obj_model
</commit_message>
<xml_diff>
--- a/tests/fixtures/example-model.xlsx
+++ b/tests/fixtures/example-model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="14070" tabRatio="993"/>
+    <workbookView windowWidth="20295" windowHeight="6945" tabRatio="993"/>
   </bookViews>
   <sheets>
     <sheet name="Table of contents" sheetId="23" r:id="rId1"/>
@@ -6454,11 +6454,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -6512,31 +6512,23 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -6548,17 +6540,10 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -6570,17 +6555,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6601,23 +6577,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6632,7 +6601,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6646,10 +6631,25 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -6674,7 +6674,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6686,7 +6686,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6698,13 +6758,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6716,7 +6776,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6728,19 +6800,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6752,79 +6836,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6836,25 +6854,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6886,17 +6886,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -6916,21 +6916,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -6938,15 +6923,6 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -6965,139 +6941,163 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -7575,9 +7575,9 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" zeroHeight="1" outlineLevelCol="2"/>
@@ -7603,6 +7603,7 @@
       </c>
       <c r="B2" s="24"/>
       <c r="C2" s="24">
+        <f>COUNTA(Model!B1:XFD1)</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updating for obj_tables changes
</commit_message>
<xml_diff>
--- a/tests/fixtures/example-model.xlsx
+++ b/tests/fixtures/example-model.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="20295" windowHeight="6945" tabRatio="993"/>
+    <workbookView windowWidth="28695" windowHeight="13965" tabRatio="993"/>
   </bookViews>
   <sheets>
-    <sheet name="Table of contents" sheetId="23" r:id="rId1"/>
+    <sheet name="!_Table of contents" sheetId="23" r:id="rId1"/>
     <sheet name="Model" sheetId="1" r:id="rId2"/>
     <sheet name="Taxon" sheetId="2" r:id="rId3"/>
     <sheet name="Environment" sheetId="19" r:id="rId4"/>
@@ -37,7 +37,7 @@
     <externalReference r:id="rId25"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Table of contents'!$A$1:$C$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'!_Table of contents'!$A$1:$C$24</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Model!$A$1:$B$12</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Submodels!$A$1:$H$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Compartments!$A$2:$U$4</definedName>
@@ -6456,9 +6456,9 @@
   <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -6512,13 +6512,74 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6533,30 +6594,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6570,15 +6608,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6593,53 +6639,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -6647,7 +6647,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -6674,31 +6674,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6710,13 +6698,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6734,37 +6728,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6776,37 +6740,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6824,7 +6770,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6836,25 +6800,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -6865,80 +6865,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -6960,144 +6886,218 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>

</xml_diff>

<commit_message>
Correct the units for dfba_obj_species
</commit_message>
<xml_diff>
--- a/tests/fixtures/example-model.xlsx
+++ b/tests/fixtures/example-model.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonrk\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\karrlab\wc_lang\tests\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C7410F9-8521-4535-9997-9E487E3B4869}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="993" firstSheet="14" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -405,7 +404,7 @@
     <definedName name="_FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" localSheetId="4">'[9]#REF'!$A$1:$H$5</definedName>
     <definedName name="_FilterDatabase_1" localSheetId="16">'[4]#REF'!$A$1:$K$5</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -5191,9 +5190,6 @@
     <t>ALA net component</t>
   </si>
   <si>
-    <t>molar / second</t>
-  </si>
-  <si>
     <t>test</t>
   </si>
   <si>
@@ -6566,12 +6562,15 @@
   </si>
   <si>
     <t>!Intention type</t>
+  </si>
+  <si>
+    <t>mole / gDCW</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
@@ -7145,10 +7144,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -7389,37 +7388,37 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C26" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:C26"/>
   <hyperlinks>
-    <hyperlink ref="A2" location="'Model'!A1" tooltip="Click to view model" display="!!ObjTables Type='Schema' ObjTablesVersion='0.0.8'" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="A3" location="'Taxon'!A1" tooltip="Click to view taxon" display="!Table" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="A4" location="'Environment'!A1" tooltip="Click to view environment" display="Model" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="A5" location="'Submodels'!A1" tooltip="Click to view submodels" display="Taxon" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="A6" location="'Compartments'!A1" tooltip="Click to view compartments" display="Environment" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="A7" location="'Species types'!A1" tooltip="Click to view species types" display="Submodels" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="A8" location="'Species'!A1" tooltip="Click to view species" display="Compartments" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="A9" location="'Initial species concentrations'!A1" tooltip="Click to view initial species concentrations" display="Species types" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="A10" location="'Observables'!A1" tooltip="Click to view observables" display="Species" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="A11" location="'Functions'!A1" tooltip="Click to view functions" display="Initial species concentrations" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="A12" location="'Reactions'!A1" tooltip="Click to view reactions" display="Observables" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="A13" location="'Rate laws'!A1" tooltip="Click to view rate laws" display="Functions" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="A14" location="'dFBA objectives'!A1" tooltip="Click to view dfba objectives" display="Reactions" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="A15" location="'dFBA objective reactions'!A1" tooltip="Click to view dfba objective reactions" display="Rate laws" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="A16" location="'dFBA objective species'!A1" tooltip="Click to view dfba objective species" display="dFBA objectives" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="A17" location="'Parameters'!A1" tooltip="Click to view parameters" display="dFBA objective reactions" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="A18" location="'Stop conditions'!A1" tooltip="Click to view stop conditions" display="dFBA objective species" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="A19" location="'Evidence'!A1" tooltip="Click to view evidence" display="Parameters" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="A21" location="'Interpretations'!A1" tooltip="Click to view interpretations" display="Observations" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="A22" location="'References'!A1" tooltip="Click to view references" display="Observation sets" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="A23" location="'Authors'!A1" tooltip="Click to view authors" display="Conclusions" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="A24" location="'Changes'!A1" tooltip="Click to view changes" display="References" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="A2" location="'Model'!A1" tooltip="Click to view model" display="!!ObjTables Type='Schema' ObjTablesVersion='0.0.8'"/>
+    <hyperlink ref="A3" location="'Taxon'!A1" tooltip="Click to view taxon" display="!Table"/>
+    <hyperlink ref="A4" location="'Environment'!A1" tooltip="Click to view environment" display="Model"/>
+    <hyperlink ref="A5" location="'Submodels'!A1" tooltip="Click to view submodels" display="Taxon"/>
+    <hyperlink ref="A6" location="'Compartments'!A1" tooltip="Click to view compartments" display="Environment"/>
+    <hyperlink ref="A7" location="'Species types'!A1" tooltip="Click to view species types" display="Submodels"/>
+    <hyperlink ref="A8" location="'Species'!A1" tooltip="Click to view species" display="Compartments"/>
+    <hyperlink ref="A9" location="'Initial species concentrations'!A1" tooltip="Click to view initial species concentrations" display="Species types"/>
+    <hyperlink ref="A10" location="'Observables'!A1" tooltip="Click to view observables" display="Species"/>
+    <hyperlink ref="A11" location="'Functions'!A1" tooltip="Click to view functions" display="Initial species concentrations"/>
+    <hyperlink ref="A12" location="'Reactions'!A1" tooltip="Click to view reactions" display="Observables"/>
+    <hyperlink ref="A13" location="'Rate laws'!A1" tooltip="Click to view rate laws" display="Functions"/>
+    <hyperlink ref="A14" location="'dFBA objectives'!A1" tooltip="Click to view dfba objectives" display="Reactions"/>
+    <hyperlink ref="A15" location="'dFBA objective reactions'!A1" tooltip="Click to view dfba objective reactions" display="Rate laws"/>
+    <hyperlink ref="A16" location="'dFBA objective species'!A1" tooltip="Click to view dfba objective species" display="dFBA objectives"/>
+    <hyperlink ref="A17" location="'Parameters'!A1" tooltip="Click to view parameters" display="dFBA objective reactions"/>
+    <hyperlink ref="A18" location="'Stop conditions'!A1" tooltip="Click to view stop conditions" display="dFBA objective species"/>
+    <hyperlink ref="A19" location="'Evidence'!A1" tooltip="Click to view evidence" display="Parameters"/>
+    <hyperlink ref="A21" location="'Interpretations'!A1" tooltip="Click to view interpretations" display="Observations"/>
+    <hyperlink ref="A22" location="'References'!A1" tooltip="Click to view references" display="Observation sets"/>
+    <hyperlink ref="A23" location="'Authors'!A1" tooltip="Click to view authors" display="Conclusions"/>
+    <hyperlink ref="A24" location="'Changes'!A1" tooltip="Click to view changes" display="References"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AML6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7545,7 +7544,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7677,7 +7676,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AMM178"/>
   <sheetViews>
@@ -12604,7 +12603,7 @@
       <c r="N178" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:N178" xr:uid="{00000000-0009-0000-0000-00000B000000}">
+  <autoFilter ref="A2:N178">
     <filterColumn colId="2">
       <customFilters and="1">
         <customFilter val="Metabolism"/>
@@ -12621,7 +12620,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AML169"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15536,14 +15535,14 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:L169" xr:uid="{00000000-0009-0000-0000-00000C000000}"/>
+  <autoFilter ref="C1:L169"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMN3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15635,7 +15634,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AML4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -15738,14 +15737,14 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AML37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -15820,21 +15819,21 @@
         <v>-34190.379999999997</v>
       </c>
       <c r="F3" s="13" t="s">
+        <v>2047</v>
+      </c>
+      <c r="J3" s="10" t="s">
         <v>1589</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="K3" s="10" t="s">
         <v>1590</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>1591</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="15.2" customHeight="1">
       <c r="A4" s="10" t="s">
+        <v>1591</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>1592</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>1593</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>1579</v>
@@ -15846,15 +15845,15 @@
         <v>1035619</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>1589</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.2" customHeight="1">
       <c r="A5" s="10" t="s">
+        <v>1593</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>1594</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>1595</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>1579</v>
@@ -15866,15 +15865,15 @@
         <v>-40890.379999999997</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>1589</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.2" customHeight="1">
       <c r="A6" s="10" t="s">
+        <v>1595</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>1596</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>1597</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>1579</v>
@@ -15886,15 +15885,15 @@
         <v>-23190.38</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>1589</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.2" customHeight="1">
       <c r="A7" s="10" t="s">
+        <v>1597</v>
+      </c>
+      <c r="B7" s="10" t="s">
         <v>1598</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>1599</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>1579</v>
@@ -15906,15 +15905,15 @@
         <v>-24290.38</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>1589</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.2" customHeight="1">
       <c r="A8" s="10" t="s">
+        <v>1599</v>
+      </c>
+      <c r="B8" s="10" t="s">
         <v>1600</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>1601</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>1579</v>
@@ -15926,15 +15925,15 @@
         <v>-1101856</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>1589</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.2" customHeight="1">
       <c r="A9" s="10" t="s">
+        <v>1601</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>1602</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>1603</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>1579</v>
@@ -15946,15 +15945,15 @@
         <v>1098019</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>1589</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.2" customHeight="1">
       <c r="A10" s="10" t="s">
+        <v>1603</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>1604</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>1605</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>1579</v>
@@ -15966,15 +15965,15 @@
         <v>-1164906</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>1589</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.2" customHeight="1">
       <c r="A11" s="10" t="s">
+        <v>1605</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>1606</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>1607</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>1579</v>
@@ -15986,15 +15985,15 @@
         <v>-22290.38</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>1589</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.2" customHeight="1">
       <c r="A12" s="10" t="s">
+        <v>1607</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>1608</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>1609</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>1579</v>
@@ -16006,15 +16005,15 @@
         <v>581419.19999999995</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>1589</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.2" customHeight="1">
       <c r="A13" s="10" t="s">
+        <v>1609</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>1610</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>1611</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>1579</v>
@@ -16026,15 +16025,15 @@
         <v>-24690.38</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>1589</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.2" customHeight="1">
       <c r="A14" s="10" t="s">
+        <v>1611</v>
+      </c>
+      <c r="B14" s="10" t="s">
         <v>1612</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>1613</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>1579</v>
@@ -16046,15 +16045,15 @@
         <v>-22690.38</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>1589</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.2" customHeight="1">
       <c r="A15" s="10" t="s">
+        <v>1613</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>1614</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>1615</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>1579</v>
@@ -16066,15 +16065,15 @@
         <v>-31190.38</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>1589</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.2" customHeight="1">
       <c r="A16" s="10" t="s">
+        <v>1615</v>
+      </c>
+      <c r="B16" s="10" t="s">
         <v>1616</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>1617</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>1579</v>
@@ -16086,15 +16085,15 @@
         <v>1052899</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>1589</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.2" customHeight="1">
       <c r="A17" s="10" t="s">
+        <v>1617</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>1618</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>1619</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>1579</v>
@@ -16106,15 +16105,15 @@
         <v>-1728316</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>1589</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.2" customHeight="1">
       <c r="A18" s="10" t="s">
+        <v>1619</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>1620</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>1621</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>1579</v>
@@ -16126,15 +16125,15 @@
         <v>-1521617000</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>1589</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.2" customHeight="1">
       <c r="A19" s="10" t="s">
+        <v>1621</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>1622</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>1623</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>1579</v>
@@ -16146,15 +16145,15 @@
         <v>4972350</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>1589</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.2" customHeight="1">
       <c r="A20" s="10" t="s">
+        <v>1623</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>1624</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>1625</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>1579</v>
@@ -16166,15 +16165,15 @@
         <v>-21590.38</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>1589</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.2" customHeight="1">
       <c r="A21" s="10" t="s">
+        <v>1625</v>
+      </c>
+      <c r="B21" s="10" t="s">
         <v>1626</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>1627</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>1579</v>
@@ -16186,15 +16185,15 @@
         <v>-29290.38</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>1589</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.2" customHeight="1">
       <c r="A22" s="10" t="s">
+        <v>1627</v>
+      </c>
+      <c r="B22" s="10" t="s">
         <v>1628</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>1629</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>1579</v>
@@ -16206,15 +16205,15 @@
         <v>-41190.379999999997</v>
       </c>
       <c r="F22" s="13" t="s">
-        <v>1589</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.2" customHeight="1">
       <c r="A23" s="10" t="s">
+        <v>1629</v>
+      </c>
+      <c r="B23" s="10" t="s">
         <v>1630</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>1631</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>1579</v>
@@ -16226,15 +16225,15 @@
         <v>-21990.38</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>1589</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.2" customHeight="1">
       <c r="A24" s="10" t="s">
+        <v>1631</v>
+      </c>
+      <c r="B24" s="10" t="s">
         <v>1632</v>
-      </c>
-      <c r="B24" s="10" t="s">
-        <v>1633</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>1579</v>
@@ -16246,15 +16245,15 @@
         <v>-21390.38</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>1589</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.2" customHeight="1">
       <c r="A25" s="10" t="s">
+        <v>1633</v>
+      </c>
+      <c r="B25" s="10" t="s">
         <v>1634</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>1635</v>
       </c>
       <c r="C25" s="12" t="s">
         <v>1579</v>
@@ -16266,15 +16265,15 @@
         <v>-23890.38</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>1589</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.2" customHeight="1">
       <c r="A26" s="10" t="s">
+        <v>1635</v>
+      </c>
+      <c r="B26" s="10" t="s">
         <v>1636</v>
-      </c>
-      <c r="B26" s="10" t="s">
-        <v>1637</v>
       </c>
       <c r="C26" s="12" t="s">
         <v>1579</v>
@@ -16286,15 +16285,15 @@
         <v>471096.2</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>1589</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.2" customHeight="1">
       <c r="A27" s="10" t="s">
+        <v>1637</v>
+      </c>
+      <c r="B27" s="10" t="s">
         <v>1638</v>
-      </c>
-      <c r="B27" s="10" t="s">
-        <v>1639</v>
       </c>
       <c r="C27" s="12" t="s">
         <v>1579</v>
@@ -16306,15 +16305,15 @@
         <v>4381069</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>1589</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15.2" customHeight="1">
       <c r="A28" s="10" t="s">
+        <v>1639</v>
+      </c>
+      <c r="B28" s="10" t="s">
         <v>1640</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>1641</v>
       </c>
       <c r="C28" s="12" t="s">
         <v>1579</v>
@@ -16326,15 +16325,15 @@
         <v>-34390.379999999997</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>1589</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.2" customHeight="1">
       <c r="A29" s="10" t="s">
+        <v>1641</v>
+      </c>
+      <c r="B29" s="10" t="s">
         <v>1642</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>1643</v>
       </c>
       <c r="C29" s="12" t="s">
         <v>1579</v>
@@ -16346,15 +16345,15 @@
         <v>-44490.38</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>1589</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.2" customHeight="1">
       <c r="A30" s="10" t="s">
+        <v>1643</v>
+      </c>
+      <c r="B30" s="10" t="s">
         <v>1644</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>1645</v>
       </c>
       <c r="C30" s="12" t="s">
         <v>1579</v>
@@ -16366,15 +16365,15 @@
         <v>-36190.379999999997</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>1589</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.2" customHeight="1">
       <c r="A31" s="10" t="s">
+        <v>1645</v>
+      </c>
+      <c r="B31" s="10" t="s">
         <v>1646</v>
-      </c>
-      <c r="B31" s="10" t="s">
-        <v>1647</v>
       </c>
       <c r="C31" s="12" t="s">
         <v>1579</v>
@@ -16386,15 +16385,15 @@
         <v>-22190.38</v>
       </c>
       <c r="F31" s="13" t="s">
-        <v>1589</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15.2" customHeight="1">
       <c r="A32" s="10" t="s">
+        <v>1647</v>
+      </c>
+      <c r="B32" s="10" t="s">
         <v>1648</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>1649</v>
       </c>
       <c r="C32" s="12" t="s">
         <v>1579</v>
@@ -16406,15 +16405,15 @@
         <v>-21990.38</v>
       </c>
       <c r="F32" s="13" t="s">
-        <v>1589</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.2" customHeight="1">
       <c r="A33" s="10" t="s">
+        <v>1649</v>
+      </c>
+      <c r="B33" s="10" t="s">
         <v>1650</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>1651</v>
       </c>
       <c r="C33" s="12" t="s">
         <v>1579</v>
@@ -16426,15 +16425,15 @@
         <v>1066339</v>
       </c>
       <c r="F33" s="13" t="s">
-        <v>1589</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15.2" customHeight="1">
       <c r="A34" s="10" t="s">
+        <v>1651</v>
+      </c>
+      <c r="B34" s="10" t="s">
         <v>1652</v>
-      </c>
-      <c r="B34" s="10" t="s">
-        <v>1653</v>
       </c>
       <c r="C34" s="12" t="s">
         <v>1579</v>
@@ -16446,15 +16445,15 @@
         <v>-1132896</v>
       </c>
       <c r="F34" s="13" t="s">
-        <v>1589</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.2" customHeight="1">
       <c r="A35" s="10" t="s">
+        <v>1653</v>
+      </c>
+      <c r="B35" s="10" t="s">
         <v>1654</v>
-      </c>
-      <c r="B35" s="10" t="s">
-        <v>1655</v>
       </c>
       <c r="C35" s="12" t="s">
         <v>1579</v>
@@ -16466,15 +16465,15 @@
         <v>-33790.379999999997</v>
       </c>
       <c r="F35" s="13" t="s">
-        <v>1589</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15.2" customHeight="1">
       <c r="A36" s="10" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
       <c r="C36" s="12" t="s">
         <v>1582</v>
@@ -16486,15 +16485,15 @@
         <v>4381069</v>
       </c>
       <c r="F36" s="13" t="s">
-        <v>1589</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="31.5" customHeight="1">
       <c r="A37" s="10" t="s">
-        <v>1657</v>
+        <v>1656</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="C37" s="12" t="s">
         <v>1582</v>
@@ -16506,7 +16505,7 @@
         <v>1066339</v>
       </c>
       <c r="F37" s="13" t="s">
-        <v>1589</v>
+        <v>2047</v>
       </c>
     </row>
   </sheetData>
@@ -16516,7 +16515,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AML97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16539,7 +16538,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1">
       <c r="A1" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="31.5" customHeight="1">
@@ -16556,7 +16555,7 @@
         <v>104</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>82</v>
@@ -16579,41 +16578,41 @@
     </row>
     <row r="3" spans="1:11" ht="31.5" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
       <c r="D3" s="9">
         <v>6.02214075862E+23</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="409.5" customHeight="1">
       <c r="A4" s="1" t="s">
+        <v>1661</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>1662</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>1663</v>
       </c>
       <c r="D4" s="1">
         <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>1663</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>1664</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>1665</v>
-      </c>
       <c r="K4" s="1" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="31.5" customHeight="1">
       <c r="A5" s="1" t="s">
+        <v>1665</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>1666</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>1667</v>
       </c>
       <c r="D5" s="1">
         <v>28800</v>
@@ -16630,7 +16629,7 @@
         <v>1100</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="31.5" customHeight="1">
@@ -16641,15 +16640,15 @@
         <v>1100</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="63" customHeight="1">
       <c r="A8" s="1" t="s">
+        <v>1668</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>1669</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>1670</v>
       </c>
       <c r="D8" s="1">
         <v>0.3</v>
@@ -16658,12 +16657,12 @@
         <v>94</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
       <c r="B9" s="8"/>
       <c r="D9" s="1">
@@ -16677,7 +16676,7 @@
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
       <c r="B10" s="8"/>
       <c r="D10" s="1">
@@ -16691,1510 +16690,1510 @@
     </row>
     <row r="11" spans="1:11" ht="47.25" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
       <c r="B11" s="8"/>
       <c r="C11" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D11" s="1">
         <v>1</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
     </row>
     <row r="12" spans="1:11" ht="47.25" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
     </row>
     <row r="13" spans="1:11" ht="47.25" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>1678</v>
+        <v>1677</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D13" s="1">
         <v>1</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
     </row>
     <row r="14" spans="1:11" ht="47.25" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D14" s="1">
         <v>1</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
     </row>
     <row r="15" spans="1:11" ht="47.25" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>1680</v>
+        <v>1679</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
     </row>
     <row r="16" spans="1:11" ht="47.25" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D16" s="1">
         <v>1</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
     </row>
     <row r="17" spans="1:11" ht="47.25" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D17" s="1">
         <v>1</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
     </row>
     <row r="18" spans="1:11" ht="47.25" customHeight="1">
       <c r="A18" s="1" t="s">
+        <v>1682</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>1683</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>1684</v>
-      </c>
       <c r="C18" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D18" s="1">
         <v>250</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J18" s="8"/>
       <c r="K18" s="1" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="47.25" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D19" s="1">
         <v>1</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
     </row>
     <row r="20" spans="1:11" ht="47.25" customHeight="1">
       <c r="A20" s="1" t="s">
+        <v>1686</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>1687</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>1688</v>
-      </c>
       <c r="C20" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D20" s="1">
         <v>180</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J20" s="8"/>
       <c r="K20" s="1" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="110.25" customHeight="1">
       <c r="A21" s="1" t="s">
+        <v>1688</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>1689</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>1690</v>
-      </c>
       <c r="C21" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D21" s="1">
         <v>1005.6</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J21" s="1" t="s">
+        <v>1690</v>
+      </c>
+      <c r="K21" s="1" t="s">
         <v>1691</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>1692</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="157.5" customHeight="1">
       <c r="A22" s="1" t="s">
+        <v>1692</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>1693</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>1694</v>
-      </c>
       <c r="C22" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D22" s="1">
         <v>4200</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J22" s="1" t="s">
+        <v>1694</v>
+      </c>
+      <c r="K22" s="1" t="s">
         <v>1695</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>1696</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="47.25" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D23" s="1">
         <v>1</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
     </row>
     <row r="24" spans="1:11" ht="47.25" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>1698</v>
+        <v>1697</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D24" s="1">
         <v>1</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
     </row>
     <row r="25" spans="1:11" ht="47.25" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D25" s="1">
         <v>1</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
     </row>
     <row r="26" spans="1:11" ht="47.25" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D26" s="1">
         <v>1</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J26" s="8"/>
       <c r="K26" s="8"/>
     </row>
     <row r="27" spans="1:11" ht="47.25" customHeight="1">
       <c r="A27" s="1" t="s">
+        <v>1700</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>1701</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>1702</v>
-      </c>
       <c r="C27" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D27" s="1">
         <v>13200</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>1703</v>
+        <v>1702</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="94.5" customHeight="1">
       <c r="A28" s="1" t="s">
+        <v>1703</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>1704</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>1705</v>
-      </c>
       <c r="C28" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D28" s="1">
         <v>0.27600000000000002</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>1706</v>
+        <v>1705</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="47.25" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D29" s="1">
         <v>1</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J29" s="8"/>
       <c r="K29" s="8"/>
     </row>
     <row r="30" spans="1:11" ht="47.25" customHeight="1">
       <c r="A30" s="1" t="s">
+        <v>1707</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>1708</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>1709</v>
-      </c>
       <c r="C30" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D30" s="1">
         <v>628.79999999999995</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="47.25" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="B31" s="8"/>
       <c r="C31" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D31" s="1">
         <v>1</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J31" s="8"/>
       <c r="K31" s="8"/>
     </row>
     <row r="32" spans="1:11" ht="47.25" customHeight="1">
       <c r="A32" s="1" t="s">
+        <v>1711</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>1712</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>1713</v>
-      </c>
       <c r="C32" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D32" s="1">
         <v>4140</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="47.25" customHeight="1">
       <c r="A33" s="1" t="s">
+        <v>1714</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>1715</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>1716</v>
-      </c>
       <c r="C33" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D33" s="1">
         <v>220</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>1717</v>
+        <v>1716</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="47.25" customHeight="1">
       <c r="A34" s="1" t="s">
-        <v>1718</v>
+        <v>1717</v>
       </c>
       <c r="B34" s="8"/>
       <c r="C34" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D34" s="1">
         <v>1</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J34" s="8"/>
       <c r="K34" s="8"/>
     </row>
     <row r="35" spans="1:11" ht="47.25" customHeight="1">
       <c r="A35" s="1" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="B35" s="8"/>
       <c r="C35" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D35" s="1">
         <v>1</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J35" s="8"/>
       <c r="K35" s="8"/>
     </row>
     <row r="36" spans="1:11" ht="47.25" customHeight="1">
       <c r="A36" s="1" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="B36" s="8"/>
       <c r="C36" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D36" s="1">
         <v>1</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J36" s="8"/>
       <c r="K36" s="8"/>
     </row>
     <row r="37" spans="1:11" ht="63" customHeight="1">
       <c r="A37" s="1" t="s">
+        <v>1720</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>1721</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>1722</v>
-      </c>
       <c r="C37" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D37" s="1">
         <v>21667.02</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="47.25" customHeight="1">
       <c r="A38" s="1" t="s">
+        <v>1723</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>1724</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>1725</v>
-      </c>
       <c r="C38" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D38" s="1">
         <v>10020</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="63" customHeight="1">
       <c r="A39" s="1" t="s">
+        <v>1726</v>
+      </c>
+      <c r="B39" s="1" t="s">
         <v>1727</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>1728</v>
-      </c>
       <c r="C39" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D39" s="1">
         <v>30.6</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>1729</v>
+        <v>1728</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="47.25" customHeight="1">
       <c r="A40" s="1" t="s">
+        <v>1729</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>1730</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>1731</v>
-      </c>
       <c r="C40" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D40" s="1">
         <v>12</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="63" customHeight="1">
       <c r="A41" s="1" t="s">
+        <v>1732</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>1733</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>1734</v>
-      </c>
       <c r="C41" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D41" s="1">
         <v>1511</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="63" customHeight="1">
       <c r="A42" s="1" t="s">
+        <v>1735</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>1736</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>1737</v>
-      </c>
       <c r="C42" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D42" s="1">
         <v>88800</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
       <c r="K42" s="1" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="47.25" customHeight="1">
       <c r="A43" s="1" t="s">
+        <v>1738</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>1739</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>1740</v>
-      </c>
       <c r="C43" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D43" s="1">
         <v>340</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J43" s="1" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
       <c r="K43" s="1" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="47.25" customHeight="1">
       <c r="A44" s="1" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D44" s="1">
         <v>1</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J44" s="8"/>
       <c r="K44" s="8"/>
     </row>
     <row r="45" spans="1:11" ht="47.25" customHeight="1">
       <c r="A45" s="1" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
       <c r="B45" s="8"/>
       <c r="C45" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D45" s="1">
         <v>1</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J45" s="8"/>
       <c r="K45" s="8"/>
     </row>
     <row r="46" spans="1:11" ht="47.25" customHeight="1">
       <c r="A46" s="1" t="s">
+        <v>1743</v>
+      </c>
+      <c r="B46" s="1" t="s">
         <v>1744</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>1745</v>
-      </c>
       <c r="C46" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D46" s="1">
         <v>213000</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="47.25" customHeight="1">
       <c r="A47" s="1" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D47" s="1">
         <v>1</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J47" s="8"/>
       <c r="K47" s="8"/>
     </row>
     <row r="48" spans="1:11" ht="47.25" customHeight="1">
       <c r="A48" s="1" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="B48" s="8"/>
       <c r="C48" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D48" s="1">
         <v>1</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J48" s="8"/>
       <c r="K48" s="8"/>
     </row>
     <row r="49" spans="1:11" ht="47.25" customHeight="1">
       <c r="A49" s="1" t="s">
+        <v>1748</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>1749</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>1750</v>
-      </c>
       <c r="C49" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D49" s="1">
         <v>9600</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="47.25" customHeight="1">
       <c r="A50" s="1" t="s">
+        <v>1751</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>1752</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>1753</v>
-      </c>
       <c r="C50" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D50" s="1">
         <v>47</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>1754</v>
+        <v>1753</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="47.25" customHeight="1">
       <c r="A51" s="1" t="s">
+        <v>1754</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>1755</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>1756</v>
-      </c>
       <c r="C51" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D51" s="1">
         <v>200</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>1757</v>
+        <v>1756</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="47.25" customHeight="1">
       <c r="A52" s="1" t="s">
-        <v>1758</v>
+        <v>1757</v>
       </c>
       <c r="B52" s="8"/>
       <c r="C52" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D52" s="1">
         <v>1</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J52" s="8"/>
       <c r="K52" s="8"/>
     </row>
     <row r="53" spans="1:11" ht="47.25" customHeight="1">
       <c r="A53" s="1" t="s">
+        <v>1758</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>1759</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>1760</v>
-      </c>
       <c r="C53" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D53" s="1">
         <v>120</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J53" s="1" t="s">
-        <v>1761</v>
+        <v>1760</v>
       </c>
       <c r="K53" s="1" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="47.25" customHeight="1">
       <c r="A54" s="1" t="s">
-        <v>1762</v>
+        <v>1761</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D54" s="1">
         <v>1</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J54" s="8"/>
       <c r="K54" s="8"/>
     </row>
     <row r="55" spans="1:11" ht="47.25" customHeight="1">
       <c r="A55" s="1" t="s">
-        <v>1763</v>
+        <v>1762</v>
       </c>
       <c r="B55" s="8"/>
       <c r="C55" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D55" s="1">
         <v>1</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J55" s="8"/>
       <c r="K55" s="8"/>
     </row>
     <row r="56" spans="1:11" ht="47.25" customHeight="1">
       <c r="A56" s="1" t="s">
-        <v>1764</v>
+        <v>1763</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D56" s="1">
         <v>1</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J56" s="8"/>
       <c r="K56" s="8"/>
     </row>
     <row r="57" spans="1:11" ht="47.25" customHeight="1">
       <c r="A57" s="1" t="s">
-        <v>1765</v>
+        <v>1764</v>
       </c>
       <c r="B57" s="8"/>
       <c r="C57" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D57" s="1">
         <v>1</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J57" s="8"/>
       <c r="K57" s="8"/>
     </row>
     <row r="58" spans="1:11" ht="47.25" customHeight="1">
       <c r="A58" s="1" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D58" s="1">
         <v>1</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J58" s="8"/>
       <c r="K58" s="8"/>
     </row>
     <row r="59" spans="1:11" ht="47.25" customHeight="1">
       <c r="A59" s="1" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
       <c r="B59" s="8"/>
       <c r="C59" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D59" s="1">
         <v>1</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J59" s="8"/>
       <c r="K59" s="8"/>
     </row>
     <row r="60" spans="1:11" ht="47.25" customHeight="1">
       <c r="A60" s="1" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D60" s="1">
         <v>1</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J60" s="8"/>
       <c r="K60" s="8"/>
     </row>
     <row r="61" spans="1:11" ht="47.25" customHeight="1">
       <c r="A61" s="1" t="s">
+        <v>1768</v>
+      </c>
+      <c r="B61" s="1" t="s">
         <v>1769</v>
       </c>
-      <c r="B61" s="1" t="s">
-        <v>1770</v>
-      </c>
       <c r="C61" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D61" s="1">
         <v>6.5</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="62" spans="1:11" ht="63" customHeight="1">
       <c r="A62" s="1" t="s">
+        <v>1771</v>
+      </c>
+      <c r="B62" s="1" t="s">
         <v>1772</v>
       </c>
-      <c r="B62" s="1" t="s">
-        <v>1773</v>
-      </c>
       <c r="C62" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D62" s="1">
         <v>1.58</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="63" spans="1:11" ht="47.25" customHeight="1">
       <c r="A63" s="1" t="s">
+        <v>1774</v>
+      </c>
+      <c r="B63" s="1" t="s">
         <v>1775</v>
       </c>
-      <c r="B63" s="1" t="s">
-        <v>1776</v>
-      </c>
       <c r="C63" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D63" s="1">
         <v>52</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="64" spans="1:11" ht="47.25" customHeight="1">
       <c r="A64" s="1" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="B64" s="8"/>
       <c r="C64" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D64" s="1">
         <v>1</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J64" s="8"/>
       <c r="K64" s="8"/>
     </row>
     <row r="65" spans="1:11" ht="47.25" customHeight="1">
       <c r="A65" s="1" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="B65" s="8"/>
       <c r="C65" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D65" s="1">
         <v>1</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J65" s="8"/>
       <c r="K65" s="8"/>
     </row>
     <row r="66" spans="1:11" ht="47.25" customHeight="1">
       <c r="A66" s="1" t="s">
-        <v>1780</v>
+        <v>1779</v>
       </c>
       <c r="B66" s="8"/>
       <c r="C66" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D66" s="1">
         <v>1</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J66" s="8"/>
       <c r="K66" s="8"/>
     </row>
     <row r="67" spans="1:11" ht="63" customHeight="1">
       <c r="A67" s="1" t="s">
-        <v>1781</v>
+        <v>1780</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D67" s="1">
         <v>1247</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>1782</v>
+        <v>1781</v>
       </c>
       <c r="K67" s="1" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
     </row>
     <row r="68" spans="1:11" ht="47.25" customHeight="1">
       <c r="A68" s="1" t="s">
-        <v>1783</v>
+        <v>1782</v>
       </c>
       <c r="B68" s="8"/>
       <c r="C68" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D68" s="1">
         <v>1</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J68" s="8"/>
       <c r="K68" s="8"/>
     </row>
     <row r="69" spans="1:11" ht="47.25" customHeight="1">
       <c r="A69" s="1" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="B69" s="8"/>
       <c r="C69" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D69" s="1">
         <v>1</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J69" s="8"/>
       <c r="K69" s="8"/>
     </row>
     <row r="70" spans="1:11" ht="47.25" customHeight="1">
       <c r="A70" s="1" t="s">
-        <v>1785</v>
+        <v>1784</v>
       </c>
       <c r="B70" s="8"/>
       <c r="C70" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D70" s="1">
         <v>1</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J70" s="8"/>
       <c r="K70" s="8"/>
     </row>
     <row r="71" spans="1:11" ht="47.25" customHeight="1">
       <c r="A71" s="1" t="s">
-        <v>1786</v>
+        <v>1785</v>
       </c>
       <c r="B71" s="8"/>
       <c r="C71" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D71" s="1">
         <v>1</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J71" s="8"/>
       <c r="K71" s="8"/>
     </row>
     <row r="72" spans="1:11" ht="47.25" customHeight="1">
       <c r="A72" s="1" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="B72" s="8"/>
       <c r="C72" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D72" s="1">
         <v>1</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J72" s="8"/>
       <c r="K72" s="8"/>
     </row>
     <row r="73" spans="1:11" ht="47.25" customHeight="1">
       <c r="A73" s="1" t="s">
-        <v>1788</v>
+        <v>1787</v>
       </c>
       <c r="B73" s="8"/>
       <c r="C73" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D73" s="1">
         <v>1</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J73" s="8"/>
       <c r="K73" s="8"/>
     </row>
     <row r="74" spans="1:11" ht="47.25" customHeight="1">
       <c r="A74" s="1" t="s">
-        <v>1789</v>
+        <v>1788</v>
       </c>
       <c r="B74" s="8"/>
       <c r="C74" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D74" s="1">
         <v>1</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J74" s="8"/>
       <c r="K74" s="8"/>
     </row>
     <row r="75" spans="1:11" ht="47.25" customHeight="1">
       <c r="A75" s="1" t="s">
-        <v>1790</v>
+        <v>1789</v>
       </c>
       <c r="B75" s="8"/>
       <c r="C75" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D75" s="1">
         <v>1</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J75" s="8"/>
       <c r="K75" s="8"/>
     </row>
     <row r="76" spans="1:11" ht="47.25" customHeight="1">
       <c r="A76" s="1" t="s">
-        <v>1791</v>
+        <v>1790</v>
       </c>
       <c r="B76" s="8"/>
       <c r="C76" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D76" s="1">
         <v>1</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J76" s="8"/>
       <c r="K76" s="8"/>
     </row>
     <row r="77" spans="1:11" ht="47.25" customHeight="1">
       <c r="A77" s="1" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
       <c r="B77" s="8"/>
       <c r="C77" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D77" s="1">
         <v>1</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J77" s="8"/>
       <c r="K77" s="8"/>
     </row>
     <row r="78" spans="1:11" ht="47.25" customHeight="1">
       <c r="A78" s="1" t="s">
-        <v>1793</v>
+        <v>1792</v>
       </c>
       <c r="B78" s="8"/>
       <c r="C78" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D78" s="1">
         <v>1</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J78" s="8"/>
       <c r="K78" s="8"/>
     </row>
     <row r="79" spans="1:11" ht="47.25" customHeight="1">
       <c r="A79" s="1" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="B79" s="8"/>
       <c r="C79" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D79" s="1">
         <v>1</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J79" s="8"/>
       <c r="K79" s="8"/>
     </row>
     <row r="80" spans="1:11" ht="47.25" customHeight="1">
       <c r="A80" s="1" t="s">
-        <v>1795</v>
+        <v>1794</v>
       </c>
       <c r="B80" s="8"/>
       <c r="C80" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D80" s="1">
         <v>1</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J80" s="8"/>
       <c r="K80" s="8"/>
     </row>
     <row r="81" spans="1:11" ht="47.25" customHeight="1">
       <c r="A81" s="1" t="s">
-        <v>1796</v>
+        <v>1795</v>
       </c>
       <c r="B81" s="8"/>
       <c r="C81" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D81" s="1">
         <v>1</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J81" s="8"/>
       <c r="K81" s="8"/>
     </row>
     <row r="82" spans="1:11" ht="47.25" customHeight="1">
       <c r="A82" s="1" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
       <c r="B82" s="8"/>
       <c r="C82" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D82" s="1">
         <v>1</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J82" s="8"/>
       <c r="K82" s="8"/>
     </row>
     <row r="83" spans="1:11" ht="47.25" customHeight="1">
       <c r="A83" s="1" t="s">
-        <v>1798</v>
+        <v>1797</v>
       </c>
       <c r="B83" s="8"/>
       <c r="C83" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D83" s="1">
         <v>1</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J83" s="8"/>
       <c r="K83" s="8"/>
     </row>
     <row r="84" spans="1:11" ht="47.25" customHeight="1">
       <c r="A84" s="1" t="s">
-        <v>1799</v>
+        <v>1798</v>
       </c>
       <c r="B84" s="8"/>
       <c r="C84" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D84" s="1">
         <v>1</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J84" s="8"/>
       <c r="K84" s="8"/>
     </row>
     <row r="85" spans="1:11" ht="47.25" customHeight="1">
       <c r="A85" s="1" t="s">
-        <v>1800</v>
+        <v>1799</v>
       </c>
       <c r="B85" s="8"/>
       <c r="C85" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D85" s="1">
         <v>1</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J85" s="8"/>
       <c r="K85" s="8"/>
     </row>
     <row r="86" spans="1:11" ht="47.25" customHeight="1">
       <c r="A86" s="1" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="B86" s="8"/>
       <c r="C86" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D86" s="1">
         <v>1</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J86" s="8"/>
       <c r="K86" s="8"/>
     </row>
     <row r="87" spans="1:11" ht="47.25" customHeight="1">
       <c r="A87" s="1" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="B87" s="8"/>
       <c r="C87" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D87" s="1">
         <v>1</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J87" s="8"/>
       <c r="K87" s="8"/>
     </row>
     <row r="88" spans="1:11" ht="63" customHeight="1">
       <c r="A88" s="1" t="s">
-        <v>1803</v>
+        <v>1802</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D88" s="1">
         <v>2.31049060186648E-4</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J88" s="1" t="s">
-        <v>1804</v>
+        <v>1803</v>
       </c>
     </row>
     <row r="89" spans="1:11" ht="94.5" customHeight="1">
       <c r="A89" s="1" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D89" s="1">
         <v>265.52119488472903</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>1782</v>
+        <v>1781</v>
       </c>
       <c r="J89" s="1" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
     </row>
     <row r="90" spans="1:11" ht="94.5" customHeight="1">
       <c r="A90" s="1" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D90" s="1">
         <v>2.3345582123025899E-4</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="J90" s="1" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
     </row>
     <row r="91" spans="1:11" ht="63" customHeight="1">
       <c r="A91" s="1" t="s">
+        <v>1807</v>
+      </c>
+      <c r="C91" s="1" t="s">
         <v>1808</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>1809</v>
       </c>
       <c r="D91" s="1">
         <v>1.8128579488019899E-7</v>
@@ -18203,15 +18202,15 @@
         <v>581</v>
       </c>
       <c r="J91" s="1" t="s">
-        <v>1804</v>
+        <v>1803</v>
       </c>
     </row>
     <row r="92" spans="1:11" ht="94.5" customHeight="1">
       <c r="A92" s="1" t="s">
-        <v>1810</v>
+        <v>1809</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>1809</v>
+        <v>1808</v>
       </c>
       <c r="D92" s="1">
         <v>5.0000000000000001E-4</v>
@@ -18220,15 +18219,15 @@
         <v>581</v>
       </c>
       <c r="J92" s="1" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
     </row>
     <row r="93" spans="1:11" ht="94.5" customHeight="1">
       <c r="A93" s="1" t="s">
-        <v>1811</v>
+        <v>1810</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>1809</v>
+        <v>1808</v>
       </c>
       <c r="D93" s="1">
         <v>1E-3</v>
@@ -18237,35 +18236,35 @@
         <v>581</v>
       </c>
       <c r="J93" s="1" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
     </row>
     <row r="94" spans="1:11" ht="409.5" customHeight="1">
       <c r="A94" s="1" t="s">
+        <v>1811</v>
+      </c>
+      <c r="B94" s="1" t="s">
         <v>1812</v>
-      </c>
-      <c r="B94" s="1" t="s">
-        <v>1813</v>
       </c>
       <c r="D94" s="1">
         <v>20</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="J94" s="1" t="s">
-        <v>1814</v>
+        <v>1813</v>
       </c>
       <c r="K94" s="1" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
     </row>
     <row r="95" spans="1:11" ht="31.5" customHeight="1">
       <c r="A95" s="1" t="s">
+        <v>1814</v>
+      </c>
+      <c r="B95" s="1" t="s">
         <v>1815</v>
-      </c>
-      <c r="B95" s="1" t="s">
-        <v>1816</v>
       </c>
       <c r="D95" s="1">
         <v>300</v>
@@ -18276,7 +18275,7 @@
     </row>
     <row r="96" spans="1:11" ht="15.75" customHeight="1">
       <c r="A96" s="1" t="s">
-        <v>1817</v>
+        <v>1816</v>
       </c>
       <c r="D96" s="1">
         <v>1</v>
@@ -18287,7 +18286,7 @@
     </row>
     <row r="97" spans="1:6" ht="15.75" customHeight="1">
       <c r="A97" s="1" t="s">
-        <v>1818</v>
+        <v>1817</v>
       </c>
       <c r="D97" s="1">
         <v>-1</v>
@@ -18297,14 +18296,14 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K97" xr:uid="{00000000-0009-0000-0000-000010000000}"/>
+  <autoFilter ref="A1:K97"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18326,7 +18325,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.2" customHeight="1">
       <c r="A1" t="s">
-        <v>1819</v>
+        <v>1818</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.2" customHeight="1">
@@ -18360,11 +18359,11 @@
     </row>
     <row r="3" spans="1:9" ht="15.2" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>1821</v>
+        <v>1820</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>94</v>
@@ -18375,11 +18374,11 @@
     </row>
     <row r="4" spans="1:9" ht="28.5">
       <c r="A4" s="1" t="s">
-        <v>1822</v>
+        <v>1821</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>1823</v>
+        <v>1822</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>94</v>
@@ -18399,7 +18398,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMT11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18418,16 +18417,16 @@
   <sheetData>
     <row r="1" spans="1:23" ht="15" customHeight="1">
       <c r="A1" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15.2" customHeight="1">
       <c r="G2" s="24" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
       <c r="H2" s="25"/>
       <c r="I2" s="24" t="s">
-        <v>1826</v>
+        <v>1825</v>
       </c>
       <c r="J2" s="25"/>
       <c r="K2" s="25"/>
@@ -18435,11 +18434,11 @@
       <c r="M2" s="25"/>
       <c r="N2" s="25"/>
       <c r="Q2" s="24" t="s">
-        <v>1827</v>
+        <v>1826</v>
       </c>
       <c r="R2" s="25"/>
       <c r="S2" s="24" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
       <c r="T2" s="25"/>
     </row>
@@ -18454,7 +18453,7 @@
         <v>104</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>82</v>
@@ -18463,10 +18462,10 @@
         <v>110</v>
       </c>
       <c r="G3" s="5" t="s">
+        <v>1828</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>1829</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>1830</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>56</v>
@@ -18478,19 +18477,19 @@
         <v>73</v>
       </c>
       <c r="L3" s="5" t="s">
+        <v>1830</v>
+      </c>
+      <c r="M3" s="5" t="s">
         <v>1831</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="N3" s="5" t="s">
         <v>1832</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="O3" s="5" t="s">
         <v>1833</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="P3" s="5" t="s">
         <v>1834</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>1835</v>
       </c>
       <c r="Q3" s="5" t="s">
         <v>31</v>
@@ -18516,23 +18515,23 @@
     </row>
     <row r="4" spans="1:23" ht="15.2" customHeight="1">
       <c r="A4" s="1" t="s">
+        <v>1835</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>1836</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="6" t="s">
         <v>1837</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>1838</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="1" t="s">
         <v>581</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>1838</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>1839</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>1840</v>
       </c>
       <c r="I4" s="1">
         <v>37</v>
@@ -18547,89 +18546,89 @@
         <v>94</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>1841</v>
+        <v>1840</v>
       </c>
     </row>
     <row r="5" spans="1:23" ht="15.2" customHeight="1">
       <c r="A5" s="1" t="s">
+        <v>1841</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>1842</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="6" t="s">
         <v>1843</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>1844</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="1" t="s">
         <v>581</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>1838</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>1839</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>1840</v>
       </c>
       <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:23" ht="15.2" customHeight="1">
       <c r="A6" s="1" t="s">
+        <v>1844</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>1845</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="6" t="s">
         <v>1846</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>1847</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="1" t="s">
         <v>581</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>1838</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>1839</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>1840</v>
       </c>
       <c r="I6" s="7"/>
     </row>
     <row r="7" spans="1:23" ht="15.2" customHeight="1">
       <c r="A7" s="1" t="s">
+        <v>1847</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>1848</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="6" t="s">
         <v>1849</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>1850</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="1" t="s">
         <v>581</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>1838</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>1839</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>1840</v>
       </c>
       <c r="I7" s="7"/>
     </row>
     <row r="8" spans="1:23" ht="15.2" customHeight="1">
       <c r="A8" s="1" t="s">
+        <v>1850</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>1851</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>1852</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="F8" s="1" t="s">
+        <v>1852</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>1853</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>1854</v>
       </c>
       <c r="I8" s="1">
         <v>37</v>
@@ -18640,18 +18639,18 @@
     </row>
     <row r="9" spans="1:23" ht="15.2" customHeight="1">
       <c r="A9" s="1" t="s">
+        <v>1854</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>1855</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>1856</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="F9" s="1" t="s">
+        <v>1856</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>1857</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>1858</v>
       </c>
       <c r="I9" s="1">
         <v>30</v>
@@ -18662,15 +18661,15 @@
     </row>
     <row r="10" spans="1:23" ht="15.2" customHeight="1">
       <c r="A10" s="1" t="s">
+        <v>1858</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>1859</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>1860</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="G10" s="1" t="s">
-        <v>1861</v>
+        <v>1860</v>
       </c>
       <c r="I10" s="1">
         <v>37</v>
@@ -18681,15 +18680,15 @@
     </row>
     <row r="11" spans="1:23" ht="31.5" customHeight="1">
       <c r="A11" s="1" t="s">
+        <v>1861</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>1862</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>1863</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="G11" s="1" t="s">
-        <v>1864</v>
+        <v>1863</v>
       </c>
       <c r="I11" s="1">
         <v>40</v>
@@ -18715,7 +18714,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18820,9 +18819,9 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B13" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:B13"/>
   <hyperlinks>
-    <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -18830,7 +18829,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMC9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18849,7 +18848,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.2" customHeight="1">
       <c r="A1" t="s">
-        <v>1865</v>
+        <v>1864</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.2" customHeight="1">
@@ -18860,7 +18859,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>1866</v>
+        <v>1865</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>44</v>
@@ -18874,38 +18873,38 @@
     </row>
     <row r="3" spans="1:6" ht="15.2" customHeight="1">
       <c r="A3" s="1" t="s">
+        <v>1866</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>1867</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>1868</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>1869</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>1841</v>
+        <v>1840</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.2" customHeight="1">
       <c r="A4" s="1" t="s">
+        <v>1869</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>1870</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>1871</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>1851</v>
+        <v>1850</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.2" customHeight="1">
       <c r="A5" s="1" t="s">
+        <v>1871</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>1872</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>1873</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>1855</v>
+        <v>1854</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.2" customHeight="1"/>
@@ -18923,7 +18922,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMI11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18945,12 +18944,12 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>1874</v>
+        <v>1873</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.2" customHeight="1">
       <c r="G2" s="24" t="s">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="H2" s="25"/>
     </row>
@@ -18965,7 +18964,7 @@
         <v>104</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>82</v>
@@ -18992,56 +18991,56 @@
         <v>53</v>
       </c>
       <c r="M3" s="5" t="s">
+        <v>1875</v>
+      </c>
+      <c r="N3" s="5" t="s">
         <v>1876</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>1877</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15.2" customHeight="1">
       <c r="A4" s="1" t="s">
+        <v>1877</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>1878</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="6" t="s">
+        <v>1837</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>1879</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>1838</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>1880</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>581</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>1880</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>1881</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>1882</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.2" customHeight="1">
       <c r="A5" s="1" t="s">
+        <v>1882</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1878</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>1883</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>1879</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>1884</v>
-      </c>
       <c r="D5" s="6" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>43</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>1884</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>1885</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>1886</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.2" customHeight="1">
@@ -19082,7 +19081,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -19103,7 +19102,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" customHeight="1">
       <c r="A1" t="s">
-        <v>1887</v>
+        <v>1886</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="31.5" customHeight="1">
@@ -19114,46 +19113,46 @@
         <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>1887</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>1888</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>1889</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>1890</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>1891</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>110</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>1891</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>1892</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>1893</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>1894</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>1895</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>1896</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>1897</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>1898</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>1899</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>1900</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>44</v>
@@ -19164,68 +19163,68 @@
     </row>
     <row r="3" spans="1:18" ht="173.25" customHeight="1">
       <c r="A3" s="1" t="s">
+        <v>1900</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>1901</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>1902</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>1903</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>1904</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1">
         <v>2008</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>1904</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>1905</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>1906</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1" t="s">
+        <v>1906</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>1907</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>1908</v>
       </c>
       <c r="R3" s="1"/>
     </row>
     <row r="4" spans="1:18" ht="173.25" customHeight="1">
       <c r="A4" s="1" t="s">
+        <v>1908</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>1909</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>1910</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>1911</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>1912</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1">
         <v>2014</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -19235,160 +19234,160 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1" t="s">
+        <v>1913</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>1914</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>1915</v>
       </c>
       <c r="R4" s="1"/>
     </row>
     <row r="5" spans="1:18" ht="299.25" customHeight="1">
       <c r="A5" s="1" t="s">
+        <v>1915</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>1916</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>1917</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>1918</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>1919</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1">
         <v>2004</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>1913</v>
+        <v>1912</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1" t="s">
+        <v>1919</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>1920</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>1921</v>
       </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1" t="s">
+        <v>1921</v>
+      </c>
+      <c r="Q5" s="1" t="s">
         <v>1922</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>1923</v>
       </c>
       <c r="R5" s="1"/>
     </row>
     <row r="6" spans="1:18" ht="173.25" customHeight="1">
       <c r="A6" s="1" t="s">
+        <v>1923</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>1924</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>1925</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>1926</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>1927</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1">
         <v>2009</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>1928</v>
+        <v>1927</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1" t="s">
+        <v>1928</v>
+      </c>
+      <c r="L6" s="1" t="s">
         <v>1929</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>1930</v>
       </c>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1" t="s">
+        <v>1930</v>
+      </c>
+      <c r="Q6" s="1" t="s">
         <v>1931</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>1932</v>
       </c>
       <c r="R6" s="1"/>
     </row>
     <row r="7" spans="1:18" ht="267.75" customHeight="1">
       <c r="A7" s="1" t="s">
+        <v>1932</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>1933</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>1934</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>1935</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>1936</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1">
         <v>2007</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>1937</v>
+        <v>1936</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1" t="s">
-        <v>1938</v>
+        <v>1937</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1" t="s">
-        <v>1939</v>
+        <v>1938</v>
       </c>
       <c r="R7" s="1"/>
     </row>
     <row r="8" spans="1:18" ht="78.75" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>1939</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>1940</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>1941</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>1942</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1">
         <v>2001</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>1943</v>
+        <v>1942</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1" t="s">
-        <v>1944</v>
+        <v>1943</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -19398,35 +19397,35 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1" t="s">
-        <v>1945</v>
+        <v>1944</v>
       </c>
       <c r="R8" s="1"/>
     </row>
     <row r="9" spans="1:18" ht="110.25" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>1945</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>1946</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>1947</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>1948</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1">
         <v>2006</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1943</v>
+        <v>1942</v>
       </c>
       <c r="H9" s="1" t="s">
+        <v>1948</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>1949</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>1950</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -19436,217 +19435,217 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1" t="s">
-        <v>1951</v>
+        <v>1950</v>
       </c>
       <c r="R9" s="1"/>
     </row>
     <row r="10" spans="1:18" ht="220.5" customHeight="1">
       <c r="A10" s="1" t="s">
+        <v>1951</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>1952</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>1953</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>1954</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>1955</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1">
         <v>1993</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>1956</v>
+        <v>1955</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1" t="s">
-        <v>1957</v>
+        <v>1956</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1" t="s">
+        <v>1957</v>
+      </c>
+      <c r="Q10" s="1" t="s">
         <v>1958</v>
-      </c>
-      <c r="Q10" s="1" t="s">
-        <v>1959</v>
       </c>
       <c r="R10" s="1"/>
     </row>
     <row r="11" spans="1:18" ht="236.25" customHeight="1">
       <c r="A11" s="1" t="s">
+        <v>1959</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>1960</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>1961</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>1962</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>1963</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1">
         <v>2010</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>1964</v>
+        <v>1963</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1" t="s">
-        <v>1965</v>
+        <v>1964</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>1938</v>
+        <v>1937</v>
       </c>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1" t="s">
+        <v>1965</v>
+      </c>
+      <c r="Q11" s="1" t="s">
         <v>1966</v>
-      </c>
-      <c r="Q11" s="1" t="s">
-        <v>1967</v>
       </c>
       <c r="R11" s="1"/>
     </row>
     <row r="12" spans="1:18" ht="236.25" customHeight="1">
       <c r="A12" s="1" t="s">
+        <v>1967</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>1968</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>1969</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>1970</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>1971</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1">
         <v>2000</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>1972</v>
+        <v>1971</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1" t="s">
+        <v>1972</v>
+      </c>
+      <c r="L12" s="1" t="s">
         <v>1973</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>1974</v>
       </c>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1" t="s">
+        <v>1974</v>
+      </c>
+      <c r="Q12" s="1" t="s">
         <v>1975</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>1976</v>
       </c>
       <c r="R12" s="1"/>
     </row>
     <row r="13" spans="1:18" ht="220.5" customHeight="1">
       <c r="A13" s="1" t="s">
+        <v>1976</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>1977</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>1978</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>1979</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>1980</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1">
         <v>1999</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>1938</v>
+        <v>1937</v>
       </c>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1" t="s">
+        <v>1981</v>
+      </c>
+      <c r="Q13" s="1" t="s">
         <v>1982</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>1983</v>
       </c>
       <c r="R13" s="1"/>
     </row>
     <row r="14" spans="1:18" ht="283.5" customHeight="1">
       <c r="A14" s="1" t="s">
+        <v>1983</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>1984</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>1985</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>1986</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>1987</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1">
         <v>1979</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>1972</v>
+        <v>1971</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1" t="s">
+        <v>1987</v>
+      </c>
+      <c r="L14" s="1" t="s">
         <v>1988</v>
-      </c>
-      <c r="L14" s="1" t="s">
-        <v>1989</v>
       </c>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1" t="s">
+        <v>1989</v>
+      </c>
+      <c r="Q14" s="1" t="s">
         <v>1990</v>
-      </c>
-      <c r="Q14" s="1" t="s">
-        <v>1991</v>
       </c>
       <c r="R14" s="1"/>
     </row>
@@ -19655,40 +19654,40 @@
         <v>115</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>1991</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>1992</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>1993</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>1994</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1">
         <v>2012</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1" t="s">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>1930</v>
+        <v>1929</v>
       </c>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1" t="s">
+        <v>1996</v>
+      </c>
+      <c r="Q15" s="1" t="s">
         <v>1997</v>
-      </c>
-      <c r="Q15" s="1" t="s">
-        <v>1998</v>
       </c>
       <c r="R15" s="1"/>
     </row>
@@ -19697,56 +19696,56 @@
         <v>214</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>1998</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>1999</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>2000</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>2001</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1">
         <v>2009</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>1905</v>
+        <v>1904</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>2002</v>
+        <v>2001</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1" t="s">
+        <v>2002</v>
+      </c>
+      <c r="L16" s="1" t="s">
         <v>2003</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>2004</v>
       </c>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1" t="s">
+        <v>2004</v>
+      </c>
+      <c r="Q16" s="1" t="s">
         <v>2005</v>
-      </c>
-      <c r="Q16" s="1" t="s">
-        <v>2006</v>
       </c>
       <c r="R16" s="1"/>
     </row>
     <row r="17" spans="1:18" ht="141.75" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -19758,23 +19757,23 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1" t="s">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="R17" s="1"/>
     </row>
     <row r="18" spans="1:18" ht="110.25" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>2011</v>
+        <v>2010</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -19786,23 +19785,23 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1" t="s">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="R18" s="1"/>
     </row>
     <row r="19" spans="1:18" ht="126" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -19814,23 +19813,23 @@
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1" t="s">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="R19" s="1"/>
     </row>
     <row r="20" spans="1:18" ht="110.25" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -19842,7 +19841,7 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1" t="s">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="R20" s="1"/>
     </row>
@@ -19852,13 +19851,13 @@
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -19870,61 +19869,61 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1" t="s">
-        <v>2021</v>
+        <v>2020</v>
       </c>
       <c r="R21" s="1"/>
     </row>
     <row r="22" spans="1:18" ht="110.25" customHeight="1">
       <c r="A22" s="3" t="s">
+        <v>2021</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>2022</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>2023</v>
       </c>
-      <c r="C22" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>2024</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>2025</v>
       </c>
       <c r="F22" s="3">
         <v>2015</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>2026</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="78.75" customHeight="1">
       <c r="A23" s="3" t="s">
+        <v>2026</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>2027</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>2028</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>2029</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>2030</v>
       </c>
       <c r="F23" s="3">
         <v>2018</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="Q23" s="3" t="s">
-        <v>2031</v>
+        <v>2030</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R23" xr:uid="{00000000-0009-0000-0000-000015000000}"/>
+  <autoFilter ref="A1:R23"/>
   <hyperlinks>
-    <hyperlink ref="Q21" r:id="rId1" xr:uid="{00000000-0004-0000-1500-000000000000}"/>
-    <hyperlink ref="Q22" r:id="rId2" xr:uid="{00000000-0004-0000-1500-000001000000}"/>
+    <hyperlink ref="Q21" r:id="rId1"/>
+    <hyperlink ref="Q22" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -19932,7 +19931,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -19950,7 +19949,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1">
       <c r="A1" t="s">
-        <v>2032</v>
+        <v>2031</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="31.5" customHeight="1">
@@ -19961,28 +19960,28 @@
         <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>2032</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>2033</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>2034</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
+        <v>1887</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>2035</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>1888</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>2036</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>2037</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>2038</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>2039</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>44</v>
@@ -19997,7 +19996,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20015,7 +20014,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" customHeight="1">
       <c r="A1" t="s">
-        <v>2040</v>
+        <v>2039</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="31.5" customHeight="1">
@@ -20029,25 +20028,25 @@
         <v>110</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>2040</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>2041</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>2042</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>2043</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>2044</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>2045</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>2046</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>2047</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>44</v>
@@ -20065,10 +20064,10 @@
         <v>53</v>
       </c>
       <c r="P2" s="2" t="s">
+        <v>1875</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>1876</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>1877</v>
       </c>
     </row>
   </sheetData>
@@ -20077,7 +20076,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20145,7 +20144,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMD8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20218,7 +20217,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AML6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20335,14 +20334,14 @@
       <c r="H6" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H6" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
+  <autoFilter ref="A1:H6"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMR5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -20566,7 +20565,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:U5" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
+  <autoFilter ref="A2:U5"/>
   <mergeCells count="2">
     <mergeCell ref="H2:K2"/>
     <mergeCell ref="M2:P2"/>
@@ -20577,7 +20576,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMN146"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -24205,7 +24204,7 @@
       <c r="N146" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:N146" xr:uid="{00000000-0009-0000-0000-000006000000}"/>
+  <autoFilter ref="A2:N146"/>
   <mergeCells count="1">
     <mergeCell ref="C2:H2"/>
   </mergeCells>
@@ -24215,7 +24214,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AML177"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -26905,7 +26904,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AML128"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -30342,7 +30341,7 @@
       <c r="D128" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="C1:L127" xr:uid="{00000000-0009-0000-0000-000008000000}"/>
+  <autoFilter ref="C1:L127"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>